<commit_message>
added volume discount WIP
</commit_message>
<xml_diff>
--- a/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
+++ b/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -22,38 +22,42 @@
     <definedName name="_Order1" hidden="1">0</definedName>
     <definedName name="_Series" hidden="1">Variables!$B$3</definedName>
     <definedName name="_Shading" hidden="1">Variables!$B$2</definedName>
-    <definedName name="Breakeven_point">'Breakeven Analysis Data'!$F$43</definedName>
+    <definedName name="Breakeven_point">'Breakeven Analysis Data'!$F$44</definedName>
     <definedName name="Company_name">'Breakeven Analysis Data'!$B$2</definedName>
     <definedName name="DATA_01" hidden="1">'Breakeven Analysis Data'!$B$2:$B$3</definedName>
     <definedName name="DATA_02" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_03" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_04" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_05" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
-    <definedName name="DATA_06" hidden="1">'Breakeven Analysis Data'!$F$12:$F$19</definedName>
+    <definedName name="DATA_06" hidden="1">'Breakeven Analysis Data'!$F$13:$F$20</definedName>
     <definedName name="DATA_07" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_08" hidden="1">'Breakeven Analysis Data'!$H$4</definedName>
-    <definedName name="Fixed_costs">'Breakeven Analysis Data'!$F$27:$F$36</definedName>
-    <definedName name="Gross_margin">'Breakeven Analysis Data'!$G$24</definedName>
+    <definedName name="Fixed_costs">'Breakeven Analysis Data'!$F$28:$F$37</definedName>
+    <definedName name="Gross_margin">'Breakeven Analysis Data'!$G$25</definedName>
     <definedName name="IntroPrintArea" hidden="1">#REF!</definedName>
     <definedName name="Look1Area">#REF!</definedName>
     <definedName name="Look2Area">#REF!</definedName>
     <definedName name="Look3Area">#REF!</definedName>
     <definedName name="Look4Area">#REF!</definedName>
     <definedName name="Look5Area">#REF!</definedName>
-    <definedName name="Net_profit">'Breakeven Analysis Data'!$G$39</definedName>
-    <definedName name="Sales_price_unit">'Breakeven Analysis Data'!$F$5</definedName>
-    <definedName name="Sales_volume_units">'Breakeven Analysis Data'!$F$6</definedName>
+    <definedName name="Net_profit">'Breakeven Analysis Data'!$G$40</definedName>
+    <definedName name="Sales_price_unitA">'Breakeven Analysis Data'!$F$5</definedName>
+    <definedName name="Sales_price_unitB">'Breakeven Analysis Data'!$H$5</definedName>
+    <definedName name="Sales_price_unitC">'Breakeven Analysis Data'!$J$5</definedName>
+    <definedName name="Sales_volume_unitsA">'Breakeven Analysis Data'!$F$6</definedName>
+    <definedName name="Sales_volume_unitsB">'Breakeven Analysis Data'!$H$6</definedName>
+    <definedName name="Sales_volume_unitsC">'Breakeven Analysis Data'!$J$6</definedName>
     <definedName name="TemplatePrintArea">'Breakeven Analysis Data'!$B$1:$G$5</definedName>
-    <definedName name="Total_fixed">'Breakeven Analysis Data'!$G$37</definedName>
-    <definedName name="Total_Sales">'Breakeven Analysis Data'!$G$7</definedName>
-    <definedName name="Total_Subscription">'Breakeven Analysis Data'!$G$10</definedName>
-    <definedName name="Total_variable">'Breakeven Analysis Data'!$G$21</definedName>
-    <definedName name="Unit_contrib_margin">'Breakeven Analysis Data'!$F$23</definedName>
-    <definedName name="Variable_cost_unit">'Breakeven Analysis Data'!$F$20</definedName>
-    <definedName name="Variable_costs_unit">'Breakeven Analysis Data'!$F$12:$F$19</definedName>
-    <definedName name="Variable_Unit_Cost">'Breakeven Analysis Data'!$F$20</definedName>
+    <definedName name="Total_fixed">'Breakeven Analysis Data'!$G$38</definedName>
+    <definedName name="Total_Sales">'Breakeven Analysis Data'!$G$8</definedName>
+    <definedName name="Total_Subscription">'Breakeven Analysis Data'!$G$11</definedName>
+    <definedName name="Total_variable">'Breakeven Analysis Data'!$G$22</definedName>
+    <definedName name="Unit_contrib_margin">'Breakeven Analysis Data'!$F$24</definedName>
+    <definedName name="Variable_cost_unit">'Breakeven Analysis Data'!$F$21</definedName>
+    <definedName name="Variable_costs_unit">'Breakeven Analysis Data'!$F$13:$F$20</definedName>
+    <definedName name="Variable_Unit_Cost">'Breakeven Analysis Data'!$F$21</definedName>
   </definedNames>
-  <calcPr calcId="171027" concurrentCalc="0"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -86,6 +90,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{7D0A91FE-B1FC-4772-B671-83EC5EA0EC0D}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Up-Front prijs van product.
+Hoeveelheidskorting is mogelijk
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{C306B6D9-DB5D-41DC-8381-E112C47706A1}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Up-Front prijs van product.
+Hoeveelheidskorting is mogelijk
+</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F6" authorId="0" shapeId="0" xr:uid="{5217D6D1-5CD7-4075-AFE8-EA322F49B4C9}">
       <text>
         <r>
@@ -99,7 +133,33 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{A3A9E55F-847E-4661-913D-184F52F6F529}">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{831FB1F6-E4B8-4DC3-9B71-8B472336E9DB}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hoeveel producten per periode verkocht worden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{30555F1F-FBCD-421F-812F-AD65AB932B8F}">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Hoeveel producten per periode verkocht worden</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{A3A9E55F-847E-4661-913D-184F52F6F529}">
       <text>
         <r>
           <rPr>
@@ -112,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{5CF3165E-FCBD-453E-AF2A-EA2B9BFC17C7}">
+    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{5CF3165E-FCBD-453E-AF2A-EA2B9BFC17C7}">
       <text>
         <r>
           <rPr>
@@ -126,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{5D839EBC-3BE3-4C34-8563-6F5A98C52E6E}">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{5D839EBC-3BE3-4C34-8563-6F5A98C52E6E}">
       <text>
         <r>
           <rPr>
@@ -140,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{DF3550BB-FD51-4154-B794-6A8344BA2F43}">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{DF3550BB-FD51-4154-B794-6A8344BA2F43}">
       <text>
         <r>
           <rPr>
@@ -153,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{70740BD0-CC66-4C54-86D3-8CFA9D18EBC2}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{70740BD0-CC66-4C54-86D3-8CFA9D18EBC2}">
       <text>
         <r>
           <rPr>
@@ -177,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{58D98360-D15F-4E39-A36D-F6F27D06BD03}">
+    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{58D98360-D15F-4E39-A36D-F6F27D06BD03}">
       <text>
         <r>
           <rPr>
@@ -191,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{0311ABD3-7CCC-4345-89C5-881F9C7EA603}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{0311ABD3-7CCC-4345-89C5-881F9C7EA603}">
       <text>
         <r>
           <rPr>
@@ -204,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{F6D60EF9-0745-4CB6-8B69-14B527E69522}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{F6D60EF9-0745-4CB6-8B69-14B527E69522}">
       <text>
         <r>
           <rPr>
@@ -219,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{609A7C58-C559-486A-8D2D-85B7A7A7AE0A}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{609A7C58-C559-486A-8D2D-85B7A7A7AE0A}">
       <text>
         <r>
           <rPr>
@@ -234,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{EA10A0B4-ED7D-4B1B-9DF6-7CF415632FED}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{EA10A0B4-ED7D-4B1B-9DF6-7CF415632FED}">
       <text>
         <r>
           <rPr>
@@ -248,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{165A2A66-A40C-4D4A-8EF3-CD46A0C51E76}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{165A2A66-A40C-4D4A-8EF3-CD46A0C51E76}">
       <text>
         <r>
           <rPr>
@@ -282,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{0D7BD022-B106-460F-B833-13D1C6EA7135}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{0D7BD022-B106-460F-B833-13D1C6EA7135}">
       <text>
         <r>
           <rPr>
@@ -301,7 +361,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>_Example</t>
   </si>
@@ -438,9 +498,6 @@
     <t xml:space="preserve">    Net Profit</t>
   </si>
   <si>
-    <t>Sales (50 users per unit, 3 months per period)</t>
-  </si>
-  <si>
     <t>Sales volume (units)</t>
   </si>
   <si>
@@ -463,15 +520,24 @@
   <si>
     <t>Subscription</t>
   </si>
+  <si>
+    <t>Sales price</t>
+  </si>
+  <si>
+    <t>Sales</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="6">
+    <numFmt numFmtId="7" formatCode="#,##0.00\ &quot;€&quot;;\-#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="mm/dd/yy"/>
     <numFmt numFmtId="165" formatCode="0_);[Red]\(0\)"/>
     <numFmt numFmtId="166" formatCode="0_);\(0\)"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ _€"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -600,7 +666,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -722,6 +788,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -729,7 +810,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="69">
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="38" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -770,9 +851,6 @@
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="37" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="38" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="38" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="38" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="38" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -857,6 +935,31 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="37" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="7" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="7" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Date" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1096,7 +1199,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('Breakeven Analysis Data'!$C$20,'Breakeven Analysis Data'!$C$23)</c:f>
+              <c:f>('Breakeven Analysis Data'!$C$21,'Breakeven Analysis Data'!$C$24)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1110,7 +1213,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Breakeven Analysis Data'!$F$20,'Breakeven Analysis Data'!$F$23)</c:f>
+              <c:f>('Breakeven Analysis Data'!$F$21,'Breakeven Analysis Data'!$F$24)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1118,7 +1221,7 @@
                   <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3750</c:v>
+                  <c:v>3250</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1383,7 +1486,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$C$13:$C$19</c:f>
+              <c:f>'Breakeven Analysis Data'!$C$14:$C$20</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1412,7 +1515,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$F$12:$F$19</c:f>
+              <c:f>'Breakeven Analysis Data'!$F$13:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1561,6 +1664,569 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Tahoma"/>
+                <a:ea typeface="Tahoma"/>
+                <a:cs typeface="Tahoma"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Unit Contribution Margin</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16864589372884201"/>
+          <c:y val="0.175999644781244"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21377659811982799"/>
+          <c:y val="0.25999974609399801"/>
+          <c:w val="0.339667261457061"/>
+          <c:h val="0.57199944140679504"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="8080FF"/>
+            </a:solidFill>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-DDBF-4905-949C-BF55817811B1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="1"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="802060"/>
+              </a:solidFill>
+              <a:ln w="12700">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:prstDash val="solid"/>
+              </a:ln>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000002-DDBF-4905-949C-BF55817811B1}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="850" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Tahoma"/>
+                    <a:ea typeface="Tahoma"/>
+                    <a:cs typeface="Tahoma"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>('Breakeven Analysis Data'!$C$21,'Breakeven Analysis Data'!$C$24)</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Variable costs per unit</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Unit contribution margin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>('Breakeven Analysis Data'!$F$21,'Breakeven Analysis Data'!$F$24)</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>850</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3250</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DDBF-4905-949C-BF55817811B1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.68408513662632997"/>
+          <c:y val="0.183999763187496"/>
+          <c:w val="0.30641311463145499"/>
+          <c:h val="0.1"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="715" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Tahoma"/>
+              <a:ea typeface="Tahoma"/>
+              <a:cs typeface="Tahoma"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9525">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="850" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Tahoma"/>
+          <a:ea typeface="Tahoma"/>
+          <a:cs typeface="Tahoma"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.5" footer="0.5"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Tahoma"/>
+                <a:ea typeface="Tahoma"/>
+                <a:cs typeface="Tahoma"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Unit Contribution Margin</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16864589372884201"/>
+          <c:y val="0.175999644781244"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.21377659811982799"/>
+          <c:y val="0.25999974609399801"/>
+          <c:w val="0.339667261457061"/>
+          <c:h val="0.57199944140679504"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:pieChart>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="8080FF"/>
+            </a:solidFill>
+            <a:ln w="12700">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:bubble3D val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000000-A48D-4222-A4F8-4CEB8D22B86C}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
+          <c:dLbls>
+            <c:numFmt formatCode="0%" sourceLinked="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="25400">
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="850" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="Tahoma"/>
+                    <a:ea typeface="Tahoma"/>
+                    <a:cs typeface="Tahoma"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-BE"/>
+              </a:p>
+            </c:txPr>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="1"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="1"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>('Breakeven Analysis Data'!$C$21,'Breakeven Analysis Data'!$C$24)</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Breakeven Analysis Data'!$C$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Variable costs per unit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>('Breakeven Analysis Data'!$F$21,'Breakeven Analysis Data'!$F$24)</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>'Breakeven Analysis Data'!$F$21</c:f>
+              <c:numCache>
+                <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>850</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+              <c15:categoryFilterExceptions>
+                <c15:categoryFilterException>
+                  <c15:sqref>'Breakeven Analysis Data'!$F$24</c15:sqref>
+                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <a:solidFill>
+                      <a:srgbClr val="802060"/>
+                    </a:solidFill>
+                    <a:ln w="12700">
+                      <a:solidFill>
+                        <a:srgbClr val="000000"/>
+                      </a:solidFill>
+                      <a:prstDash val="solid"/>
+                    </a:ln>
+                  </c15:spPr>
+                  <c15:bubble3D val="0"/>
+                </c15:categoryFilterException>
+              </c15:categoryFilterExceptions>
+            </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-A48D-4222-A4F8-4CEB8D22B86C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:showLeaderLines val="1"/>
+        </c:dLbls>
+        <c:firstSliceAng val="0"/>
+      </c:pieChart>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.68408513662632997"/>
+          <c:y val="0.183999763187496"/>
+          <c:w val="0.30641311463145499"/>
+          <c:h val="0.1"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400">
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="715" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Tahoma"/>
+              <a:ea typeface="Tahoma"/>
+              <a:cs typeface="Tahoma"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-BE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="FFFFFF"/>
+    </a:solidFill>
+    <a:ln w="9525">
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="850" b="0" i="0" u="none" strike="noStrike" baseline="0">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Tahoma"/>
+          <a:ea typeface="Tahoma"/>
+          <a:cs typeface="Tahoma"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-BE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.5" footer="0.5"/>
+    <c:pageSetup orientation="landscape"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
@@ -1614,7 +2280,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$48</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$49</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1648,42 +2314,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$48:$N$48</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$49:$N$49</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1700,7 +2366,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$50</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1734,42 +2400,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$50:$N$50</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$51:$N$51</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>47300</c:v>
+                  <c:v>149900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48320</c:v>
+                  <c:v>151600</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>49340</c:v>
+                  <c:v>153300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50360</c:v>
+                  <c:v>155000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>51380</c:v>
+                  <c:v>156700</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52400</c:v>
+                  <c:v>158400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53420</c:v>
+                  <c:v>160100</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>54440</c:v>
+                  <c:v>161800</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55460</c:v>
+                  <c:v>163500</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>56480</c:v>
+                  <c:v>165200</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>57500</c:v>
+                  <c:v>166900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1786,7 +2452,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$51</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1820,7 +2486,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$51:$N$51</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$52:$N$52</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1828,34 +2494,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5520.0000000000009</c:v>
+                  <c:v>8200</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11040.000000000002</c:v>
+                  <c:v>16400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16560</c:v>
+                  <c:v>24600</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22080.000000000004</c:v>
+                  <c:v>32800</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>27600</c:v>
+                  <c:v>41000</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>33120</c:v>
+                  <c:v>49200</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>38639.999999999993</c:v>
+                  <c:v>57400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44160.000000000007</c:v>
+                  <c:v>65600</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49680</c:v>
+                  <c:v>73800</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>55200</c:v>
+                  <c:v>82000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1872,7 +2538,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$52</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1904,42 +2570,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$52:$N$52</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$53:$N$53</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-47300</c:v>
+                  <c:v>-149900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-42800</c:v>
+                  <c:v>-143400</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-38300</c:v>
+                  <c:v>-136900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-33800</c:v>
+                  <c:v>-130400</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-29299.999999999996</c:v>
+                  <c:v>-123900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-24800</c:v>
+                  <c:v>-117400</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-20300</c:v>
+                  <c:v>-110900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-15800.000000000007</c:v>
+                  <c:v>-104400</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-11299.999999999993</c:v>
+                  <c:v>-97900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-6800</c:v>
+                  <c:v>-91400</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2300</c:v>
+                  <c:v>-84900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2241,43 +2907,47 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$5" horiz="1" inc="100" max="10000" min="500" page="10" val="4600"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$5" horiz="1" inc="100" max="10000" min="500" page="10" val="4100"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" max="50" min="1" page="10" val="12"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" max="50" min="1" page="10" val="20"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$18" horiz="1" inc="100" max="1000" page="10" val="300"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$19" horiz="1" inc="100" max="1000" page="10" val="300"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$16" horiz="1" inc="50" max="1000" page="10" val="250"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$17" horiz="1" inc="50" max="1000" page="10" val="250"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$27" horiz="1" inc="1000" max="30000" min="10000" page="1000" val="20000"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$10" horiz="1" inc="100" max="10000" page="0" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$9" horiz="1" inc="100" max="10000" page="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$6" horiz="1" max="50" min="1" page="10" val="10"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$J$6" horiz="1" max="50" min="1" page="10" val="10"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>127000</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>120465</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>558800</xdr:rowOff>
+      <xdr:rowOff>331304</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>339587</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>25466</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2308,13 +2978,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>165976</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>318376</xdr:colOff>
-      <xdr:row>42</xdr:row>
+      <xdr:row>43</xdr:row>
       <xdr:rowOff>241300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2355,7 +3025,7 @@
           <xdr:col>6</xdr:col>
           <xdr:colOff>790575</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:rowOff>139262</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2448,13 +3118,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2498,13 +3168,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>15</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>828675</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2548,63 +3218,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>25</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
-          <xdr:row>26</xdr:row>
-          <xdr:rowOff>161925</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1034" name="Scroll Bar 10" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1034"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>790575</xdr:colOff>
-          <xdr:row>8</xdr:row>
+          <xdr:row>9</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2642,6 +3262,182 @@
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>26933</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>156013</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>8</xdr:col>
+          <xdr:colOff>809624</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1048" name="Scroll Bar 24" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1048"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7147AF22-DC74-4F9E-8B86-A36A4AD7D1E6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>20364</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>4927</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>10</xdr:col>
+          <xdr:colOff>791561</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>4927</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1050" name="Scroll Bar 26" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1050"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E19ABF4-45CD-45D5-AD45-D9A156AD54D5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>204515</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>297602</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>506464</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>196524</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="14" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234553F2-1143-4083-ACD9-F85DFEC544EB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>77604</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>343890</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>271101</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>192497</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="15" name="Chart 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{989F1835-9811-4745-945F-5107EAFA85E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -3004,10 +3800,10 @@
     <tabColor indexed="26"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3018,73 +3814,94 @@
     <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="20" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="10" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="20" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="20" customWidth="1"/>
     <col min="9" max="14" width="12.7109375" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="4"/>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="23"/>
     </row>
     <row r="2" spans="1:10" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A2" s="4"/>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="29"/>
+      <c r="C2" s="28"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="16"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:10" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="13"/>
-      <c r="B3" s="42" t="s">
+      <c r="B3" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="42"/>
+      <c r="C3" s="41"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="17"/>
-      <c r="H3" s="21"/>
-    </row>
-    <row r="4" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="H3" s="66">
+        <v>0.1</v>
+      </c>
+      <c r="J3" s="66">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
-      <c r="B4" s="43" t="s">
-        <v>45</v>
-      </c>
-      <c r="C4" s="43"/>
-      <c r="D4" s="30"/>
+      <c r="B4" s="42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="42"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="5"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="7"/>
+      <c r="F4" s="61">
+        <v>50</v>
+      </c>
+      <c r="G4" s="60"/>
+      <c r="H4" s="63">
+        <v>200</v>
+      </c>
+      <c r="I4" s="67"/>
+      <c r="J4" s="62">
+        <v>500</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
-        <v>8</v>
+      <c r="C5" s="53" t="s">
+        <v>49</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="31">
-        <v>4600</v>
+      <c r="F5" s="64">
+        <v>4100</v>
       </c>
       <c r="G5" s="7"/>
+      <c r="H5" s="64">
+        <f>Sales_price_unitA*(H4/F4)*(1-H3)</f>
+        <v>14760</v>
+      </c>
+      <c r="J5" s="64">
+        <f>Sales_price_unitA*(J4/F4)*(1-J3)</f>
+        <v>30750</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
@@ -3093,264 +3910,276 @@
         <v>23</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="45">
-        <v>12</v>
+      <c r="F6" s="44">
+        <v>20</v>
       </c>
       <c r="G6" s="8"/>
+      <c r="H6" s="44">
+        <v>10</v>
+      </c>
+      <c r="J6" s="44">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B7" s="36"/>
-      <c r="C7" s="23" t="s">
+      <c r="A7" s="4"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="68">
+        <f>IF(OR(Sales_price_unitA&lt;&gt;0,Sales_volume_unitsA&lt;&gt;0),Sales_price_unitA*Sales_volume_unitsA,0)</f>
+        <v>82000</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="68">
+        <f>IF(OR(Sales_price_unitB&lt;&gt;0,Sales_volume_unitsB&lt;&gt;0),Sales_price_unitB*Sales_volume_unitsB,0)</f>
+        <v>147600</v>
+      </c>
+      <c r="J7" s="68">
+        <f>IF(OR(Sales_price_unitC&lt;&gt;0,Sales_volume_unitsC&lt;&gt;0),Sales_price_unitC*Sales_volume_unitsC,0)</f>
+        <v>307500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B8" s="35"/>
+      <c r="C8" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="33">
-        <f>IF(OR(Sales_price_unit&lt;&gt;0,Sales_volume_units&lt;&gt;0),Sales_price_unit*Sales_volume_units,0)</f>
-        <v>55200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="36"/>
-      <c r="C8" s="23"/>
-      <c r="G8" s="20"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="54" t="s">
-        <v>47</v>
-      </c>
-      <c r="E9" s="4"/>
-      <c r="F9" s="45">
-        <v>0</v>
-      </c>
-      <c r="G9" s="18"/>
+      <c r="G8" s="65">
+        <f>F7+H7+J7</f>
+        <v>537100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B9" s="35"/>
+      <c r="C9" s="22"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="11"/>
-      <c r="C10" s="59" t="s">
-        <v>48</v>
+      <c r="C10" s="53" t="s">
+        <v>46</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="58"/>
-      <c r="G10" s="60">
-        <f>F9</f>
+      <c r="F10" s="44">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G10" s="18"/>
+    </row>
+    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="11"/>
+      <c r="C11" s="58" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="59">
+        <f>F10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="44"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="18"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="4"/>
-      <c r="B12" s="11"/>
-      <c r="C12" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="32">
-        <v>100</v>
-      </c>
-      <c r="G12" s="57"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="11"/>
-      <c r="C13" s="54" t="s">
-        <v>30</v>
+      <c r="C13" s="35" t="s">
+        <v>36</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="55"/>
+      <c r="F13" s="31">
+        <v>100</v>
+      </c>
+      <c r="G13" s="56"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="11"/>
-      <c r="C14" s="54" t="s">
-        <v>31</v>
+      <c r="C14" s="53" t="s">
+        <v>30</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="32">
-        <v>100</v>
-      </c>
-      <c r="G14" s="55"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="54"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="54" t="s">
-        <v>41</v>
+      <c r="C15" s="53" t="s">
+        <v>31</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="32">
-        <v>0</v>
-      </c>
-      <c r="G15" s="55"/>
+      <c r="F15" s="31">
+        <v>100</v>
+      </c>
+      <c r="G15" s="54"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="54" t="s">
-        <v>42</v>
+      <c r="C16" s="53" t="s">
+        <v>41</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="32">
-        <v>250</v>
-      </c>
-      <c r="G16" s="55"/>
+      <c r="F16" s="31">
+        <v>0</v>
+      </c>
+      <c r="G16" s="54"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="54" t="s">
-        <v>32</v>
+      <c r="C17" s="53" t="s">
+        <v>42</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="32">
-        <v>0</v>
-      </c>
-      <c r="G17" s="55"/>
+      <c r="F17" s="31">
+        <v>250</v>
+      </c>
+      <c r="G17" s="54"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="11"/>
-      <c r="C18" s="54" t="s">
-        <v>29</v>
+      <c r="C18" s="53" t="s">
+        <v>32</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="32">
-        <v>300</v>
-      </c>
-      <c r="G18" s="55"/>
+      <c r="F18" s="31">
+        <v>0</v>
+      </c>
+      <c r="G18" s="54"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="11"/>
-      <c r="C19" s="11" t="s">
-        <v>21</v>
+      <c r="C19" s="53" t="s">
+        <v>29</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="32">
-        <v>100</v>
-      </c>
-      <c r="G19" s="55"/>
+      <c r="F19" s="31">
+        <v>300</v>
+      </c>
+      <c r="G19" s="54"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="11"/>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="31">
+        <v>100</v>
+      </c>
+      <c r="G20" s="54"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="4"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="34">
+      <c r="E21" s="3"/>
+      <c r="F21" s="33">
         <f>IF(SUM(Variable_costs_unit),SUM(Variable_costs_unit),0)</f>
         <v>850</v>
       </c>
-      <c r="G20" s="56"/>
-    </row>
-    <row r="21" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="19"/>
-      <c r="G21" s="46">
-        <f>IF(Variable_Unit_Cost,Variable_Unit_Cost*Sales_volume_units,0)</f>
-        <v>10200</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G21" s="55"/>
+    </row>
+    <row r="22" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="11"/>
-      <c r="C22" s="35"/>
+      <c r="C22" s="34" t="s">
+        <v>22</v>
+      </c>
       <c r="E22" s="3"/>
       <c r="F22" s="19"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="1"/>
+      <c r="G22" s="45">
+        <f>IF(Variable_Unit_Cost,Variable_Unit_Cost*Sales_volume_unitsA,0)</f>
+        <v>17000</v>
+      </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="11"/>
-      <c r="C23" s="35" t="s">
-        <v>16</v>
-      </c>
+      <c r="C23" s="34"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="33">
-        <f>IF(Sales_price_unit&gt;0,MAX(0,Sales_price_unit-Variable_Unit_Cost),0)</f>
-        <v>3750</v>
-      </c>
+      <c r="F23" s="19"/>
       <c r="G23" s="19"/>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="11"/>
-      <c r="C24" s="35" t="s">
-        <v>10</v>
+      <c r="C24" s="34" t="s">
+        <v>16</v>
       </c>
       <c r="E24" s="3"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="33">
-        <f>IF(OR(Total_Sales&lt;&gt;0,Total_variable&lt;&gt;0),Total_Sales-Total_variable,0)</f>
-        <v>45000</v>
-      </c>
+      <c r="F24" s="32">
+        <f>IF(Sales_price_unitA&gt;0,MAX(0,Sales_price_unitA-Variable_Unit_Cost),0)</f>
+        <v>3250</v>
+      </c>
+      <c r="G24" s="19"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="22"/>
+      <c r="C25" s="34" t="s">
+        <v>10</v>
+      </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="32">
+        <f>IF(OR(Total_Sales&lt;&gt;0,Total_variable&lt;&gt;0),Total_Sales-Total_variable,0)</f>
+        <v>520100</v>
+      </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A27" s="4"/>
+      <c r="B27" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="51"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="32">
-        <v>20000</v>
-      </c>
-      <c r="G27" s="1"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="50"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="1"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="11"/>
-      <c r="C28" s="36" t="s">
-        <v>37</v>
+      <c r="C28" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="E28" s="3"/>
-      <c r="F28" s="32">
-        <v>0</v>
+      <c r="F28" s="31">
+        <v>80000</v>
       </c>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
@@ -3358,12 +4187,12 @@
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="11"/>
-      <c r="C29" s="36" t="s">
-        <v>35</v>
+      <c r="C29" s="35" t="s">
+        <v>37</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="32">
-        <v>10000</v>
+      <c r="F29" s="31">
+        <v>0</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -3371,12 +4200,12 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="11"/>
-      <c r="C30" s="36" t="s">
-        <v>34</v>
+      <c r="C30" s="35" t="s">
+        <v>35</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="32">
-        <v>800</v>
+      <c r="F30" s="31">
+        <v>30000</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -3384,12 +4213,12 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="11"/>
-      <c r="C31" s="36" t="s">
-        <v>38</v>
+      <c r="C31" s="35" t="s">
+        <v>34</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="32">
-        <v>3000</v>
+      <c r="F31" s="31">
+        <v>2400</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -3397,12 +4226,12 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="11"/>
-      <c r="C32" s="54" t="s">
-        <v>39</v>
+      <c r="C32" s="35" t="s">
+        <v>38</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="32">
-        <v>1000</v>
+      <c r="F32" s="31">
+        <v>10000</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -3410,35 +4239,35 @@
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="11"/>
-      <c r="C33" s="11" t="s">
-        <v>6</v>
+      <c r="C33" s="53" t="s">
+        <v>39</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="32"/>
+      <c r="F33" s="31">
+        <v>5000</v>
+      </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="54" t="s">
-        <v>28</v>
+      <c r="C34" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="47">
-        <v>5000</v>
-      </c>
+      <c r="F34" s="31"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="54" t="s">
-        <v>40</v>
+      <c r="C35" s="53" t="s">
+        <v>28</v>
       </c>
       <c r="E35" s="3"/>
-      <c r="F35" s="50">
+      <c r="F35" s="46">
         <v>5000</v>
       </c>
       <c r="G35" s="1"/>
@@ -3447,497 +4276,510 @@
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="11"/>
-      <c r="C36" s="11" t="s">
-        <v>7</v>
+      <c r="C36" s="53" t="s">
+        <v>40</v>
       </c>
       <c r="E36" s="3"/>
-      <c r="F36" s="31">
-        <v>2500</v>
+      <c r="F36" s="49">
+        <v>15000</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="35" t="s">
+      <c r="C37" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="30">
+        <v>2500</v>
+      </c>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="18"/>
-      <c r="G37" s="48">
+      <c r="E38" s="3"/>
+      <c r="F38" s="18"/>
+      <c r="G38" s="47">
         <f>IF(SUM(Fixed_costs)&lt;&gt;0,SUM(Fixed_costs),0)</f>
-        <v>47300</v>
-      </c>
-      <c r="H37" s="1"/>
-    </row>
-    <row r="38" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="36"/>
-      <c r="C38" s="36"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="20"/>
+        <v>149900</v>
+      </c>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="11"/>
-      <c r="C39" s="35" t="s">
+      <c r="B39" s="35"/>
+      <c r="C39" s="35"/>
+      <c r="F39" s="18"/>
+      <c r="G39" s="20"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="E39" s="3"/>
-      <c r="G39" s="49">
+      <c r="E40" s="3"/>
+      <c r="G40" s="48">
         <f>IF(OR(Gross_margin&lt;&gt;0,Total_fixed&lt;&gt;0),Gross_margin-Total_fixed,0)</f>
-        <v>-2300</v>
-      </c>
-      <c r="H39" s="1"/>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B40" s="36"/>
-      <c r="C40" s="36"/>
-      <c r="G40" s="20"/>
-    </row>
-    <row r="41" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
-      <c r="B41" s="36"/>
-      <c r="C41" s="36"/>
-      <c r="F41" s="25"/>
+        <v>370200</v>
+      </c>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35"/>
+      <c r="G41" s="20"/>
     </row>
     <row r="42" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
-      <c r="B42" s="25" t="s">
+      <c r="B42" s="35"/>
+      <c r="C42" s="35"/>
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
+      <c r="B43" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C42" s="25"/>
-      <c r="D42" s="25"/>
-      <c r="E42" s="25"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1"/>
-    </row>
-    <row r="43" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B43" s="41" t="s">
+      <c r="C43" s="24"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="24"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+    </row>
+    <row r="44" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B44" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C43" s="41"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="27"/>
-      <c r="F43" s="40">
+      <c r="C44" s="40"/>
+      <c r="D44" s="26"/>
+      <c r="E44" s="26"/>
+      <c r="F44" s="39">
         <f>IF(AND(Unit_contrib_margin&gt;0,Total_fixed&gt;0),Total_fixed/Unit_contrib_margin,"")</f>
-        <v>12.613333333333333</v>
-      </c>
-      <c r="G43" s="26"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="27"/>
-      <c r="J43" s="28"/>
-    </row>
-    <row r="44" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B44" s="41" t="s">
+        <v>46.123076923076923</v>
+      </c>
+      <c r="G44" s="25"/>
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="27"/>
+    </row>
+    <row r="45" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B45" s="40" t="s">
         <v>20</v>
       </c>
-      <c r="C44" s="41"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="28"/>
-      <c r="G44" s="26"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="27"/>
-      <c r="J44" s="28"/>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B45" s="36" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0,0)</f>
+      <c r="C45" s="40"/>
+      <c r="D45" s="26"/>
+      <c r="E45" s="26"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="25"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="27"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B46" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="35"/>
+      <c r="D46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0,0)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.1,0)</f>
-        <v>1.2000000000000002</v>
-      </c>
-      <c r="F45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.2,0)</f>
-        <v>2.4000000000000004</v>
-      </c>
-      <c r="G45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.3,0)</f>
-        <v>3.5999999999999996</v>
-      </c>
-      <c r="H45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.4,0)</f>
-        <v>4.8000000000000007</v>
-      </c>
-      <c r="I45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.5,0)</f>
+      <c r="E46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.1,0)</f>
+        <v>2</v>
+      </c>
+      <c r="F46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.2,0)</f>
+        <v>4</v>
+      </c>
+      <c r="G46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.3,0)</f>
         <v>6</v>
       </c>
-      <c r="J45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.6,0)</f>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="K45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.7,0)</f>
-        <v>8.3999999999999986</v>
-      </c>
-      <c r="L45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.8,0)</f>
-        <v>9.6000000000000014</v>
-      </c>
-      <c r="M45" s="37">
-        <f>IF(Sales_volume_units,Sales_volume_units*0.9,0)</f>
-        <v>10.8</v>
-      </c>
-      <c r="N45" s="37">
-        <f>Sales_volume_units</f>
+      <c r="H46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.4,0)</f>
+        <v>8</v>
+      </c>
+      <c r="I46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.5,0)</f>
+        <v>10</v>
+      </c>
+      <c r="J46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.6,0)</f>
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="36" t="s">
+      <c r="K46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.7,0)</f>
+        <v>14</v>
+      </c>
+      <c r="L46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.8,0)</f>
+        <v>16</v>
+      </c>
+      <c r="M46" s="36">
+        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.9,0)</f>
+        <v>18</v>
+      </c>
+      <c r="N46" s="36">
+        <f>Sales_volume_unitsA</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B47" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="36"/>
-      <c r="D46" s="38">
-        <f t="shared" ref="D46:N46" si="0">Sales_price_unit</f>
-        <v>4600</v>
-      </c>
-      <c r="E46" s="38">
+      <c r="C47" s="35"/>
+      <c r="D47" s="37">
+        <f t="shared" ref="D47:N47" si="0">Sales_price_unitA</f>
+        <v>4100</v>
+      </c>
+      <c r="E47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="F46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="F47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="G46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="G47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="H46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="H47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="I46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="I47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="J46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="J47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="K46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="K47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="L46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="L47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="M46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="M47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-      <c r="N46" s="38">
+        <v>4100</v>
+      </c>
+      <c r="N47" s="37">
         <f t="shared" si="0"/>
-        <v>4600</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B47" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="C47" s="36"/>
-      <c r="D47" s="38">
-        <f t="shared" ref="D47:N47" si="1">Total_Subscription*D45</f>
+        <v>4100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B48" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="35"/>
+      <c r="D48" s="37">
+        <f t="shared" ref="D48:N48" si="1">Total_Subscription*D46</f>
         <v>0</v>
       </c>
-      <c r="E47" s="38">
+      <c r="E48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="F47" s="38">
+      <c r="F48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G47" s="38">
+      <c r="G48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="H47" s="38">
+      <c r="H48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I47" s="38">
+      <c r="I48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J47" s="38">
+      <c r="J48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K47" s="38">
+      <c r="K48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L47" s="38">
+      <c r="L48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M47" s="38">
+      <c r="M48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N47" s="38">
+      <c r="N48" s="37">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="36" t="s">
+    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B49" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C48" s="36"/>
-      <c r="D48" s="38">
-        <f t="shared" ref="D48:N48" si="2">Total_fixed</f>
-        <v>47300</v>
-      </c>
-      <c r="E48" s="38">
+      <c r="C49" s="35"/>
+      <c r="D49" s="37">
+        <f t="shared" ref="D49:N49" si="2">Total_fixed</f>
+        <v>149900</v>
+      </c>
+      <c r="E49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="F48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="F49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="G48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="G49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="H48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="H49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="I48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="I49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="J48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="J49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="K48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="K49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="L48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="L49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="M48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="M49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-      <c r="N48" s="38">
+        <v>149900</v>
+      </c>
+      <c r="N49" s="37">
         <f t="shared" si="2"/>
-        <v>47300</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B49" s="39" t="s">
+        <v>149900</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B50" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="C49" s="39"/>
-      <c r="D49" s="38">
-        <f t="shared" ref="D49:N49" si="3">Variable_Unit_Cost*D45</f>
+      <c r="C50" s="38"/>
+      <c r="D50" s="37">
+        <f t="shared" ref="D50:N50" si="3">Variable_Unit_Cost*D46</f>
         <v>0</v>
       </c>
-      <c r="E49" s="38">
+      <c r="E50" s="37">
         <f t="shared" si="3"/>
-        <v>1020.0000000000001</v>
-      </c>
-      <c r="F49" s="38">
+        <v>1700</v>
+      </c>
+      <c r="F50" s="37">
         <f t="shared" si="3"/>
-        <v>2040.0000000000002</v>
-      </c>
-      <c r="G49" s="38">
-        <f t="shared" si="3"/>
-        <v>3059.9999999999995</v>
-      </c>
-      <c r="H49" s="38">
-        <f t="shared" si="3"/>
-        <v>4080.0000000000005</v>
-      </c>
-      <c r="I49" s="38">
+        <v>3400</v>
+      </c>
+      <c r="G50" s="37">
         <f t="shared" si="3"/>
         <v>5100</v>
       </c>
-      <c r="J49" s="38">
+      <c r="H50" s="37">
         <f t="shared" si="3"/>
-        <v>6119.9999999999991</v>
-      </c>
-      <c r="K49" s="38">
+        <v>6800</v>
+      </c>
+      <c r="I50" s="37">
         <f t="shared" si="3"/>
-        <v>7139.9999999999991</v>
-      </c>
-      <c r="L49" s="38">
-        <f t="shared" si="3"/>
-        <v>8160.0000000000009</v>
-      </c>
-      <c r="M49" s="38">
-        <f t="shared" si="3"/>
-        <v>9180</v>
-      </c>
-      <c r="N49" s="38">
+        <v>8500</v>
+      </c>
+      <c r="J50" s="37">
         <f t="shared" si="3"/>
         <v>10200</v>
       </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B50" s="39" t="s">
+      <c r="K50" s="37">
+        <f t="shared" si="3"/>
+        <v>11900</v>
+      </c>
+      <c r="L50" s="37">
+        <f t="shared" si="3"/>
+        <v>13600</v>
+      </c>
+      <c r="M50" s="37">
+        <f t="shared" si="3"/>
+        <v>15300</v>
+      </c>
+      <c r="N50" s="37">
+        <f t="shared" si="3"/>
+        <v>17000</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B51" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C50" s="39"/>
-      <c r="D50" s="38">
-        <f t="shared" ref="D50:N50" si="4">SUM(D48:D49)</f>
-        <v>47300</v>
-      </c>
-      <c r="E50" s="38">
+      <c r="C51" s="38"/>
+      <c r="D51" s="37">
+        <f t="shared" ref="D51:N51" si="4">SUM(D49:D50)</f>
+        <v>149900</v>
+      </c>
+      <c r="E51" s="37">
         <f t="shared" si="4"/>
-        <v>48320</v>
-      </c>
-      <c r="F50" s="38">
+        <v>151600</v>
+      </c>
+      <c r="F51" s="37">
         <f t="shared" si="4"/>
-        <v>49340</v>
-      </c>
-      <c r="G50" s="38">
+        <v>153300</v>
+      </c>
+      <c r="G51" s="37">
         <f t="shared" si="4"/>
-        <v>50360</v>
-      </c>
-      <c r="H50" s="38">
+        <v>155000</v>
+      </c>
+      <c r="H51" s="37">
         <f t="shared" si="4"/>
-        <v>51380</v>
-      </c>
-      <c r="I50" s="38">
+        <v>156700</v>
+      </c>
+      <c r="I51" s="37">
         <f t="shared" si="4"/>
-        <v>52400</v>
-      </c>
-      <c r="J50" s="38">
+        <v>158400</v>
+      </c>
+      <c r="J51" s="37">
         <f t="shared" si="4"/>
-        <v>53420</v>
-      </c>
-      <c r="K50" s="38">
+        <v>160100</v>
+      </c>
+      <c r="K51" s="37">
         <f t="shared" si="4"/>
-        <v>54440</v>
-      </c>
-      <c r="L50" s="38">
+        <v>161800</v>
+      </c>
+      <c r="L51" s="37">
         <f t="shared" si="4"/>
-        <v>55460</v>
-      </c>
-      <c r="M50" s="38">
+        <v>163500</v>
+      </c>
+      <c r="M51" s="37">
         <f t="shared" si="4"/>
-        <v>56480</v>
-      </c>
-      <c r="N50" s="38">
+        <v>165200</v>
+      </c>
+      <c r="N51" s="37">
         <f t="shared" si="4"/>
-        <v>57500</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="36" t="s">
+        <v>166900</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="36"/>
-      <c r="D51" s="52">
-        <f>(D46*D45)+D47</f>
+      <c r="C52" s="35"/>
+      <c r="D52" s="51">
+        <f>(D47*D46)+D48</f>
         <v>0</v>
       </c>
-      <c r="E51" s="52">
-        <f t="shared" ref="E51:N51" si="5">(E46*E45)+E47</f>
-        <v>5520.0000000000009</v>
-      </c>
-      <c r="F51" s="52">
+      <c r="E52" s="51">
+        <f t="shared" ref="E52:N52" si="5">(E47*E46)+E48</f>
+        <v>8200</v>
+      </c>
+      <c r="F52" s="51">
         <f t="shared" si="5"/>
-        <v>11040.000000000002</v>
-      </c>
-      <c r="G51" s="52">
+        <v>16400</v>
+      </c>
+      <c r="G52" s="51">
         <f t="shared" si="5"/>
-        <v>16560</v>
-      </c>
-      <c r="H51" s="52">
+        <v>24600</v>
+      </c>
+      <c r="H52" s="51">
         <f t="shared" si="5"/>
-        <v>22080.000000000004</v>
-      </c>
-      <c r="I51" s="52">
+        <v>32800</v>
+      </c>
+      <c r="I52" s="51">
         <f t="shared" si="5"/>
-        <v>27600</v>
-      </c>
-      <c r="J51" s="52">
+        <v>41000</v>
+      </c>
+      <c r="J52" s="51">
         <f t="shared" si="5"/>
-        <v>33120</v>
-      </c>
-      <c r="K51" s="52">
+        <v>49200</v>
+      </c>
+      <c r="K52" s="51">
         <f t="shared" si="5"/>
-        <v>38639.999999999993</v>
-      </c>
-      <c r="L51" s="52">
+        <v>57400</v>
+      </c>
+      <c r="L52" s="51">
         <f t="shared" si="5"/>
-        <v>44160.000000000007</v>
-      </c>
-      <c r="M51" s="52">
+        <v>65600</v>
+      </c>
+      <c r="M52" s="51">
         <f t="shared" si="5"/>
-        <v>49680</v>
-      </c>
-      <c r="N51" s="52">
+        <v>73800</v>
+      </c>
+      <c r="N52" s="51">
         <f t="shared" si="5"/>
-        <v>55200</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B52" s="39" t="s">
+        <v>82000</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B53" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C52" s="39"/>
-      <c r="D52" s="53">
-        <f>D51-D50</f>
-        <v>-47300</v>
-      </c>
-      <c r="E52" s="53">
-        <f t="shared" ref="E52:N52" si="6">E51-E50</f>
-        <v>-42800</v>
-      </c>
-      <c r="F52" s="53">
+      <c r="C53" s="38"/>
+      <c r="D53" s="52">
+        <f>D52-D51</f>
+        <v>-149900</v>
+      </c>
+      <c r="E53" s="52">
+        <f t="shared" ref="E53:N53" si="6">E52-E51</f>
+        <v>-143400</v>
+      </c>
+      <c r="F53" s="52">
         <f t="shared" si="6"/>
-        <v>-38300</v>
-      </c>
-      <c r="G52" s="53">
+        <v>-136900</v>
+      </c>
+      <c r="G53" s="52">
         <f t="shared" si="6"/>
-        <v>-33800</v>
-      </c>
-      <c r="H52" s="53">
+        <v>-130400</v>
+      </c>
+      <c r="H53" s="52">
         <f t="shared" si="6"/>
-        <v>-29299.999999999996</v>
-      </c>
-      <c r="I52" s="53">
+        <v>-123900</v>
+      </c>
+      <c r="I53" s="52">
         <f t="shared" si="6"/>
-        <v>-24800</v>
-      </c>
-      <c r="J52" s="53">
+        <v>-117400</v>
+      </c>
+      <c r="J53" s="52">
         <f t="shared" si="6"/>
-        <v>-20300</v>
-      </c>
-      <c r="K52" s="53">
+        <v>-110900</v>
+      </c>
+      <c r="K53" s="52">
         <f t="shared" si="6"/>
-        <v>-15800.000000000007</v>
-      </c>
-      <c r="L52" s="53">
+        <v>-104400</v>
+      </c>
+      <c r="L53" s="52">
         <f t="shared" si="6"/>
-        <v>-11299.999999999993</v>
-      </c>
-      <c r="M52" s="53">
+        <v>-97900</v>
+      </c>
+      <c r="M53" s="52">
         <f t="shared" si="6"/>
-        <v>-6800</v>
-      </c>
-      <c r="N52" s="53">
+        <v>-91400</v>
+      </c>
+      <c r="N53" s="52">
         <f t="shared" si="6"/>
-        <v>-2300</v>
+        <v>-84900</v>
       </c>
     </row>
   </sheetData>
@@ -3953,13 +4795,13 @@
     </scenario>
   </scenarios>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F44 F25:F26 F55:F65547 G4 G2 G38 F37 G40 F39 D49:N49 H56:H65547 J43:J44 G26 F9:F11 G9:G19" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations disablePrompts="1" count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F45 F26:F27 F56:F65548 G10:G20 G2 G39 F38 G41 F40 D50:N50 H57:H65548 J44:J45 G27 F10:F12" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>-10000000</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F43 G21:G25 H4 H2 F20:F24 G56:G65547 G37 F38 G39 G5:G7" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between (10,000,000) and 10,000,000." sqref="F12:F19 F27:F36 F9:F10 F5:F6" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F44 G22:G26 G8 H2 F21:F25 G57:G65548 G38 F39 G40" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between (10,000,000) and 10,000,000." sqref="F13:F20 F28:F37 F10:F11" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>-10000000</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
@@ -3987,7 +4829,7 @@
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>790575</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>152400</xdr:rowOff>
+                    <xdr:rowOff>142875</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4024,13 +4866,13 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>18</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
-                    <xdr:row>18</xdr:row>
+                    <xdr:row>19</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4046,13 +4888,13 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>15</xdr:row>
+                    <xdr:row>16</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>828675</xdr:colOff>
-                    <xdr:row>16</xdr:row>
+                    <xdr:row>17</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4062,20 +4904,20 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId8" name="Scroll Bar 10">
+            <control shapeId="1046" r:id="rId8" name="Scroll Bar 22">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>25</xdr:row>
-                    <xdr:rowOff>190500</xdr:rowOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
-                    <xdr:colOff>828675</xdr:colOff>
-                    <xdr:row>26</xdr:row>
-                    <xdr:rowOff>161925</xdr:rowOff>
+                    <xdr:colOff>790575</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4084,20 +4926,42 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId9" name="Scroll Bar 22">
+            <control shapeId="1048" r:id="rId9" name="Scroll Bar 24">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>4</xdr:row>
+                    <xdr:rowOff>152400</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>8</xdr:col>
+                    <xdr:colOff>809625</xdr:colOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1050" r:id="rId10" name="Scroll Bar 26">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>10</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>8</xdr:row>
+                    <xdr:row>5</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
+                    <xdr:col>10</xdr:col>
                     <xdr:colOff>790575</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>

</xml_diff>

<commit_message>
added multi tier pricing WIP
</commit_message>
<xml_diff>
--- a/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
+++ b/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
@@ -22,40 +22,40 @@
     <definedName name="_Order1" hidden="1">0</definedName>
     <definedName name="_Series" hidden="1">Variables!$B$3</definedName>
     <definedName name="_Shading" hidden="1">Variables!$B$2</definedName>
-    <definedName name="Breakeven_point">'Breakeven Analysis Data'!$F$44</definedName>
+    <definedName name="Breakeven_point">'Breakeven Analysis Data'!$F$45</definedName>
     <definedName name="Company_name">'Breakeven Analysis Data'!$B$2</definedName>
     <definedName name="DATA_01" hidden="1">'Breakeven Analysis Data'!$B$2:$B$3</definedName>
     <definedName name="DATA_02" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_03" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_04" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_05" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
-    <definedName name="DATA_06" hidden="1">'Breakeven Analysis Data'!$F$13:$F$20</definedName>
+    <definedName name="DATA_06" hidden="1">'Breakeven Analysis Data'!$F$14:$F$21</definedName>
     <definedName name="DATA_07" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
-    <definedName name="DATA_08" hidden="1">'Breakeven Analysis Data'!$H$4</definedName>
-    <definedName name="Fixed_costs">'Breakeven Analysis Data'!$F$28:$F$37</definedName>
-    <definedName name="Gross_margin">'Breakeven Analysis Data'!$G$25</definedName>
+    <definedName name="DATA_08" hidden="1">'Breakeven Analysis Data'!$H$5</definedName>
+    <definedName name="Fixed_costs">'Breakeven Analysis Data'!$F$29:$F$38</definedName>
+    <definedName name="Gross_margin">'Breakeven Analysis Data'!$G$26</definedName>
     <definedName name="IntroPrintArea" hidden="1">#REF!</definedName>
     <definedName name="Look1Area">#REF!</definedName>
     <definedName name="Look2Area">#REF!</definedName>
     <definedName name="Look3Area">#REF!</definedName>
     <definedName name="Look4Area">#REF!</definedName>
     <definedName name="Look5Area">#REF!</definedName>
-    <definedName name="Net_profit">'Breakeven Analysis Data'!$G$40</definedName>
-    <definedName name="Sales_price_unitA">'Breakeven Analysis Data'!$F$5</definedName>
-    <definedName name="Sales_price_unitB">'Breakeven Analysis Data'!$H$5</definedName>
-    <definedName name="Sales_price_unitC">'Breakeven Analysis Data'!$J$5</definedName>
-    <definedName name="Sales_volume_unitsA">'Breakeven Analysis Data'!$F$6</definedName>
-    <definedName name="Sales_volume_unitsB">'Breakeven Analysis Data'!$H$6</definedName>
-    <definedName name="Sales_volume_unitsC">'Breakeven Analysis Data'!$J$6</definedName>
+    <definedName name="Net_profit">'Breakeven Analysis Data'!$G$41</definedName>
+    <definedName name="Sales_price_unitA">'Breakeven Analysis Data'!$F$6</definedName>
+    <definedName name="Sales_price_unitB">'Breakeven Analysis Data'!$H$6</definedName>
+    <definedName name="Sales_price_unitC">'Breakeven Analysis Data'!$J$6</definedName>
+    <definedName name="Sales_volume_unitsA">'Breakeven Analysis Data'!$F$7</definedName>
+    <definedName name="Sales_volume_unitsB">'Breakeven Analysis Data'!$H$7</definedName>
+    <definedName name="Sales_volume_unitsC">'Breakeven Analysis Data'!$J$7</definedName>
     <definedName name="TemplatePrintArea">'Breakeven Analysis Data'!$B$1:$G$5</definedName>
-    <definedName name="Total_fixed">'Breakeven Analysis Data'!$G$38</definedName>
-    <definedName name="Total_Sales">'Breakeven Analysis Data'!$G$8</definedName>
-    <definedName name="Total_Subscription">'Breakeven Analysis Data'!$G$11</definedName>
-    <definedName name="Total_variable">'Breakeven Analysis Data'!$G$22</definedName>
-    <definedName name="Unit_contrib_margin">'Breakeven Analysis Data'!$F$24</definedName>
-    <definedName name="Variable_cost_unit">'Breakeven Analysis Data'!$F$21</definedName>
-    <definedName name="Variable_costs_unit">'Breakeven Analysis Data'!$F$13:$F$20</definedName>
-    <definedName name="Variable_Unit_Cost">'Breakeven Analysis Data'!$F$21</definedName>
+    <definedName name="Total_fixed">'Breakeven Analysis Data'!$G$39</definedName>
+    <definedName name="Total_Sales">'Breakeven Analysis Data'!$G$9</definedName>
+    <definedName name="Total_Subscription">'Breakeven Analysis Data'!$G$12</definedName>
+    <definedName name="Total_variable">'Breakeven Analysis Data'!$G$23</definedName>
+    <definedName name="Unit_contrib_margin">'Breakeven Analysis Data'!$F$25</definedName>
+    <definedName name="Variable_cost_unit">'Breakeven Analysis Data'!$F$22</definedName>
+    <definedName name="Variable_costs_unit">'Breakeven Analysis Data'!$F$14:$F$21</definedName>
+    <definedName name="Variable_Unit_Cost">'Breakeven Analysis Data'!$F$22</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -75,7 +75,7 @@
     <author>Tuur</author>
   </authors>
   <commentList>
-    <comment ref="F5" authorId="0" shapeId="0" xr:uid="{3A85B171-98A2-477D-A064-7900A68AFBB8}">
+    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{3A85B171-98A2-477D-A064-7900A68AFBB8}">
       <text>
         <r>
           <rPr>
@@ -90,7 +90,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H5" authorId="0" shapeId="0" xr:uid="{7D0A91FE-B1FC-4772-B671-83EC5EA0EC0D}">
+    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{7D0A91FE-B1FC-4772-B671-83EC5EA0EC0D}">
       <text>
         <r>
           <rPr>
@@ -105,7 +105,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{C306B6D9-DB5D-41DC-8381-E112C47706A1}">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{C306B6D9-DB5D-41DC-8381-E112C47706A1}">
       <text>
         <r>
           <rPr>
@@ -120,7 +120,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{5217D6D1-5CD7-4075-AFE8-EA322F49B4C9}">
+    <comment ref="F7" authorId="0" shapeId="0" xr:uid="{5217D6D1-5CD7-4075-AFE8-EA322F49B4C9}">
       <text>
         <r>
           <rPr>
@@ -133,7 +133,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{831FB1F6-E4B8-4DC3-9B71-8B472336E9DB}">
+    <comment ref="H7" authorId="0" shapeId="0" xr:uid="{831FB1F6-E4B8-4DC3-9B71-8B472336E9DB}">
       <text>
         <r>
           <rPr>
@@ -146,7 +146,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{30555F1F-FBCD-421F-812F-AD65AB932B8F}">
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{30555F1F-FBCD-421F-812F-AD65AB932B8F}">
       <text>
         <r>
           <rPr>
@@ -159,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F10" authorId="0" shapeId="0" xr:uid="{A3A9E55F-847E-4661-913D-184F52F6F529}">
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{A3A9E55F-847E-4661-913D-184F52F6F529}">
       <text>
         <r>
           <rPr>
@@ -172,7 +172,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F13" authorId="0" shapeId="0" xr:uid="{5CF3165E-FCBD-453E-AF2A-EA2B9BFC17C7}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{5CF3165E-FCBD-453E-AF2A-EA2B9BFC17C7}">
       <text>
         <r>
           <rPr>
@@ -186,7 +186,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{5D839EBC-3BE3-4C34-8563-6F5A98C52E6E}">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{5D839EBC-3BE3-4C34-8563-6F5A98C52E6E}">
       <text>
         <r>
           <rPr>
@@ -200,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{DF3550BB-FD51-4154-B794-6A8344BA2F43}">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{DF3550BB-FD51-4154-B794-6A8344BA2F43}">
       <text>
         <r>
           <rPr>
@@ -213,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{70740BD0-CC66-4C54-86D3-8CFA9D18EBC2}">
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{70740BD0-CC66-4C54-86D3-8CFA9D18EBC2}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F19" authorId="0" shapeId="0" xr:uid="{58D98360-D15F-4E39-A36D-F6F27D06BD03}">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{58D98360-D15F-4E39-A36D-F6F27D06BD03}">
       <text>
         <r>
           <rPr>
@@ -251,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{0311ABD3-7CCC-4345-89C5-881F9C7EA603}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{0311ABD3-7CCC-4345-89C5-881F9C7EA603}">
       <text>
         <r>
           <rPr>
@@ -264,7 +264,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{F6D60EF9-0745-4CB6-8B69-14B527E69522}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{F6D60EF9-0745-4CB6-8B69-14B527E69522}">
       <text>
         <r>
           <rPr>
@@ -279,7 +279,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{609A7C58-C559-486A-8D2D-85B7A7A7AE0A}">
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{609A7C58-C559-486A-8D2D-85B7A7A7AE0A}">
       <text>
         <r>
           <rPr>
@@ -294,7 +294,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{EA10A0B4-ED7D-4B1B-9DF6-7CF415632FED}">
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{EA10A0B4-ED7D-4B1B-9DF6-7CF415632FED}">
       <text>
         <r>
           <rPr>
@@ -308,7 +308,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{165A2A66-A40C-4D4A-8EF3-CD46A0C51E76}">
+    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{165A2A66-A40C-4D4A-8EF3-CD46A0C51E76}">
       <text>
         <r>
           <rPr>
@@ -342,7 +342,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{0D7BD022-B106-460F-B833-13D1C6EA7135}">
+    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{0D7BD022-B106-460F-B833-13D1C6EA7135}">
       <text>
         <r>
           <rPr>
@@ -361,7 +361,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>_Example</t>
   </si>
@@ -524,7 +524,13 @@
     <t>Sales price</t>
   </si>
   <si>
-    <t>Sales</t>
+    <t>Discount:</t>
+  </si>
+  <si>
+    <t>Sales (1 year per period)</t>
+  </si>
+  <si>
+    <t>Amount of users</t>
   </si>
 </sst>
 </file>
@@ -666,7 +672,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -803,6 +809,19 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" applyFont="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -843,10 +862,6 @@
     </xf>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="centerContinuous"/>
-    </xf>
-    <xf numFmtId="37" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
@@ -941,24 +956,28 @@
     <xf numFmtId="38" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="7" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="7" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="37" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1199,7 +1218,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('Breakeven Analysis Data'!$C$21,'Breakeven Analysis Data'!$C$24)</c:f>
+              <c:f>('Breakeven Analysis Data'!$C$22,'Breakeven Analysis Data'!$C$25)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1213,7 +1232,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Breakeven Analysis Data'!$F$21,'Breakeven Analysis Data'!$F$24)</c:f>
+              <c:f>('Breakeven Analysis Data'!$F$22,'Breakeven Analysis Data'!$F$25)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1221,7 +1240,7 @@
                   <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3250</c:v>
+                  <c:v>2550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1486,7 +1505,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$C$14:$C$20</c:f>
+              <c:f>'Breakeven Analysis Data'!$C$15:$C$21</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1515,7 +1534,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$F$13:$F$20</c:f>
+              <c:f>'Breakeven Analysis Data'!$F$14:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="8"/>
@@ -1794,7 +1813,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('Breakeven Analysis Data'!$C$21,'Breakeven Analysis Data'!$C$24)</c:f>
+              <c:f>('Breakeven Analysis Data'!$C$22,'Breakeven Analysis Data'!$C$25)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1808,7 +1827,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Breakeven Analysis Data'!$F$21,'Breakeven Analysis Data'!$F$24)</c:f>
+              <c:f>('Breakeven Analysis Data'!$F$22,'Breakeven Analysis Data'!$F$25)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="2"/>
@@ -1816,7 +1835,7 @@
                   <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3250</c:v>
+                  <c:v>2550</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1942,291 +1961,6 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" u="none" strike="noStrike" baseline="0">
-                <a:solidFill>
-                  <a:srgbClr val="000000"/>
-                </a:solidFill>
-                <a:latin typeface="Tahoma"/>
-                <a:ea typeface="Tahoma"/>
-                <a:cs typeface="Tahoma"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Unit Contribution Margin</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.16864589372884201"/>
-          <c:y val="0.175999644781244"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25400">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout>
-        <c:manualLayout>
-          <c:layoutTarget val="inner"/>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.21377659811982799"/>
-          <c:y val="0.25999974609399801"/>
-          <c:w val="0.339667261457061"/>
-          <c:h val="0.57199944140679504"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:pieChart>
-        <c:varyColors val="1"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="8080FF"/>
-            </a:solidFill>
-            <a:ln w="12700">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:prstDash val="solid"/>
-            </a:ln>
-          </c:spPr>
-          <c:dPt>
-            <c:idx val="0"/>
-            <c:bubble3D val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000000-A48D-4222-A4F8-4CEB8D22B86C}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
-          <c:dLbls>
-            <c:numFmt formatCode="0%" sourceLinked="0"/>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="25400">
-                <a:noFill/>
-              </a:ln>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="850" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                    <a:solidFill>
-                      <a:srgbClr val="000000"/>
-                    </a:solidFill>
-                    <a:latin typeface="Tahoma"/>
-                    <a:ea typeface="Tahoma"/>
-                    <a:cs typeface="Tahoma"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-BE"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="1"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="1"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-            </c:extLst>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>('Breakeven Analysis Data'!$C$21,'Breakeven Analysis Data'!$C$24)</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Breakeven Analysis Data'!$C$21</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Variable costs per unit</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                  <c15:fullRef>
-                    <c15:sqref>('Breakeven Analysis Data'!$F$21,'Breakeven Analysis Data'!$F$24)</c15:sqref>
-                  </c15:fullRef>
-                </c:ext>
-              </c:extLst>
-              <c:f>'Breakeven Analysis Data'!$F$21</c:f>
-              <c:numCache>
-                <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>850</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-              <c15:categoryFilterExceptions>
-                <c15:categoryFilterException>
-                  <c15:sqref>'Breakeven Analysis Data'!$F$24</c15:sqref>
-                  <c15:spPr xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <a:solidFill>
-                      <a:srgbClr val="802060"/>
-                    </a:solidFill>
-                    <a:ln w="12700">
-                      <a:solidFill>
-                        <a:srgbClr val="000000"/>
-                      </a:solidFill>
-                      <a:prstDash val="solid"/>
-                    </a:ln>
-                  </c15:spPr>
-                  <c15:bubble3D val="0"/>
-                </c15:categoryFilterException>
-              </c15:categoryFilterExceptions>
-            </c:ext>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-A48D-4222-A4F8-4CEB8D22B86C}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-          <c:showLeaderLines val="1"/>
-        </c:dLbls>
-        <c:firstSliceAng val="0"/>
-      </c:pieChart>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln w="25400">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.68408513662632997"/>
-          <c:y val="0.183999763187496"/>
-          <c:w val="0.30641311463145499"/>
-          <c:h val="0.1"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="25400">
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="715" b="0" i="0" u="none" strike="noStrike" baseline="0">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:latin typeface="Tahoma"/>
-              <a:ea typeface="Tahoma"/>
-              <a:cs typeface="Tahoma"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-BE"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="zero"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="FFFFFF"/>
-    </a:solidFill>
-    <a:ln w="9525">
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr sz="850" b="0" i="0" u="none" strike="noStrike" baseline="0">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:latin typeface="Tahoma"/>
-          <a:ea typeface="Tahoma"/>
-          <a:cs typeface="Tahoma"/>
-        </a:defRPr>
-      </a:pPr>
-      <a:endParaRPr lang="en-BE"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.5" footer="0.5"/>
-    <c:pageSetup orientation="landscape"/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
               <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
@@ -2280,7 +2014,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$49</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$50</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2314,42 +2048,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$49:$N$49</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$50:$N$50</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2366,7 +2100,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$51</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$52</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2400,42 +2134,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$51:$N$51</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$52:$N$52</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>149900</c:v>
+                  <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>151600</c:v>
+                  <c:v>148725</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>153300</c:v>
+                  <c:v>152550</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>155000</c:v>
+                  <c:v>156375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>156700</c:v>
+                  <c:v>160200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>158400</c:v>
+                  <c:v>164025</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>160100</c:v>
+                  <c:v>167850</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>161800</c:v>
+                  <c:v>171675</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>163500</c:v>
+                  <c:v>175500</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>165200</c:v>
+                  <c:v>179325</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>166900</c:v>
+                  <c:v>183150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2452,7 +2186,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$52</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2486,7 +2220,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$52:$N$52</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$53:$N$53</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2494,34 +2228,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8200</c:v>
+                  <c:v>17550</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16400</c:v>
+                  <c:v>35100</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24600</c:v>
+                  <c:v>52650</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>32800</c:v>
+                  <c:v>70200</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>41000</c:v>
+                  <c:v>87750</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49200</c:v>
+                  <c:v>105300</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>57400</c:v>
+                  <c:v>122849.99999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>65600</c:v>
+                  <c:v>140400</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>73800</c:v>
+                  <c:v>157950</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>82000</c:v>
+                  <c:v>175500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2538,7 +2272,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$53</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2570,42 +2304,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$53:$N$53</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$54:$N$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-149900</c:v>
+                  <c:v>-144900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-143400</c:v>
+                  <c:v>-131175</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-136900</c:v>
+                  <c:v>-117450</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-130400</c:v>
+                  <c:v>-103725</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-123900</c:v>
+                  <c:v>-90000</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-117400</c:v>
+                  <c:v>-76275</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-110900</c:v>
+                  <c:v>-62550</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-104400</c:v>
+                  <c:v>-48825.000000000015</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-97900</c:v>
+                  <c:v>-35100</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-91400</c:v>
+                  <c:v>-21375</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-84900</c:v>
+                  <c:v>-7650</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2907,31 +2641,31 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$5" horiz="1" inc="100" max="10000" min="500" page="10" val="4100"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" inc="100" max="10000" min="500" page="10" val="3400"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" max="50" min="1" page="10" val="20"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$7" horiz="1" max="50" min="1" page="10" val="30"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$19" horiz="1" inc="100" max="1000" page="10" val="300"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$20" horiz="1" inc="100" max="1000" page="10" val="300"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$17" horiz="1" inc="50" max="1000" page="10" val="250"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$18" horiz="1" inc="50" max="1000" page="10" val="250"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$10" horiz="1" inc="100" max="10000" page="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$11" horiz="1" inc="100" max="10000" page="0" val="500"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$6" horiz="1" max="50" min="1" page="10" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$7" horiz="1" max="50" min="1" page="10" val="10"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$J$6" horiz="1" max="50" min="1" page="10" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$J$7" horiz="1" max="50" min="1" page="10" val="5"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2946,7 +2680,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>339587</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>25466</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2978,13 +2712,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>165976</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>318376</xdr:colOff>
-      <xdr:row>43</xdr:row>
+      <xdr:row>44</xdr:row>
       <xdr:rowOff>241300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3018,14 +2752,14 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>3</xdr:row>
+          <xdr:row>4</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>790575</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>139262</xdr:rowOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3068,13 +2802,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>4</xdr:row>
+          <xdr:row>5</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>790575</xdr:colOff>
-          <xdr:row>5</xdr:row>
+          <xdr:row>6</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -3118,13 +2852,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>19</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>20</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -3168,13 +2902,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>16</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>828675</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -3218,13 +2952,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
           <xdr:colOff>790575</xdr:colOff>
-          <xdr:row>9</xdr:row>
+          <xdr:row>10</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -3267,14 +3001,14 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>26933</xdr:colOff>
-          <xdr:row>4</xdr:row>
-          <xdr:rowOff>156013</xdr:rowOff>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>152400</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>809624</xdr:colOff>
-          <xdr:row>6</xdr:row>
+          <xdr:colOff>809625</xdr:colOff>
+          <xdr:row>7</xdr:row>
           <xdr:rowOff>28575</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -3285,7 +3019,7 @@
                   <a14:compatExt spid="_x0000_s1048"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7147AF22-DC74-4F9E-8B86-A36A4AD7D1E6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000018040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3317,15 +3051,15 @@
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>20364</xdr:colOff>
-          <xdr:row>5</xdr:row>
-          <xdr:rowOff>4927</xdr:rowOff>
+          <xdr:colOff>19050</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>10</xdr:col>
-          <xdr:colOff>791561</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>4927</xdr:rowOff>
+          <xdr:colOff>790575</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3335,7 +3069,7 @@
                   <a14:compatExt spid="_x0000_s1050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E19ABF4-45CD-45D5-AD45-D9A156AD54D5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00001A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3380,7 +3114,7 @@
         <xdr:cNvPr id="14" name="Chart 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{234553F2-1143-4083-ACD9-F85DFEC544EB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3395,44 +3129,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>77604</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>343890</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>26</xdr:col>
-      <xdr:colOff>271101</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>192497</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="15" name="Chart 7">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{989F1835-9811-4745-945F-5107EAFA85E9}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3800,10 +3496,10 @@
     <tabColor indexed="26"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3813,386 +3509,385 @@
     <col min="3" max="3" width="9.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="20" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="19" customWidth="1"/>
     <col min="7" max="7" width="15.42578125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="19" customWidth="1"/>
     <col min="9" max="14" width="12.7109375" style="1" customWidth="1"/>
     <col min="15" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="61.5" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="4"/>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="23"/>
-    </row>
-    <row r="2" spans="1:10" ht="27.75" x14ac:dyDescent="0.4">
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="22"/>
+    </row>
+    <row r="2" spans="1:11" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A2" s="4"/>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="28"/>
+      <c r="C2" s="27"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="16"/>
       <c r="H2" s="9"/>
     </row>
-    <row r="3" spans="1:10" s="14" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="41"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="66">
+    </row>
+    <row r="4" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="41" t="s">
+        <v>51</v>
+      </c>
+      <c r="C4" s="41"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="65" t="s">
+        <v>50</v>
+      </c>
+      <c r="H4" s="67">
         <v>0.1</v>
       </c>
-      <c r="J3" s="66">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4"/>
-      <c r="B4" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="29"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="61">
-        <v>50</v>
-      </c>
-      <c r="G4" s="60"/>
-      <c r="H4" s="63">
-        <v>200</v>
-      </c>
-      <c r="I4" s="67"/>
-      <c r="J4" s="62">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="I4" s="14"/>
+      <c r="J4" s="67">
+        <v>0.2</v>
+      </c>
+      <c r="K4" s="14"/>
+    </row>
+    <row r="5" spans="1:11" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4"/>
       <c r="B5" s="11"/>
-      <c r="C5" s="53" t="s">
-        <v>49</v>
+      <c r="C5" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="64">
-        <v>4100</v>
-      </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="64">
-        <f>Sales_price_unitA*(H4/F4)*(1-H3)</f>
-        <v>14760</v>
-      </c>
-      <c r="J5" s="64">
-        <f>Sales_price_unitA*(J4/F4)*(1-J3)</f>
-        <v>30750</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F5" s="60">
+        <v>50</v>
+      </c>
+      <c r="G5" s="59"/>
+      <c r="H5" s="66">
+        <v>200</v>
+      </c>
+      <c r="I5" s="63"/>
+      <c r="J5" s="68">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="12"/>
-      <c r="C6" s="12" t="s">
-        <v>23</v>
+      <c r="C6" s="52" t="s">
+        <v>49</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="44">
-        <v>20</v>
-      </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="44">
-        <v>10</v>
-      </c>
-      <c r="J6" s="44">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F6" s="61">
+        <v>3400</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="61">
+        <f>Sales_price_unitA*(H5/F5)*(1-H4)</f>
+        <v>12240</v>
+      </c>
+      <c r="J6" s="61">
+        <f>Sales_price_unitA*(J5/F5)*(1-J4)</f>
+        <v>27200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="12"/>
-      <c r="C7" s="12"/>
+      <c r="C7" s="12" t="s">
+        <v>23</v>
+      </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="68">
+      <c r="F7" s="43">
+        <v>30</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="43">
+        <v>10</v>
+      </c>
+      <c r="J7" s="43">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B8" s="34"/>
+      <c r="C8" s="12"/>
+      <c r="F8" s="64">
         <f>IF(OR(Sales_price_unitA&lt;&gt;0,Sales_volume_unitsA&lt;&gt;0),Sales_price_unitA*Sales_volume_unitsA,0)</f>
-        <v>82000</v>
-      </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="68">
+        <v>102000</v>
+      </c>
+      <c r="G8" s="8"/>
+      <c r="H8" s="64">
         <f>IF(OR(Sales_price_unitB&lt;&gt;0,Sales_volume_unitsB&lt;&gt;0),Sales_price_unitB*Sales_volume_unitsB,0)</f>
-        <v>147600</v>
-      </c>
-      <c r="J7" s="68">
+        <v>122400</v>
+      </c>
+      <c r="J8" s="64">
         <f>IF(OR(Sales_price_unitC&lt;&gt;0,Sales_volume_unitsC&lt;&gt;0),Sales_price_unitC*Sales_volume_unitsC,0)</f>
-        <v>307500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B8" s="35"/>
-      <c r="C8" s="22" t="s">
+        <v>136000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B9" s="34"/>
+      <c r="C9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="65">
-        <f>F7+H7+J7</f>
-        <v>537100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B9" s="35"/>
-      <c r="C9" s="22"/>
-      <c r="G9" s="20"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G9" s="62">
+        <f>F8+H8+J8</f>
+        <v>360400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="11"/>
-      <c r="C10" s="53" t="s">
-        <v>46</v>
-      </c>
+      <c r="C10" s="21"/>
       <c r="E10" s="4"/>
-      <c r="F10" s="44">
-        <v>0</v>
-      </c>
-      <c r="G10" s="18"/>
-    </row>
-    <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G10" s="19"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="11"/>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="43">
+        <v>500</v>
+      </c>
+      <c r="G11" s="17"/>
+    </row>
+    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="59">
-        <f>F10</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="43" t="s">
+      <c r="E12" s="4"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="58">
+        <f>F11</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="4"/>
+      <c r="B13" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="43"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A13" s="4"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="35" t="s">
-        <v>36</v>
-      </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="31">
-        <v>100</v>
-      </c>
-      <c r="G13" s="56"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="42"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="11"/>
-      <c r="C14" s="53" t="s">
-        <v>30</v>
+      <c r="C14" s="34" t="s">
+        <v>36</v>
       </c>
       <c r="E14" s="3"/>
-      <c r="F14" s="31"/>
-      <c r="G14" s="54"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F14" s="30">
+        <v>100</v>
+      </c>
+      <c r="G14" s="55"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="11"/>
-      <c r="C15" s="53" t="s">
-        <v>31</v>
+      <c r="C15" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="31">
-        <v>100</v>
-      </c>
-      <c r="G15" s="54"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F15" s="30"/>
+      <c r="G15" s="53"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="11"/>
-      <c r="C16" s="53" t="s">
-        <v>41</v>
+      <c r="C16" s="52" t="s">
+        <v>31</v>
       </c>
       <c r="E16" s="3"/>
-      <c r="F16" s="31">
-        <v>0</v>
-      </c>
-      <c r="G16" s="54"/>
+      <c r="F16" s="30">
+        <v>100</v>
+      </c>
+      <c r="G16" s="53"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="11"/>
-      <c r="C17" s="53" t="s">
-        <v>42</v>
+      <c r="C17" s="52" t="s">
+        <v>41</v>
       </c>
       <c r="E17" s="3"/>
-      <c r="F17" s="31">
-        <v>250</v>
-      </c>
-      <c r="G17" s="54"/>
+      <c r="F17" s="30">
+        <v>0</v>
+      </c>
+      <c r="G17" s="53"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="11"/>
-      <c r="C18" s="53" t="s">
-        <v>32</v>
+      <c r="C18" s="52" t="s">
+        <v>42</v>
       </c>
       <c r="E18" s="3"/>
-      <c r="F18" s="31">
-        <v>0</v>
-      </c>
-      <c r="G18" s="54"/>
+      <c r="F18" s="30">
+        <v>250</v>
+      </c>
+      <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="11"/>
-      <c r="C19" s="53" t="s">
-        <v>29</v>
+      <c r="C19" s="52" t="s">
+        <v>32</v>
       </c>
       <c r="E19" s="3"/>
-      <c r="F19" s="31">
-        <v>300</v>
-      </c>
-      <c r="G19" s="54"/>
+      <c r="F19" s="30">
+        <v>0</v>
+      </c>
+      <c r="G19" s="53"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="11"/>
-      <c r="C20" s="11" t="s">
-        <v>21</v>
+      <c r="C20" s="52" t="s">
+        <v>29</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="31">
-        <v>100</v>
-      </c>
-      <c r="G20" s="54"/>
+      <c r="F20" s="30">
+        <v>300</v>
+      </c>
+      <c r="G20" s="53"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="11"/>
-      <c r="C21" s="34" t="s">
+      <c r="C21" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="30">
+        <v>100</v>
+      </c>
+      <c r="G21" s="53"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="4"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="33">
+      <c r="E22" s="3"/>
+      <c r="F22" s="32">
         <f>IF(SUM(Variable_costs_unit),SUM(Variable_costs_unit),0)</f>
         <v>850</v>
       </c>
-      <c r="G21" s="55"/>
-    </row>
-    <row r="22" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="34" t="s">
-        <v>22</v>
-      </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="19"/>
-      <c r="G22" s="45">
-        <f>IF(Variable_Unit_Cost,Variable_Unit_Cost*Sales_volume_unitsA,0)</f>
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G22" s="54"/>
+    </row>
+    <row r="23" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="11"/>
-      <c r="C23" s="34"/>
+      <c r="C23" s="33" t="s">
+        <v>22</v>
+      </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="19"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="1"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="44">
+        <f>IF(Variable_Unit_Cost,Variable_Unit_Cost*(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC),0)</f>
+        <v>38250</v>
+      </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="11"/>
-      <c r="C24" s="34" t="s">
-        <v>16</v>
-      </c>
+      <c r="C24" s="33"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="32">
-        <f>IF(Sales_price_unitA&gt;0,MAX(0,Sales_price_unitA-Variable_Unit_Cost),0)</f>
-        <v>3250</v>
-      </c>
-      <c r="G24" s="19"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="34" t="s">
-        <v>10</v>
+      <c r="C25" s="33" t="s">
+        <v>16</v>
       </c>
       <c r="E25" s="3"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="32">
-        <f>IF(OR(Total_Sales&lt;&gt;0,Total_variable&lt;&gt;0),Total_Sales-Total_variable,0)</f>
-        <v>520100</v>
-      </c>
+      <c r="F25" s="31">
+        <f>IF(Sales_price_unitA&gt;0,MAX(0,Sales_price_unitA-Variable_Unit_Cost),0)</f>
+        <v>2550</v>
+      </c>
+      <c r="G25" s="18"/>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="21"/>
+      <c r="C26" s="33" t="s">
+        <v>10</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="18"/>
-      <c r="G26" s="19"/>
+      <c r="G26" s="31">
+        <f>IF(OR(Total_Sales&lt;&gt;0,Total_variable&lt;&gt;0),Total_Sales-Total_variable,0)</f>
+        <v>322150</v>
+      </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-      <c r="B27" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="C27" s="43"/>
-      <c r="D27" s="6"/>
-      <c r="E27" s="6"/>
-      <c r="F27" s="50"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="17"/>
       <c r="G27" s="18"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="31">
-        <v>80000</v>
-      </c>
-      <c r="G28" s="1"/>
+      <c r="B28" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="42"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="17"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="11"/>
-      <c r="C29" s="35" t="s">
-        <v>37</v>
+      <c r="C29" s="34" t="s">
+        <v>33</v>
       </c>
       <c r="E29" s="3"/>
-      <c r="F29" s="31">
-        <v>0</v>
+      <c r="F29" s="30">
+        <v>60000</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -4200,12 +3895,12 @@
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="11"/>
-      <c r="C30" s="35" t="s">
-        <v>35</v>
+      <c r="C30" s="34" t="s">
+        <v>37</v>
       </c>
       <c r="E30" s="3"/>
-      <c r="F30" s="31">
-        <v>30000</v>
+      <c r="F30" s="30">
+        <v>0</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -4213,12 +3908,12 @@
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="11"/>
-      <c r="C31" s="35" t="s">
-        <v>34</v>
+      <c r="C31" s="34" t="s">
+        <v>35</v>
       </c>
       <c r="E31" s="3"/>
-      <c r="F31" s="31">
-        <v>2400</v>
+      <c r="F31" s="30">
+        <v>30000</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -4226,12 +3921,12 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="11"/>
-      <c r="C32" s="35" t="s">
-        <v>38</v>
+      <c r="C32" s="34" t="s">
+        <v>34</v>
       </c>
       <c r="E32" s="3"/>
-      <c r="F32" s="31">
-        <v>10000</v>
+      <c r="F32" s="30">
+        <v>2400</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -4239,12 +3934,12 @@
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="11"/>
-      <c r="C33" s="53" t="s">
-        <v>39</v>
+      <c r="C33" s="34" t="s">
+        <v>38</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="31">
-        <v>5000</v>
+      <c r="F33" s="30">
+        <v>10000</v>
       </c>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
@@ -4252,36 +3947,36 @@
     <row r="34" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="11"/>
-      <c r="C34" s="11" t="s">
-        <v>6</v>
+      <c r="C34" s="52" t="s">
+        <v>39</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="31"/>
+      <c r="F34" s="30">
+        <v>5000</v>
+      </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="53" t="s">
-        <v>28</v>
+      <c r="C35" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="E35" s="3"/>
-      <c r="F35" s="46">
-        <v>5000</v>
-      </c>
+      <c r="F35" s="30"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="11"/>
-      <c r="C36" s="53" t="s">
-        <v>40</v>
+      <c r="C36" s="52" t="s">
+        <v>28</v>
       </c>
       <c r="E36" s="3"/>
-      <c r="F36" s="49">
-        <v>15000</v>
+      <c r="F36" s="45">
+        <v>20000</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
@@ -4289,519 +3984,532 @@
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" s="4"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="11" t="s">
-        <v>7</v>
+      <c r="C37" s="52" t="s">
+        <v>40</v>
       </c>
       <c r="E37" s="3"/>
-      <c r="F37" s="30">
-        <v>2500</v>
+      <c r="F37" s="48">
+        <v>15000</v>
       </c>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" s="4"/>
       <c r="B38" s="11"/>
-      <c r="C38" s="34" t="s">
+      <c r="C38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="E38" s="3"/>
+      <c r="F38" s="29">
+        <v>2500</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="18"/>
-      <c r="G38" s="47">
+      <c r="E39" s="3"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="46">
         <f>IF(SUM(Fixed_costs)&lt;&gt;0,SUM(Fixed_costs),0)</f>
-        <v>149900</v>
-      </c>
-      <c r="H38" s="1"/>
-    </row>
-    <row r="39" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="35"/>
-      <c r="C39" s="35"/>
-      <c r="F39" s="18"/>
-      <c r="G39" s="20"/>
+        <v>144900</v>
+      </c>
       <c r="H39" s="1"/>
     </row>
     <row r="40" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="4"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="34" t="s">
+      <c r="B40" s="34"/>
+      <c r="C40" s="34"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="19"/>
+      <c r="H40" s="1"/>
+    </row>
+    <row r="41" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="G40" s="48">
+      <c r="E41" s="3"/>
+      <c r="G41" s="47">
         <f>IF(OR(Gross_margin&lt;&gt;0,Total_fixed&lt;&gt;0),Gross_margin-Total_fixed,0)</f>
-        <v>370200</v>
-      </c>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B41" s="35"/>
-      <c r="C41" s="35"/>
-      <c r="G41" s="20"/>
-    </row>
-    <row r="42" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
-      <c r="B42" s="35"/>
-      <c r="C42" s="35"/>
-      <c r="F42" s="24"/>
+        <v>177250</v>
+      </c>
+      <c r="H41" s="1"/>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B42" s="34"/>
+      <c r="C42" s="34"/>
+      <c r="G42" s="19"/>
     </row>
     <row r="43" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
-      <c r="B43" s="24" t="s">
+      <c r="B43" s="34"/>
+      <c r="C43" s="34"/>
+      <c r="F43" s="23"/>
+    </row>
+    <row r="44" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
+      <c r="B44" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="24"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="1"/>
-    </row>
-    <row r="44" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B44" s="40" t="s">
+      <c r="C44" s="23"/>
+      <c r="D44" s="23"/>
+      <c r="E44" s="23"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+    </row>
+    <row r="45" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B45" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C44" s="40"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="39">
+      <c r="C45" s="39"/>
+      <c r="D45" s="25"/>
+      <c r="E45" s="25"/>
+      <c r="F45" s="38">
         <f>IF(AND(Unit_contrib_margin&gt;0,Total_fixed&gt;0),Total_fixed/Unit_contrib_margin,"")</f>
-        <v>46.123076923076923</v>
-      </c>
-      <c r="G44" s="25"/>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="27"/>
-    </row>
-    <row r="45" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B45" s="40" t="s">
+        <v>56.823529411764703</v>
+      </c>
+      <c r="G45" s="24"/>
+      <c r="H45" s="25"/>
+      <c r="I45" s="25"/>
+      <c r="J45" s="26"/>
+    </row>
+    <row r="46" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B46" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="40"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="26"/>
-      <c r="I45" s="26"/>
-      <c r="J45" s="27"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B46" s="35" t="s">
+      <c r="C46" s="39"/>
+      <c r="D46" s="25"/>
+      <c r="E46" s="25"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="24"/>
+      <c r="H46" s="25"/>
+      <c r="I46" s="25"/>
+      <c r="J46" s="26"/>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B47" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="C46" s="35"/>
-      <c r="D46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0,0)</f>
+      <c r="C47" s="34"/>
+      <c r="D47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0,0)</f>
         <v>0</v>
       </c>
-      <c r="E46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.1,0)</f>
-        <v>2</v>
-      </c>
-      <c r="F46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.2,0)</f>
-        <v>4</v>
-      </c>
-      <c r="G46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.3,0)</f>
-        <v>6</v>
-      </c>
-      <c r="H46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.4,0)</f>
+      <c r="E47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.1,0)</f>
+        <v>4.5</v>
+      </c>
+      <c r="F47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.2,0)</f>
+        <v>9</v>
+      </c>
+      <c r="G47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.3,0)</f>
+        <v>13.5</v>
+      </c>
+      <c r="H47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.4,0)</f>
+        <v>18</v>
+      </c>
+      <c r="I47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.5,0)</f>
+        <v>22.5</v>
+      </c>
+      <c r="J47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.6,0)</f>
+        <v>27</v>
+      </c>
+      <c r="K47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.7,0)</f>
+        <v>31.499999999999996</v>
+      </c>
+      <c r="L47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.8,0)</f>
+        <v>36</v>
+      </c>
+      <c r="M47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.9,0)</f>
+        <v>40.5</v>
+      </c>
+      <c r="N47" s="35">
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*1,0)</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B48" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="I46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.5,0)</f>
-        <v>10</v>
-      </c>
-      <c r="J46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.6,0)</f>
+      <c r="C48" s="34"/>
+      <c r="D48" s="36">
+        <f>Sales_price_unitA+Sales_price_unitB+Sales_price_unitC</f>
+        <v>42840</v>
+      </c>
+      <c r="E48" s="36">
+        <f t="shared" ref="D48:N48" si="0">Sales_price_unitA</f>
+        <v>3400</v>
+      </c>
+      <c r="F48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="G48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="H48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="I48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="J48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="K48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="L48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="M48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+      <c r="N48" s="36">
+        <f t="shared" si="0"/>
+        <v>3400</v>
+      </c>
+    </row>
+    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B49" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="34"/>
+      <c r="D49" s="36">
+        <f t="shared" ref="D49:N49" si="1">Total_Subscription*D47</f>
+        <v>0</v>
+      </c>
+      <c r="E49" s="36">
+        <f t="shared" si="1"/>
+        <v>2250</v>
+      </c>
+      <c r="F49" s="36">
+        <f t="shared" si="1"/>
+        <v>4500</v>
+      </c>
+      <c r="G49" s="36">
+        <f t="shared" si="1"/>
+        <v>6750</v>
+      </c>
+      <c r="H49" s="36">
+        <f t="shared" si="1"/>
+        <v>9000</v>
+      </c>
+      <c r="I49" s="36">
+        <f t="shared" si="1"/>
+        <v>11250</v>
+      </c>
+      <c r="J49" s="36">
+        <f t="shared" si="1"/>
+        <v>13500</v>
+      </c>
+      <c r="K49" s="36">
+        <f t="shared" si="1"/>
+        <v>15749.999999999998</v>
+      </c>
+      <c r="L49" s="36">
+        <f t="shared" si="1"/>
+        <v>18000</v>
+      </c>
+      <c r="M49" s="36">
+        <f t="shared" si="1"/>
+        <v>20250</v>
+      </c>
+      <c r="N49" s="36">
+        <f t="shared" si="1"/>
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B50" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="34"/>
+      <c r="D50" s="36">
+        <f t="shared" ref="D50:N50" si="2">Total_fixed</f>
+        <v>144900</v>
+      </c>
+      <c r="E50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="F50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="G50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="H50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="I50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="J50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="K50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="L50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="M50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+      <c r="N50" s="36">
+        <f t="shared" si="2"/>
+        <v>144900</v>
+      </c>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B51" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="K46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.7,0)</f>
-        <v>14</v>
-      </c>
-      <c r="L46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.8,0)</f>
-        <v>16</v>
-      </c>
-      <c r="M46" s="36">
-        <f>IF(Sales_volume_unitsA,Sales_volume_unitsA*0.9,0)</f>
-        <v>18</v>
-      </c>
-      <c r="N46" s="36">
-        <f>Sales_volume_unitsA</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B47" s="35" t="s">
-        <v>8</v>
-      </c>
-      <c r="C47" s="35"/>
-      <c r="D47" s="37">
-        <f t="shared" ref="D47:N47" si="0">Sales_price_unitA</f>
-        <v>4100</v>
-      </c>
-      <c r="E47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="F47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="G47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="H47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="I47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="J47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="K47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="L47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="M47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-      <c r="N47" s="37">
-        <f t="shared" si="0"/>
-        <v>4100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B48" s="35" t="s">
-        <v>48</v>
-      </c>
-      <c r="C48" s="35"/>
-      <c r="D48" s="37">
-        <f t="shared" ref="D48:N48" si="1">Total_Subscription*D46</f>
+      <c r="C51" s="37"/>
+      <c r="D51" s="36">
+        <f t="shared" ref="D51:N51" si="3">Variable_Unit_Cost*D47</f>
         <v>0</v>
       </c>
-      <c r="E48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="K48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="L48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="M48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N48" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B49" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="C49" s="35"/>
-      <c r="D49" s="37">
-        <f t="shared" ref="D49:N49" si="2">Total_fixed</f>
-        <v>149900</v>
-      </c>
-      <c r="E49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="F49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="G49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="H49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="I49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="J49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="K49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="L49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="M49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-      <c r="N49" s="37">
-        <f t="shared" si="2"/>
-        <v>149900</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B50" s="38" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="38"/>
-      <c r="D50" s="37">
-        <f t="shared" ref="D50:N50" si="3">Variable_Unit_Cost*D46</f>
-        <v>0</v>
-      </c>
-      <c r="E50" s="37">
+      <c r="E51" s="36">
         <f t="shared" si="3"/>
-        <v>1700</v>
-      </c>
-      <c r="F50" s="37">
+        <v>3825</v>
+      </c>
+      <c r="F51" s="36">
         <f t="shared" si="3"/>
-        <v>3400</v>
-      </c>
-      <c r="G50" s="37">
+        <v>7650</v>
+      </c>
+      <c r="G51" s="36">
         <f t="shared" si="3"/>
-        <v>5100</v>
-      </c>
-      <c r="H50" s="37">
-        <f t="shared" si="3"/>
-        <v>6800</v>
-      </c>
-      <c r="I50" s="37">
-        <f t="shared" si="3"/>
-        <v>8500</v>
-      </c>
-      <c r="J50" s="37">
-        <f t="shared" si="3"/>
-        <v>10200</v>
-      </c>
-      <c r="K50" s="37">
-        <f t="shared" si="3"/>
-        <v>11900</v>
-      </c>
-      <c r="L50" s="37">
-        <f t="shared" si="3"/>
-        <v>13600</v>
-      </c>
-      <c r="M50" s="37">
+        <v>11475</v>
+      </c>
+      <c r="H51" s="36">
         <f t="shared" si="3"/>
         <v>15300</v>
       </c>
-      <c r="N50" s="37">
+      <c r="I51" s="36">
         <f t="shared" si="3"/>
-        <v>17000</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B51" s="38" t="s">
+        <v>19125</v>
+      </c>
+      <c r="J51" s="36">
+        <f t="shared" si="3"/>
+        <v>22950</v>
+      </c>
+      <c r="K51" s="36">
+        <f t="shared" si="3"/>
+        <v>26774.999999999996</v>
+      </c>
+      <c r="L51" s="36">
+        <f t="shared" si="3"/>
+        <v>30600</v>
+      </c>
+      <c r="M51" s="36">
+        <f t="shared" si="3"/>
+        <v>34425</v>
+      </c>
+      <c r="N51" s="36">
+        <f t="shared" si="3"/>
+        <v>38250</v>
+      </c>
+    </row>
+    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B52" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C51" s="38"/>
-      <c r="D51" s="37">
-        <f t="shared" ref="D51:N51" si="4">SUM(D49:D50)</f>
-        <v>149900</v>
-      </c>
-      <c r="E51" s="37">
+      <c r="C52" s="37"/>
+      <c r="D52" s="36">
+        <f t="shared" ref="D52:N52" si="4">SUM(D50:D51)</f>
+        <v>144900</v>
+      </c>
+      <c r="E52" s="36">
         <f t="shared" si="4"/>
-        <v>151600</v>
-      </c>
-      <c r="F51" s="37">
+        <v>148725</v>
+      </c>
+      <c r="F52" s="36">
         <f t="shared" si="4"/>
-        <v>153300</v>
-      </c>
-      <c r="G51" s="37">
+        <v>152550</v>
+      </c>
+      <c r="G52" s="36">
         <f t="shared" si="4"/>
-        <v>155000</v>
-      </c>
-      <c r="H51" s="37">
+        <v>156375</v>
+      </c>
+      <c r="H52" s="36">
         <f t="shared" si="4"/>
-        <v>156700</v>
-      </c>
-      <c r="I51" s="37">
+        <v>160200</v>
+      </c>
+      <c r="I52" s="36">
         <f t="shared" si="4"/>
-        <v>158400</v>
-      </c>
-      <c r="J51" s="37">
+        <v>164025</v>
+      </c>
+      <c r="J52" s="36">
         <f t="shared" si="4"/>
-        <v>160100</v>
-      </c>
-      <c r="K51" s="37">
+        <v>167850</v>
+      </c>
+      <c r="K52" s="36">
         <f t="shared" si="4"/>
-        <v>161800</v>
-      </c>
-      <c r="L51" s="37">
+        <v>171675</v>
+      </c>
+      <c r="L52" s="36">
         <f t="shared" si="4"/>
-        <v>163500</v>
-      </c>
-      <c r="M51" s="37">
+        <v>175500</v>
+      </c>
+      <c r="M52" s="36">
         <f t="shared" si="4"/>
-        <v>165200</v>
-      </c>
-      <c r="N51" s="37">
+        <v>179325</v>
+      </c>
+      <c r="N52" s="36">
         <f t="shared" si="4"/>
-        <v>166900</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="35" t="s">
+        <v>183150</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C52" s="35"/>
-      <c r="D52" s="51">
-        <f>(D47*D46)+D48</f>
+      <c r="C53" s="34"/>
+      <c r="D53" s="50">
+        <f>(D48*D47)+D49</f>
         <v>0</v>
       </c>
-      <c r="E52" s="51">
-        <f t="shared" ref="E52:N52" si="5">(E47*E46)+E48</f>
-        <v>8200</v>
-      </c>
-      <c r="F52" s="51">
+      <c r="E53" s="50">
+        <f t="shared" ref="E53:N53" si="5">(E48*E47)+E49</f>
+        <v>17550</v>
+      </c>
+      <c r="F53" s="50">
         <f t="shared" si="5"/>
-        <v>16400</v>
-      </c>
-      <c r="G52" s="51">
+        <v>35100</v>
+      </c>
+      <c r="G53" s="50">
         <f t="shared" si="5"/>
-        <v>24600</v>
-      </c>
-      <c r="H52" s="51">
+        <v>52650</v>
+      </c>
+      <c r="H53" s="50">
         <f t="shared" si="5"/>
-        <v>32800</v>
-      </c>
-      <c r="I52" s="51">
+        <v>70200</v>
+      </c>
+      <c r="I53" s="50">
         <f t="shared" si="5"/>
-        <v>41000</v>
-      </c>
-      <c r="J52" s="51">
+        <v>87750</v>
+      </c>
+      <c r="J53" s="50">
         <f t="shared" si="5"/>
-        <v>49200</v>
-      </c>
-      <c r="K52" s="51">
+        <v>105300</v>
+      </c>
+      <c r="K53" s="50">
         <f t="shared" si="5"/>
-        <v>57400</v>
-      </c>
-      <c r="L52" s="51">
+        <v>122849.99999999999</v>
+      </c>
+      <c r="L53" s="50">
         <f t="shared" si="5"/>
-        <v>65600</v>
-      </c>
-      <c r="M52" s="51">
+        <v>140400</v>
+      </c>
+      <c r="M53" s="50">
         <f t="shared" si="5"/>
-        <v>73800</v>
-      </c>
-      <c r="N52" s="51">
+        <v>157950</v>
+      </c>
+      <c r="N53" s="50">
         <f t="shared" si="5"/>
-        <v>82000</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B53" s="38" t="s">
+        <v>175500</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B54" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="C53" s="38"/>
-      <c r="D53" s="52">
-        <f>D52-D51</f>
-        <v>-149900</v>
-      </c>
-      <c r="E53" s="52">
-        <f t="shared" ref="E53:N53" si="6">E52-E51</f>
-        <v>-143400</v>
-      </c>
-      <c r="F53" s="52">
+      <c r="C54" s="37"/>
+      <c r="D54" s="51">
+        <f>D53-D52</f>
+        <v>-144900</v>
+      </c>
+      <c r="E54" s="51">
+        <f t="shared" ref="E54:N54" si="6">E53-E52</f>
+        <v>-131175</v>
+      </c>
+      <c r="F54" s="51">
         <f t="shared" si="6"/>
-        <v>-136900</v>
-      </c>
-      <c r="G53" s="52">
+        <v>-117450</v>
+      </c>
+      <c r="G54" s="51">
         <f t="shared" si="6"/>
-        <v>-130400</v>
-      </c>
-      <c r="H53" s="52">
+        <v>-103725</v>
+      </c>
+      <c r="H54" s="51">
         <f t="shared" si="6"/>
-        <v>-123900</v>
-      </c>
-      <c r="I53" s="52">
+        <v>-90000</v>
+      </c>
+      <c r="I54" s="51">
         <f t="shared" si="6"/>
-        <v>-117400</v>
-      </c>
-      <c r="J53" s="52">
+        <v>-76275</v>
+      </c>
+      <c r="J54" s="51">
         <f t="shared" si="6"/>
-        <v>-110900</v>
-      </c>
-      <c r="K53" s="52">
+        <v>-62550</v>
+      </c>
+      <c r="K54" s="51">
         <f t="shared" si="6"/>
-        <v>-104400</v>
-      </c>
-      <c r="L53" s="52">
+        <v>-48825.000000000015</v>
+      </c>
+      <c r="L54" s="51">
         <f t="shared" si="6"/>
-        <v>-97900</v>
-      </c>
-      <c r="M53" s="52">
+        <v>-35100</v>
+      </c>
+      <c r="M54" s="51">
         <f t="shared" si="6"/>
-        <v>-91400</v>
-      </c>
-      <c r="N53" s="52">
+        <v>-21375</v>
+      </c>
+      <c r="N54" s="51">
         <f t="shared" si="6"/>
-        <v>-84900</v>
+        <v>-7650</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0" sort="0"/>
   <scenarios current="0" show="0" sqref="H30">
     <scenario name="Lower price" count="2" user="Sally Herigstad" comment="Created by SH on 2/18/2004">
-      <inputCells r="F5" val="4" numFmtId="37"/>
-      <inputCells r="F6" val="600" numFmtId="37"/>
+      <inputCells r="F6" val="4" numFmtId="37"/>
+      <inputCells r="F7" val="600" numFmtId="37"/>
     </scenario>
     <scenario name="Higher price" count="2" user="Sally Herigstad" comment="Created by SH on 2/18/2004">
-      <inputCells r="F5" val="6" numFmtId="37"/>
-      <inputCells r="F6" val="450" numFmtId="37"/>
+      <inputCells r="F6" val="6" numFmtId="37"/>
+      <inputCells r="F7" val="450" numFmtId="37"/>
     </scenario>
   </scenarios>
   <phoneticPr fontId="0" type="noConversion"/>
-  <dataValidations disablePrompts="1" count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F45 F26:F27 F56:F65548 G10:G20 G2 G39 F38 G41 F40 D50:N50 H57:H65548 J44:J45 G27 F10:F12" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <dataValidations count="3">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F46 F27:F28 F57:F65549 G2 G40 F39 G42 F41 D51:N51 H58:H65549 J45:J46 G28 F11:F13 G11:G21" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>-10000000</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F44 G22:G26 G8 H2 F21:F25 G57:G65548 G38 F39 G40" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between (10,000,000) and 10,000,000." sqref="F13:F20 F28:F37 F10:F11" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F45 G23:G27 G9 H2 F22:F26 G58:G65549 G39 F40 G41" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between (10,000,000) and 10,000,000." sqref="F14:F21 F29:F38 F11:F12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>-10000000</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
@@ -4822,14 +4530,14 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>3</xdr:row>
+                    <xdr:row>4</xdr:row>
                     <xdr:rowOff>190500</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>790575</xdr:colOff>
-                    <xdr:row>4</xdr:row>
-                    <xdr:rowOff>142875</xdr:rowOff>
+                    <xdr:row>6</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -4844,13 +4552,13 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>4</xdr:row>
+                    <xdr:row>5</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>790575</xdr:colOff>
-                    <xdr:row>5</xdr:row>
+                    <xdr:row>6</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4866,13 +4574,13 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>18</xdr:row>
+                    <xdr:row>19</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>838200</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>20</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4888,13 +4596,13 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>16</xdr:row>
+                    <xdr:row>17</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>828675</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>18</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4910,13 +4618,13 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>790575</xdr:colOff>
-                    <xdr:row>9</xdr:row>
+                    <xdr:row>10</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4932,13 +4640,13 @@
                   <from>
                     <xdr:col>8</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>4</xdr:row>
+                    <xdr:row>5</xdr:row>
                     <xdr:rowOff>152400</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>8</xdr:col>
                     <xdr:colOff>809625</xdr:colOff>
-                    <xdr:row>6</xdr:row>
+                    <xdr:row>7</xdr:row>
                     <xdr:rowOff>28575</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4954,13 +4662,13 @@
                   <from>
                     <xdr:col>10</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>5</xdr:row>
+                    <xdr:row>6</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>10</xdr:col>
                     <xdr:colOff>790575</xdr:colOff>
-                    <xdr:row>6</xdr:row>
+                    <xdr:row>7</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>

<commit_message>
deleted old breakeven file
</commit_message>
<xml_diff>
--- a/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
+++ b/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Breakeven Analysis Data" sheetId="2" r:id="rId1"/>
@@ -810,16 +810,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color auto="1"/>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
+      <right style="thin">
+        <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -970,13 +970,13 @@
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="38" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1240,7 +1240,7 @@
                   <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2550</c:v>
+                  <c:v>2350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1835,7 +1835,7 @@
                   <c:v>850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2550</c:v>
+                  <c:v>2350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2142,34 +2142,34 @@
                   <c:v>144900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>148725</c:v>
+                  <c:v>146811.73499999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>152550</c:v>
+                  <c:v>149490</c:v>
                 </c:pt>
                 <c:pt idx="3">
+                  <c:v>151785</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>154080</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>156375</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>160200</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>164025</c:v>
-                </c:pt>
                 <c:pt idx="6">
+                  <c:v>158670</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>160965</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>163260</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>165555</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>167850</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>171675</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>175500</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>179325</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>183150</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2228,34 +2228,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17550</c:v>
+                  <c:v>7197.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>35100</c:v>
+                  <c:v>17280</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>52650</c:v>
+                  <c:v>25920</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70200</c:v>
+                  <c:v>34560</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>87750</c:v>
+                  <c:v>43200</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>105300</c:v>
+                  <c:v>51840</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>122849.99999999999</c:v>
+                  <c:v>60479.999999999993</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>140400</c:v>
+                  <c:v>69120</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>157950</c:v>
+                  <c:v>77760</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>175500</c:v>
+                  <c:v>86400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2312,34 +2312,34 @@
                   <c:v>-144900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-131175</c:v>
+                  <c:v>-139614.61499999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-117450</c:v>
+                  <c:v>-132210</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-103725</c:v>
+                  <c:v>-125865</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-90000</c:v>
+                  <c:v>-119520</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-76275</c:v>
+                  <c:v>-113175</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-62550</c:v>
+                  <c:v>-106830</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-48825.000000000015</c:v>
+                  <c:v>-100485</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-35100</c:v>
+                  <c:v>-94140</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-21375</c:v>
+                  <c:v>-87795</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-7650</c:v>
+                  <c:v>-81450</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2641,11 +2641,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" inc="100" max="10000" min="500" page="10" val="3400"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" inc="100" max="10000" min="500" page="10" val="3200"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$7" horiz="1" max="50" min="1" page="10" val="30"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$7" horiz="1" max="50" min="1" page="10" val="20"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2657,15 +2657,15 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$11" horiz="1" inc="100" max="10000" page="0" val="500"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$11" horiz="1" inc="100" max="10000" page="0" val="0"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$7" horiz="1" max="50" min="1" page="10" val="10"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$7" horiz="1" max="50" min="1" page="10" val="5"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$J$7" horiz="1" max="50" min="1" page="10" val="5"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$J$7" horiz="1" max="50" min="1" page="10" val="2"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2856,8 +2856,8 @@
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>838200</xdr:colOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>19050</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
@@ -2906,8 +2906,8 @@
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>828675</xdr:colOff>
+          <xdr:col>7</xdr:col>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
@@ -3498,8 +3498,8 @@
   </sheetPr>
   <dimension ref="A1:N54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B19" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3510,10 +3510,14 @@
     <col min="4" max="4" width="17.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="19" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="19" customWidth="1"/>
-    <col min="9" max="14" width="12.7109375" style="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="7" max="7" width="12.28515625" style="10" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="14" width="12.7109375" style="1" customWidth="1"/>
+    <col min="15" max="16" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.140625" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.65">
@@ -3563,11 +3567,11 @@
       <c r="G4" s="65" t="s">
         <v>50</v>
       </c>
-      <c r="H4" s="67">
+      <c r="H4" s="66">
         <v>0.1</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="67">
+      <c r="J4" s="66">
         <v>0.2</v>
       </c>
       <c r="K4" s="14"/>
@@ -3583,7 +3587,7 @@
         <v>50</v>
       </c>
       <c r="G5" s="59"/>
-      <c r="H5" s="66">
+      <c r="H5" s="67">
         <v>200</v>
       </c>
       <c r="I5" s="63"/>
@@ -3599,16 +3603,16 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="61">
-        <v>3400</v>
+        <v>3200</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="61">
         <f>Sales_price_unitA*(H5/F5)*(1-H4)</f>
-        <v>12240</v>
+        <v>11520</v>
       </c>
       <c r="J6" s="61">
         <f>Sales_price_unitA*(J5/F5)*(1-J4)</f>
-        <v>27200</v>
+        <v>25600</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -3619,14 +3623,14 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="43">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="43">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J7" s="43">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -3634,16 +3638,16 @@
       <c r="C8" s="12"/>
       <c r="F8" s="64">
         <f>IF(OR(Sales_price_unitA&lt;&gt;0,Sales_volume_unitsA&lt;&gt;0),Sales_price_unitA*Sales_volume_unitsA,0)</f>
-        <v>102000</v>
+        <v>64000</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="64">
         <f>IF(OR(Sales_price_unitB&lt;&gt;0,Sales_volume_unitsB&lt;&gt;0),Sales_price_unitB*Sales_volume_unitsB,0)</f>
-        <v>122400</v>
+        <v>57600</v>
       </c>
       <c r="J8" s="64">
         <f>IF(OR(Sales_price_unitC&lt;&gt;0,Sales_volume_unitsC&lt;&gt;0),Sales_price_unitC*Sales_volume_unitsC,0)</f>
-        <v>136000</v>
+        <v>51200</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -3653,7 +3657,7 @@
       </c>
       <c r="G9" s="62">
         <f>F8+H8+J8</f>
-        <v>360400</v>
+        <v>172800</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3672,7 +3676,7 @@
       </c>
       <c r="E11" s="4"/>
       <c r="F11" s="43">
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="G11" s="17"/>
     </row>
@@ -3686,7 +3690,7 @@
       <c r="F12" s="56"/>
       <c r="G12" s="58">
         <f>F11</f>
-        <v>500</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3817,7 +3821,7 @@
       <c r="F23" s="18"/>
       <c r="G23" s="44">
         <f>IF(Variable_Unit_Cost,Variable_Unit_Cost*(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC),0)</f>
-        <v>38250</v>
+        <v>22950</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -3838,7 +3842,7 @@
       <c r="E25" s="3"/>
       <c r="F25" s="31">
         <f>IF(Sales_price_unitA&gt;0,MAX(0,Sales_price_unitA-Variable_Unit_Cost),0)</f>
-        <v>2550</v>
+        <v>2350</v>
       </c>
       <c r="G25" s="18"/>
       <c r="H25" s="1"/>
@@ -3853,7 +3857,7 @@
       <c r="F26" s="18"/>
       <c r="G26" s="31">
         <f>IF(OR(Total_Sales&lt;&gt;0,Total_variable&lt;&gt;0),Total_Sales-Total_variable,0)</f>
-        <v>322150</v>
+        <v>149850</v>
       </c>
       <c r="H26" s="1"/>
     </row>
@@ -4037,7 +4041,7 @@
       <c r="E41" s="3"/>
       <c r="G41" s="47">
         <f>IF(OR(Gross_margin&lt;&gt;0,Total_fixed&lt;&gt;0),Gross_margin-Total_fixed,0)</f>
-        <v>177250</v>
+        <v>4950</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -4070,7 +4074,7 @@
       <c r="E45" s="25"/>
       <c r="F45" s="38">
         <f>IF(AND(Unit_contrib_margin&gt;0,Total_fixed&gt;0),Total_fixed/Unit_contrib_margin,"")</f>
-        <v>56.823529411764703</v>
+        <v>61.659574468085104</v>
       </c>
       <c r="G45" s="24"/>
       <c r="H45" s="25"/>
@@ -4100,44 +4104,44 @@
         <v>0</v>
       </c>
       <c r="E47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.1,0)</f>
-        <v>4.5</v>
+        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.0833,0)</f>
+        <v>2.2490999999999999</v>
       </c>
       <c r="F47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.2,0)</f>
-        <v>9</v>
+        <v>5.4</v>
       </c>
       <c r="G47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.3,0)</f>
-        <v>13.5</v>
+        <v>8.1</v>
       </c>
       <c r="H47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.4,0)</f>
-        <v>18</v>
+        <v>10.8</v>
       </c>
       <c r="I47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.5,0)</f>
-        <v>22.5</v>
+        <v>13.5</v>
       </c>
       <c r="J47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.6,0)</f>
-        <v>27</v>
+        <v>16.2</v>
       </c>
       <c r="K47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.7,0)</f>
-        <v>31.499999999999996</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="L47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.8,0)</f>
-        <v>36</v>
+        <v>21.6</v>
       </c>
       <c r="M47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.9,0)</f>
-        <v>40.5</v>
+        <v>24.3</v>
       </c>
       <c r="N47" s="35">
         <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*1,0)</f>
-        <v>45</v>
+        <v>27</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -4146,48 +4150,48 @@
       </c>
       <c r="C48" s="34"/>
       <c r="D48" s="36">
-        <f>Sales_price_unitA+Sales_price_unitB+Sales_price_unitC</f>
-        <v>42840</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="E48" s="36">
-        <f t="shared" ref="D48:N48" si="0">Sales_price_unitA</f>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="F48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="G48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="H48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="I48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="J48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="K48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="L48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="M48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
       <c r="N48" s="36">
-        <f t="shared" si="0"/>
-        <v>3400</v>
+        <f>(Sales_price_unitA)</f>
+        <v>3200</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.2">
@@ -4196,48 +4200,48 @@
       </c>
       <c r="C49" s="34"/>
       <c r="D49" s="36">
-        <f t="shared" ref="D49:N49" si="1">Total_Subscription*D47</f>
+        <f>Total_Subscription*D47</f>
         <v>0</v>
       </c>
       <c r="E49" s="36">
-        <f t="shared" si="1"/>
-        <v>2250</v>
+        <f>Total_Subscription*E47</f>
+        <v>0</v>
       </c>
       <c r="F49" s="36">
-        <f t="shared" si="1"/>
-        <v>4500</v>
+        <f>Total_Subscription*F47</f>
+        <v>0</v>
       </c>
       <c r="G49" s="36">
-        <f t="shared" si="1"/>
-        <v>6750</v>
+        <f>Total_Subscription*G47</f>
+        <v>0</v>
       </c>
       <c r="H49" s="36">
-        <f t="shared" si="1"/>
-        <v>9000</v>
+        <f>Total_Subscription*H47</f>
+        <v>0</v>
       </c>
       <c r="I49" s="36">
-        <f t="shared" si="1"/>
-        <v>11250</v>
+        <f>Total_Subscription*I47</f>
+        <v>0</v>
       </c>
       <c r="J49" s="36">
-        <f t="shared" si="1"/>
-        <v>13500</v>
+        <f>Total_Subscription*J47</f>
+        <v>0</v>
       </c>
       <c r="K49" s="36">
-        <f t="shared" si="1"/>
-        <v>15749.999999999998</v>
+        <f>Total_Subscription*K47</f>
+        <v>0</v>
       </c>
       <c r="L49" s="36">
-        <f t="shared" si="1"/>
-        <v>18000</v>
+        <f>Total_Subscription*L47</f>
+        <v>0</v>
       </c>
       <c r="M49" s="36">
-        <f t="shared" si="1"/>
-        <v>20250</v>
+        <f>Total_Subscription*M47</f>
+        <v>0</v>
       </c>
       <c r="N49" s="36">
-        <f t="shared" si="1"/>
-        <v>22500</v>
+        <f>Total_Subscription*N47</f>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
@@ -4246,47 +4250,47 @@
       </c>
       <c r="C50" s="34"/>
       <c r="D50" s="36">
-        <f t="shared" ref="D50:N50" si="2">Total_fixed</f>
+        <f t="shared" ref="D50:N50" si="0">Total_fixed</f>
         <v>144900</v>
       </c>
       <c r="E50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="F50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="G50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="H50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="I50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="J50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="K50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="L50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="M50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
       <c r="N50" s="36">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>144900</v>
       </c>
     </row>
@@ -4296,48 +4300,48 @@
       </c>
       <c r="C51" s="37"/>
       <c r="D51" s="36">
-        <f t="shared" ref="D51:N51" si="3">Variable_Unit_Cost*D47</f>
+        <f>Variable_Unit_Cost*D47</f>
         <v>0</v>
       </c>
       <c r="E51" s="36">
-        <f t="shared" si="3"/>
-        <v>3825</v>
+        <f>Variable_Unit_Cost*E47</f>
+        <v>1911.7349999999999</v>
       </c>
       <c r="F51" s="36">
-        <f t="shared" si="3"/>
-        <v>7650</v>
+        <f>Variable_Unit_Cost*F47</f>
+        <v>4590</v>
       </c>
       <c r="G51" s="36">
-        <f t="shared" si="3"/>
+        <f>Variable_Unit_Cost*G47</f>
+        <v>6885</v>
+      </c>
+      <c r="H51" s="36">
+        <f>Variable_Unit_Cost*H47</f>
+        <v>9180</v>
+      </c>
+      <c r="I51" s="36">
+        <f>Variable_Unit_Cost*I47</f>
         <v>11475</v>
       </c>
-      <c r="H51" s="36">
-        <f t="shared" si="3"/>
-        <v>15300</v>
-      </c>
-      <c r="I51" s="36">
-        <f t="shared" si="3"/>
-        <v>19125</v>
-      </c>
       <c r="J51" s="36">
-        <f t="shared" si="3"/>
+        <f>Variable_Unit_Cost*J47</f>
+        <v>13770</v>
+      </c>
+      <c r="K51" s="36">
+        <f>Variable_Unit_Cost*K47</f>
+        <v>16064.999999999998</v>
+      </c>
+      <c r="L51" s="36">
+        <f>Variable_Unit_Cost*L47</f>
+        <v>18360</v>
+      </c>
+      <c r="M51" s="36">
+        <f>Variable_Unit_Cost*M47</f>
+        <v>20655</v>
+      </c>
+      <c r="N51" s="36">
+        <f>Variable_Unit_Cost*N47</f>
         <v>22950</v>
-      </c>
-      <c r="K51" s="36">
-        <f t="shared" si="3"/>
-        <v>26774.999999999996</v>
-      </c>
-      <c r="L51" s="36">
-        <f t="shared" si="3"/>
-        <v>30600</v>
-      </c>
-      <c r="M51" s="36">
-        <f t="shared" si="3"/>
-        <v>34425</v>
-      </c>
-      <c r="N51" s="36">
-        <f t="shared" si="3"/>
-        <v>38250</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
@@ -4346,48 +4350,48 @@
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="36">
-        <f t="shared" ref="D52:N52" si="4">SUM(D50:D51)</f>
+        <f t="shared" ref="D52:N52" si="1">SUM(D50:D51)</f>
         <v>144900</v>
       </c>
       <c r="E52" s="36">
-        <f t="shared" si="4"/>
-        <v>148725</v>
+        <f t="shared" si="1"/>
+        <v>146811.73499999999</v>
       </c>
       <c r="F52" s="36">
-        <f t="shared" si="4"/>
-        <v>152550</v>
+        <f t="shared" si="1"/>
+        <v>149490</v>
       </c>
       <c r="G52" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
+        <v>151785</v>
+      </c>
+      <c r="H52" s="36">
+        <f t="shared" si="1"/>
+        <v>154080</v>
+      </c>
+      <c r="I52" s="36">
+        <f t="shared" si="1"/>
         <v>156375</v>
       </c>
-      <c r="H52" s="36">
-        <f t="shared" si="4"/>
-        <v>160200</v>
-      </c>
-      <c r="I52" s="36">
-        <f t="shared" si="4"/>
-        <v>164025</v>
-      </c>
       <c r="J52" s="36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
+        <v>158670</v>
+      </c>
+      <c r="K52" s="36">
+        <f t="shared" si="1"/>
+        <v>160965</v>
+      </c>
+      <c r="L52" s="36">
+        <f t="shared" si="1"/>
+        <v>163260</v>
+      </c>
+      <c r="M52" s="36">
+        <f t="shared" si="1"/>
+        <v>165555</v>
+      </c>
+      <c r="N52" s="36">
+        <f t="shared" si="1"/>
         <v>167850</v>
-      </c>
-      <c r="K52" s="36">
-        <f t="shared" si="4"/>
-        <v>171675</v>
-      </c>
-      <c r="L52" s="36">
-        <f t="shared" si="4"/>
-        <v>175500</v>
-      </c>
-      <c r="M52" s="36">
-        <f t="shared" si="4"/>
-        <v>179325</v>
-      </c>
-      <c r="N52" s="36">
-        <f t="shared" si="4"/>
-        <v>183150</v>
       </c>
     </row>
     <row r="53" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
@@ -4400,44 +4404,44 @@
         <v>0</v>
       </c>
       <c r="E53" s="50">
-        <f t="shared" ref="E53:N53" si="5">(E48*E47)+E49</f>
-        <v>17550</v>
+        <f>(E48*E47)+E49</f>
+        <v>7197.12</v>
       </c>
       <c r="F53" s="50">
-        <f t="shared" si="5"/>
-        <v>35100</v>
+        <f>(F48*F47)+F49</f>
+        <v>17280</v>
       </c>
       <c r="G53" s="50">
-        <f t="shared" si="5"/>
-        <v>52650</v>
+        <f>(G48*G47)+G49</f>
+        <v>25920</v>
       </c>
       <c r="H53" s="50">
-        <f t="shared" si="5"/>
-        <v>70200</v>
+        <f>(H48*H47)+H49</f>
+        <v>34560</v>
       </c>
       <c r="I53" s="50">
-        <f t="shared" si="5"/>
-        <v>87750</v>
+        <f>(I48*I47)+I49</f>
+        <v>43200</v>
       </c>
       <c r="J53" s="50">
-        <f t="shared" si="5"/>
-        <v>105300</v>
+        <f>(J48*J47)+J49</f>
+        <v>51840</v>
       </c>
       <c r="K53" s="50">
-        <f t="shared" si="5"/>
-        <v>122849.99999999999</v>
+        <f>(K48*K47)+K49</f>
+        <v>60479.999999999993</v>
       </c>
       <c r="L53" s="50">
-        <f t="shared" si="5"/>
-        <v>140400</v>
+        <f>(L48*L47)+L49</f>
+        <v>69120</v>
       </c>
       <c r="M53" s="50">
-        <f t="shared" si="5"/>
-        <v>157950</v>
+        <f>(M48*M47)+M49</f>
+        <v>77760</v>
       </c>
       <c r="N53" s="50">
-        <f t="shared" si="5"/>
-        <v>175500</v>
+        <f>(N48*N47)+N49</f>
+        <v>86400</v>
       </c>
     </row>
     <row r="54" spans="2:14" x14ac:dyDescent="0.2">
@@ -4450,44 +4454,44 @@
         <v>-144900</v>
       </c>
       <c r="E54" s="51">
-        <f t="shared" ref="E54:N54" si="6">E53-E52</f>
-        <v>-131175</v>
+        <f t="shared" ref="E54:N54" si="2">E53-E52</f>
+        <v>-139614.61499999999</v>
       </c>
       <c r="F54" s="51">
-        <f t="shared" si="6"/>
-        <v>-117450</v>
+        <f t="shared" si="2"/>
+        <v>-132210</v>
       </c>
       <c r="G54" s="51">
-        <f t="shared" si="6"/>
-        <v>-103725</v>
+        <f t="shared" si="2"/>
+        <v>-125865</v>
       </c>
       <c r="H54" s="51">
-        <f t="shared" si="6"/>
-        <v>-90000</v>
+        <f t="shared" si="2"/>
+        <v>-119520</v>
       </c>
       <c r="I54" s="51">
-        <f t="shared" si="6"/>
-        <v>-76275</v>
+        <f t="shared" si="2"/>
+        <v>-113175</v>
       </c>
       <c r="J54" s="51">
-        <f t="shared" si="6"/>
-        <v>-62550</v>
+        <f t="shared" si="2"/>
+        <v>-106830</v>
       </c>
       <c r="K54" s="51">
-        <f t="shared" si="6"/>
-        <v>-48825.000000000015</v>
+        <f t="shared" si="2"/>
+        <v>-100485</v>
       </c>
       <c r="L54" s="51">
-        <f t="shared" si="6"/>
-        <v>-35100</v>
+        <f t="shared" si="2"/>
+        <v>-94140</v>
       </c>
       <c r="M54" s="51">
-        <f t="shared" si="6"/>
-        <v>-21375</v>
+        <f t="shared" si="2"/>
+        <v>-87795</v>
       </c>
       <c r="N54" s="51">
-        <f t="shared" si="6"/>
-        <v>-7650</v>
+        <f t="shared" si="2"/>
+        <v>-81450</v>
       </c>
     </row>
   </sheetData>
@@ -4578,8 +4582,8 @@
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>838200</xdr:colOff>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>19050</xdr:colOff>
                     <xdr:row>20</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
@@ -4600,8 +4604,8 @@
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>828675</xdr:colOff>
+                    <xdr:col>7</xdr:col>
+                    <xdr:colOff>9525</xdr:colOff>
                     <xdr:row>18</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </to>

</xml_diff>

<commit_message>
Added pricing tier in table working
</commit_message>
<xml_diff>
--- a/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
+++ b/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" tabRatio="646" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Breakeven Analysis Data" sheetId="2" r:id="rId1"/>
     <sheet name="Breakeven Analysis Chart" sheetId="5" r:id="rId2"/>
-    <sheet name="Variables" sheetId="3" state="veryHidden" r:id="rId3"/>
+    <sheet name="Hosting Cost" sheetId="6" r:id="rId3"/>
+    <sheet name="Variables" sheetId="3" state="veryHidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_Example" hidden="1">Variables!$B$1</definedName>
@@ -22,25 +23,25 @@
     <definedName name="_Order1" hidden="1">0</definedName>
     <definedName name="_Series" hidden="1">Variables!$B$3</definedName>
     <definedName name="_Shading" hidden="1">Variables!$B$2</definedName>
-    <definedName name="Breakeven_point">'Breakeven Analysis Data'!$F$45</definedName>
+    <definedName name="Breakeven_point">'Breakeven Analysis Data'!$F$43</definedName>
     <definedName name="Company_name">'Breakeven Analysis Data'!$B$2</definedName>
     <definedName name="DATA_01" hidden="1">'Breakeven Analysis Data'!$B$2:$B$3</definedName>
     <definedName name="DATA_02" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_03" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_04" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_05" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
-    <definedName name="DATA_06" hidden="1">'Breakeven Analysis Data'!$F$14:$F$21</definedName>
+    <definedName name="DATA_06" hidden="1">'Breakeven Analysis Data'!$F$12:$F$19</definedName>
     <definedName name="DATA_07" hidden="1">'Breakeven Analysis Data'!#REF!</definedName>
     <definedName name="DATA_08" hidden="1">'Breakeven Analysis Data'!$H$5</definedName>
-    <definedName name="Fixed_costs">'Breakeven Analysis Data'!$F$29:$F$38</definedName>
-    <definedName name="Gross_margin">'Breakeven Analysis Data'!$G$26</definedName>
+    <definedName name="Fixed_costs">'Breakeven Analysis Data'!$F$27:$F$36</definedName>
+    <definedName name="Gross_margin">'Breakeven Analysis Data'!$G$24</definedName>
     <definedName name="IntroPrintArea" hidden="1">#REF!</definedName>
     <definedName name="Look1Area">#REF!</definedName>
     <definedName name="Look2Area">#REF!</definedName>
     <definedName name="Look3Area">#REF!</definedName>
     <definedName name="Look4Area">#REF!</definedName>
     <definedName name="Look5Area">#REF!</definedName>
-    <definedName name="Net_profit">'Breakeven Analysis Data'!$G$41</definedName>
+    <definedName name="Net_profit">'Breakeven Analysis Data'!$G$39</definedName>
     <definedName name="Sales_price_unitA">'Breakeven Analysis Data'!$F$6</definedName>
     <definedName name="Sales_price_unitB">'Breakeven Analysis Data'!$H$6</definedName>
     <definedName name="Sales_price_unitC">'Breakeven Analysis Data'!$J$6</definedName>
@@ -48,14 +49,14 @@
     <definedName name="Sales_volume_unitsB">'Breakeven Analysis Data'!$H$7</definedName>
     <definedName name="Sales_volume_unitsC">'Breakeven Analysis Data'!$J$7</definedName>
     <definedName name="TemplatePrintArea">'Breakeven Analysis Data'!$B$1:$G$5</definedName>
-    <definedName name="Total_fixed">'Breakeven Analysis Data'!$G$39</definedName>
+    <definedName name="Total_fixed">'Breakeven Analysis Data'!$G$37</definedName>
     <definedName name="Total_Sales">'Breakeven Analysis Data'!$G$9</definedName>
-    <definedName name="Total_Subscription">'Breakeven Analysis Data'!$G$12</definedName>
-    <definedName name="Total_variable">'Breakeven Analysis Data'!$G$23</definedName>
-    <definedName name="Unit_contrib_margin">'Breakeven Analysis Data'!$F$25</definedName>
-    <definedName name="Variable_cost_unit">'Breakeven Analysis Data'!$F$22</definedName>
-    <definedName name="Variable_costs_unit">'Breakeven Analysis Data'!$F$14:$F$21</definedName>
-    <definedName name="Variable_Unit_Cost">'Breakeven Analysis Data'!$F$22</definedName>
+    <definedName name="Total_Subscription">'Breakeven Analysis Data'!#REF!</definedName>
+    <definedName name="Total_variable">'Breakeven Analysis Data'!$G$21</definedName>
+    <definedName name="Unit_contrib_margin">'Breakeven Analysis Data'!$F$23</definedName>
+    <definedName name="Variable_cost_unit">'Breakeven Analysis Data'!$F$20</definedName>
+    <definedName name="Variable_costs_unit">'Breakeven Analysis Data'!$F$12:$F$19</definedName>
+    <definedName name="Variable_Unit_Cost">'Breakeven Analysis Data'!$F$20</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -159,7 +160,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{A3A9E55F-847E-4661-913D-184F52F6F529}">
+    <comment ref="F12" authorId="0" shapeId="0" xr:uid="{5CF3165E-FCBD-453E-AF2A-EA2B9BFC17C7}">
       <text>
         <r>
           <rPr>
@@ -168,25 +169,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Prijs maandelijks aangerekend voor hosting, support,...</t>
+          <t>Kost van 1 jaar servers te draaien</t>
         </r>
       </text>
     </comment>
-    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{5CF3165E-FCBD-453E-AF2A-EA2B9BFC17C7}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Kost van het opzetten van de servers per unit
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{5D839EBC-3BE3-4C34-8563-6F5A98C52E6E}">
+    <comment ref="F14" authorId="0" shapeId="0" xr:uid="{5D839EBC-3BE3-4C34-8563-6F5A98C52E6E}">
       <text>
         <r>
           <rPr>
@@ -200,7 +187,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{DF3550BB-FD51-4154-B794-6A8344BA2F43}">
+    <comment ref="F15" authorId="0" shapeId="0" xr:uid="{DF3550BB-FD51-4154-B794-6A8344BA2F43}">
       <text>
         <r>
           <rPr>
@@ -213,7 +200,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{70740BD0-CC66-4C54-86D3-8CFA9D18EBC2}">
+    <comment ref="F16" authorId="0" shapeId="0" xr:uid="{70740BD0-CC66-4C54-86D3-8CFA9D18EBC2}">
       <text>
         <r>
           <rPr>
@@ -237,7 +224,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{58D98360-D15F-4E39-A36D-F6F27D06BD03}">
+    <comment ref="F18" authorId="0" shapeId="0" xr:uid="{58D98360-D15F-4E39-A36D-F6F27D06BD03}">
       <text>
         <r>
           <rPr>
@@ -251,7 +238,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{0311ABD3-7CCC-4345-89C5-881F9C7EA603}">
+    <comment ref="F28" authorId="0" shapeId="0" xr:uid="{0311ABD3-7CCC-4345-89C5-881F9C7EA603}">
       <text>
         <r>
           <rPr>
@@ -264,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{F6D60EF9-0745-4CB6-8B69-14B527E69522}">
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{F6D60EF9-0745-4CB6-8B69-14B527E69522}">
       <text>
         <r>
           <rPr>
@@ -279,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{609A7C58-C559-486A-8D2D-85B7A7A7AE0A}">
+    <comment ref="F30" authorId="0" shapeId="0" xr:uid="{609A7C58-C559-486A-8D2D-85B7A7A7AE0A}">
       <text>
         <r>
           <rPr>
@@ -294,7 +281,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{EA10A0B4-ED7D-4B1B-9DF6-7CF415632FED}">
+    <comment ref="F31" authorId="0" shapeId="0" xr:uid="{EA10A0B4-ED7D-4B1B-9DF6-7CF415632FED}">
       <text>
         <r>
           <rPr>
@@ -308,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F36" authorId="0" shapeId="0" xr:uid="{165A2A66-A40C-4D4A-8EF3-CD46A0C51E76}">
+    <comment ref="F34" authorId="0" shapeId="0" xr:uid="{165A2A66-A40C-4D4A-8EF3-CD46A0C51E76}">
       <text>
         <r>
           <rPr>
@@ -342,7 +329,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F37" authorId="0" shapeId="0" xr:uid="{0D7BD022-B106-460F-B833-13D1C6EA7135}">
+    <comment ref="F35" authorId="0" shapeId="0" xr:uid="{0D7BD022-B106-460F-B833-13D1C6EA7135}">
       <text>
         <r>
           <rPr>
@@ -361,7 +348,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>_Example</t>
   </si>
@@ -387,9 +374,6 @@
     <t>Other fixed costs</t>
   </si>
   <si>
-    <t>Sales price per unit</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Total Sales</t>
   </si>
   <si>
@@ -498,29 +482,6 @@
     <t xml:space="preserve">    Net Profit</t>
   </si>
   <si>
-    <t>Sales volume (units)</t>
-  </si>
-  <si>
-    <t>Subscription per period</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Total Subscription</t>
-    </r>
-  </si>
-  <si>
-    <t>Subscription</t>
-  </si>
-  <si>
     <t>Sales price</t>
   </si>
   <si>
@@ -531,6 +492,60 @@
   </si>
   <si>
     <t>Amount of users</t>
+  </si>
+  <si>
+    <t>Sales volume 50</t>
+  </si>
+  <si>
+    <t>Sales price per unit 50</t>
+  </si>
+  <si>
+    <t>Sales volume 200</t>
+  </si>
+  <si>
+    <t>Sales price per unit 200</t>
+  </si>
+  <si>
+    <t>Sales volume 500</t>
+  </si>
+  <si>
+    <t>Sales price per unit 500</t>
+  </si>
+  <si>
+    <t>Zie sheet "Hosting cost"</t>
+  </si>
+  <si>
+    <t>Hosting Cost</t>
+  </si>
+  <si>
+    <t>Instance:</t>
+  </si>
+  <si>
+    <t>t2.small</t>
+  </si>
+  <si>
+    <t>t2.micro</t>
+  </si>
+  <si>
+    <t>Price per hour ($):</t>
+  </si>
+  <si>
+    <t>Working hours:</t>
+  </si>
+  <si>
+    <t>Working days:</t>
+  </si>
+  <si>
+    <t>Total ($)</t>
+  </si>
+  <si>
+    <t>Working weeks:</t>
+  </si>
+  <si>
+    <t>Total (Euro)</t>
+  </si>
+  <si>
+    <t>Dollar to Euro</t>
   </si>
 </sst>
 </file>
@@ -646,7 +661,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -668,6 +683,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -829,7 +850,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="72">
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="38" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -943,13 +964,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="38" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="37" fontId="1" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="37" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -979,6 +993,16 @@
     <xf numFmtId="38" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="40" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="38" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Date" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1218,7 +1242,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('Breakeven Analysis Data'!$C$22,'Breakeven Analysis Data'!$C$25)</c:f>
+              <c:f>('Breakeven Analysis Data'!$C$20,'Breakeven Analysis Data'!$C$23)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1232,15 +1256,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Breakeven Analysis Data'!$F$22,'Breakeven Analysis Data'!$F$25)</c:f>
+              <c:f>('Breakeven Analysis Data'!$F$20,'Breakeven Analysis Data'!$F$23)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>850</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2350</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1505,7 +1529,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$C$15:$C$21</c:f>
+              <c:f>'Breakeven Analysis Data'!$C$13:$C$19</c:f>
               <c:strCache>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
@@ -1534,12 +1558,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$F$14:$F$21</c:f>
+              <c:f>'Breakeven Analysis Data'!$F$12:$F$19</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -1548,13 +1572,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>250</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>300</c:v>
+                  <c:v>500</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>100</c:v>
@@ -1813,7 +1837,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>('Breakeven Analysis Data'!$C$22,'Breakeven Analysis Data'!$C$25)</c:f>
+              <c:f>('Breakeven Analysis Data'!$C$20,'Breakeven Analysis Data'!$C$23)</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -1827,15 +1851,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>('Breakeven Analysis Data'!$F$22,'Breakeven Analysis Data'!$F$25)</c:f>
+              <c:f>('Breakeven Analysis Data'!$F$20,'Breakeven Analysis Data'!$F$23)</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>850</c:v>
+                  <c:v>1700</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2350</c:v>
+                  <c:v>1400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2014,7 +2038,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$50</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$51</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2048,42 +2072,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$50:$N$50</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$51:$N$51</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2100,7 +2124,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$52</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$53</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2134,42 +2158,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$52:$N$52</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$53:$N$53</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>144900</c:v>
+                  <c:v>124900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>146811.73499999999</c:v>
+                  <c:v>129150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>149490</c:v>
+                  <c:v>133400</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>151785</c:v>
+                  <c:v>137650</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>154080</c:v>
+                  <c:v>141900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>156375</c:v>
+                  <c:v>146150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>158670</c:v>
+                  <c:v>150400</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>160965</c:v>
+                  <c:v>154650</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>163260</c:v>
+                  <c:v>158900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>165555</c:v>
+                  <c:v>163150</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>167850</c:v>
+                  <c:v>167400</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2186,7 +2210,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$53</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$54</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2220,7 +2244,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$53:$N$53</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$54:$N$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2228,34 +2252,34 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7197.12</c:v>
+                  <c:v>18290</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17280</c:v>
+                  <c:v>36580</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>25920</c:v>
+                  <c:v>54870</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34560</c:v>
+                  <c:v>73160</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>43200</c:v>
+                  <c:v>91450</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51840</c:v>
+                  <c:v>109740</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>60479.999999999993</c:v>
+                  <c:v>128030</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>69120</c:v>
+                  <c:v>146320</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>77760</c:v>
+                  <c:v>164610</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>86400</c:v>
+                  <c:v>182900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2272,7 +2296,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Breakeven Analysis Data'!$B$54</c:f>
+              <c:f>'Breakeven Analysis Data'!$B$55</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2304,42 +2328,42 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$54:$N$54</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$55:$N$55</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>-144900</c:v>
+                  <c:v>-124900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-139614.61499999999</c:v>
+                  <c:v>-110860</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-132210</c:v>
+                  <c:v>-96820</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-125865</c:v>
+                  <c:v>-82780</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-119520</c:v>
+                  <c:v>-68740</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-113175</c:v>
+                  <c:v>-54700</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-106830</c:v>
+                  <c:v>-40660</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-100485</c:v>
+                  <c:v>-26620</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-94140</c:v>
+                  <c:v>-12580</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>-87795</c:v>
+                  <c:v>1460</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-81450</c:v>
+                  <c:v>15500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2641,30 +2665,26 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" inc="100" max="10000" min="500" page="10" val="3200"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" inc="100" max="10000" min="500" page="10" val="3100"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$7" horiz="1" max="50" min="1" page="10" val="20"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$7" horiz="1" max="50" min="1" page="10" val="25"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$20" horiz="1" inc="100" max="1000" page="10" val="300"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$18" horiz="1" inc="100" max="1000" page="10" val="500"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$18" horiz="1" inc="50" max="1000" page="10" val="250"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$16" horiz="1" inc="50" max="1000" page="10" val="500"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$11" horiz="1" inc="100" max="10000" page="0" val="0"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$7" horiz="1" max="50" min="1" page="10" val="5"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$H$7" horiz="1" max="50" min="1" page="10" val="5"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp7.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$J$7" horiz="1" max="50" min="1" page="10" val="2"/>
 </file>
 
@@ -2680,7 +2700,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>339587</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>10</xdr:row>
       <xdr:rowOff>25466</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2712,13 +2732,13 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>165976</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>25400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>318376</xdr:colOff>
-      <xdr:row>44</xdr:row>
+      <xdr:row>42</xdr:row>
       <xdr:rowOff>241300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2852,13 +2872,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>19</xdr:row>
+          <xdr:row>17</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>20</xdr:row>
+          <xdr:row>18</xdr:row>
           <xdr:rowOff>19050</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2902,13 +2922,13 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>17</xdr:row>
+          <xdr:row>15</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:from>
         <xdr:to>
           <xdr:col>7</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
-          <xdr:row>18</xdr:row>
+          <xdr:row>16</xdr:row>
           <xdr:rowOff>9525</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
@@ -2920,56 +2940,6 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln w="9525">
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a:ln>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>790575</xdr:colOff>
-          <xdr:row>10</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1046" name="Scroll Bar 22" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1046"/>
-                </a:ext>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3107,7 +3077,7 @@
       <xdr:col>33</xdr:col>
       <xdr:colOff>506464</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>196524</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3496,10 +3466,10 @@
     <tabColor indexed="26"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N54"/>
+  <dimension ref="A1:N55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3537,7 +3507,7 @@
     <row r="2" spans="1:11" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A2" s="4"/>
       <c r="B2" s="27" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="2"/>
@@ -3549,7 +3519,7 @@
     <row r="3" spans="1:11" s="14" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="13"/>
       <c r="B3" s="40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" s="40"/>
       <c r="D3" s="15"/>
@@ -3558,20 +3528,20 @@
     <row r="4" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
       <c r="B4" s="41" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="C4" s="41"/>
       <c r="D4" s="28"/>
       <c r="E4" s="5"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="65" t="s">
-        <v>50</v>
-      </c>
-      <c r="H4" s="66">
+      <c r="G4" s="62" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="63">
         <v>0.1</v>
       </c>
       <c r="I4" s="14"/>
-      <c r="J4" s="66">
+      <c r="J4" s="63">
         <v>0.2</v>
       </c>
       <c r="K4" s="14"/>
@@ -3580,18 +3550,18 @@
       <c r="A5" s="4"/>
       <c r="B5" s="11"/>
       <c r="C5" s="1" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="60">
+      <c r="F5" s="57">
         <v>50</v>
       </c>
-      <c r="G5" s="59"/>
-      <c r="H5" s="67">
+      <c r="G5" s="56"/>
+      <c r="H5" s="64">
         <v>200</v>
       </c>
-      <c r="I5" s="63"/>
-      <c r="J5" s="68">
+      <c r="I5" s="60"/>
+      <c r="J5" s="65">
         <v>500</v>
       </c>
     </row>
@@ -3599,31 +3569,31 @@
       <c r="A6" s="4"/>
       <c r="B6" s="12"/>
       <c r="C6" s="52" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="61">
-        <v>3200</v>
+      <c r="F6" s="58">
+        <v>3100</v>
       </c>
       <c r="G6" s="7"/>
-      <c r="H6" s="61">
+      <c r="H6" s="58">
         <f>Sales_price_unitA*(H5/F5)*(1-H4)</f>
-        <v>11520</v>
-      </c>
-      <c r="J6" s="61">
+        <v>11160</v>
+      </c>
+      <c r="J6" s="58">
         <f>Sales_price_unitA*(J5/F5)*(1-J4)</f>
-        <v>25600</v>
+        <v>24800</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="12"/>
       <c r="C7" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="43">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="43">
@@ -3636,28 +3606,28 @@
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B8" s="34"/>
       <c r="C8" s="12"/>
-      <c r="F8" s="64">
+      <c r="F8" s="61">
         <f>IF(OR(Sales_price_unitA&lt;&gt;0,Sales_volume_unitsA&lt;&gt;0),Sales_price_unitA*Sales_volume_unitsA,0)</f>
-        <v>64000</v>
+        <v>77500</v>
       </c>
       <c r="G8" s="8"/>
-      <c r="H8" s="64">
+      <c r="H8" s="61">
         <f>IF(OR(Sales_price_unitB&lt;&gt;0,Sales_volume_unitsB&lt;&gt;0),Sales_price_unitB*Sales_volume_unitsB,0)</f>
-        <v>57600</v>
-      </c>
-      <c r="J8" s="64">
+        <v>55800</v>
+      </c>
+      <c r="J8" s="61">
         <f>IF(OR(Sales_price_unitC&lt;&gt;0,Sales_volume_unitsC&lt;&gt;0),Sales_price_unitC*Sales_volume_unitsC,0)</f>
-        <v>51200</v>
+        <v>49600</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B9" s="34"/>
       <c r="C9" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" s="62">
+        <v>8</v>
+      </c>
+      <c r="G9" s="59">
         <f>F8+H8+J8</f>
-        <v>172800</v>
+        <v>182900</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3668,73 +3638,74 @@
       <c r="G10" s="19"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="E11" s="4"/>
-      <c r="F11" s="43">
-        <v>0</v>
-      </c>
+      <c r="B11" s="42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="17"/>
       <c r="G11" s="17"/>
     </row>
-    <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="11"/>
-      <c r="C12" s="57" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="56"/>
-      <c r="G12" s="58">
-        <f>F11</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="34" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="3"/>
+      <c r="F12" s="30">
+        <v>500</v>
+      </c>
+      <c r="G12" s="55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="6"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="17"/>
-      <c r="G13" s="17"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="52" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="53"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="11"/>
-      <c r="C14" s="34" t="s">
-        <v>36</v>
+      <c r="C14" s="52" t="s">
+        <v>30</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="30">
         <v>100</v>
       </c>
-      <c r="G14" s="55"/>
+      <c r="G14" s="53"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="11"/>
       <c r="C15" s="52" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="E15" s="3"/>
-      <c r="F15" s="30"/>
+      <c r="F15" s="30">
+        <v>0</v>
+      </c>
       <c r="G15" s="53"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="11"/>
       <c r="C16" s="52" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="30">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="G16" s="53"/>
     </row>
@@ -3742,7 +3713,7 @@
       <c r="A17" s="4"/>
       <c r="B17" s="11"/>
       <c r="C17" s="52" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="30">
@@ -3754,144 +3725,146 @@
       <c r="A18" s="4"/>
       <c r="B18" s="11"/>
       <c r="C18" s="52" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="30">
-        <v>250</v>
+        <v>500</v>
       </c>
       <c r="G18" s="53"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="11"/>
-      <c r="C19" s="52" t="s">
-        <v>32</v>
+      <c r="C19" s="11" t="s">
+        <v>20</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="30">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="G19" s="53"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="11"/>
-      <c r="C20" s="52" t="s">
-        <v>29</v>
+      <c r="C20" s="33" t="s">
+        <v>14</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="30">
-        <v>300</v>
-      </c>
-      <c r="G20" s="53"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F20" s="32">
+        <f>IF(SUM(Variable_costs_unit),SUM(Variable_costs_unit),0)</f>
+        <v>1700</v>
+      </c>
+      <c r="G20" s="54"/>
+    </row>
+    <row r="21" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="11"/>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="33" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="3"/>
-      <c r="F21" s="30">
-        <v>100</v>
-      </c>
-      <c r="G21" s="53"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="44">
+        <f>IF(Variable_Unit_Cost,Variable_Unit_Cost*(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC),0)</f>
+        <v>54400</v>
+      </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="11"/>
-      <c r="C22" s="33" t="s">
-        <v>15</v>
-      </c>
+      <c r="C22" s="33"/>
       <c r="E22" s="3"/>
-      <c r="F22" s="32">
-        <f>IF(SUM(Variable_costs_unit),SUM(Variable_costs_unit),0)</f>
-        <v>850</v>
-      </c>
-      <c r="G22" s="54"/>
-    </row>
-    <row r="23" spans="1:8" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="11"/>
       <c r="C23" s="33" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="44">
-        <f>IF(Variable_Unit_Cost,Variable_Unit_Cost*(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC),0)</f>
-        <v>22950</v>
-      </c>
+      <c r="F23" s="31">
+        <f>IF(Sales_price_unitA&gt;0,MAX(0,Sales_price_unitA-Variable_Unit_Cost),0)</f>
+        <v>1400</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="11"/>
-      <c r="C24" s="33"/>
+      <c r="C24" s="33" t="s">
+        <v>9</v>
+      </c>
       <c r="E24" s="3"/>
       <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
+      <c r="G24" s="31">
+        <f>IF(OR(Total_Sales&lt;&gt;0,Total_variable&lt;&gt;0),Total_Sales-Total_variable,0)</f>
+        <v>128500</v>
+      </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="11"/>
-      <c r="C25" s="33" t="s">
-        <v>16</v>
-      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="20"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="31">
-        <f>IF(Sales_price_unitA&gt;0,MAX(0,Sales_price_unitA-Variable_Unit_Cost),0)</f>
-        <v>2350</v>
-      </c>
+      <c r="F25" s="17"/>
       <c r="G25" s="18"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="33" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="31">
-        <f>IF(OR(Total_Sales&lt;&gt;0,Total_variable&lt;&gt;0),Total_Sales-Total_variable,0)</f>
-        <v>149850</v>
-      </c>
+      <c r="B26" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="C26" s="42"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="49"/>
+      <c r="G26" s="17"/>
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="20"/>
+      <c r="C27" s="34" t="s">
+        <v>32</v>
+      </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="17"/>
-      <c r="G27" s="18"/>
+      <c r="F27" s="30">
+        <v>50000</v>
+      </c>
+      <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
-      <c r="B28" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="17"/>
+      <c r="B28" s="11"/>
+      <c r="C28" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="3"/>
+      <c r="F28" s="30">
+        <v>0</v>
+      </c>
+      <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="11"/>
       <c r="C29" s="34" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="30">
-        <v>60000</v>
+        <v>20000</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -3900,11 +3873,11 @@
       <c r="A30" s="4"/>
       <c r="B30" s="11"/>
       <c r="C30" s="34" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="30">
-        <v>0</v>
+        <v>2400</v>
       </c>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
@@ -3913,11 +3886,11 @@
       <c r="A31" s="4"/>
       <c r="B31" s="11"/>
       <c r="C31" s="34" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E31" s="3"/>
       <c r="F31" s="30">
-        <v>30000</v>
+        <v>10000</v>
       </c>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
@@ -3925,12 +3898,12 @@
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="11"/>
-      <c r="C32" s="34" t="s">
-        <v>34</v>
+      <c r="C32" s="52" t="s">
+        <v>38</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="30">
-        <v>2400</v>
+        <v>5000</v>
       </c>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
@@ -3938,13 +3911,11 @@
     <row r="33" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="11"/>
-      <c r="C33" s="34" t="s">
-        <v>38</v>
+      <c r="C33" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="E33" s="3"/>
-      <c r="F33" s="30">
-        <v>10000</v>
-      </c>
+      <c r="F33" s="30"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
@@ -3952,11 +3923,11 @@
       <c r="A34" s="4"/>
       <c r="B34" s="11"/>
       <c r="C34" s="52" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="30">
-        <v>5000</v>
+      <c r="F34" s="45">
+        <v>20000</v>
       </c>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
@@ -3964,534 +3935,660 @@
     <row r="35" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="11"/>
-      <c r="C35" s="11" t="s">
-        <v>6</v>
+      <c r="C35" s="52" t="s">
+        <v>39</v>
       </c>
       <c r="E35" s="3"/>
-      <c r="F35" s="30"/>
+      <c r="F35" s="48">
+        <v>15000</v>
+      </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="11"/>
-      <c r="C36" s="52" t="s">
-        <v>28</v>
+      <c r="C36" s="11" t="s">
+        <v>7</v>
       </c>
       <c r="E36" s="3"/>
-      <c r="F36" s="45">
-        <v>20000</v>
+      <c r="F36" s="29">
+        <v>2500</v>
       </c>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="11"/>
-      <c r="C37" s="52" t="s">
-        <v>40</v>
+      <c r="C37" s="33" t="s">
+        <v>24</v>
       </c>
       <c r="E37" s="3"/>
-      <c r="F37" s="48">
-        <v>15000</v>
-      </c>
-      <c r="G37" s="1"/>
+      <c r="F37" s="17"/>
+      <c r="G37" s="46">
+        <f>IF(SUM(Fixed_costs)&lt;&gt;0,SUM(Fixed_costs),0)</f>
+        <v>124900</v>
+      </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A38" s="4"/>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="29">
-        <v>2500</v>
-      </c>
-      <c r="G38" s="1"/>
+    <row r="38" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="34"/>
+      <c r="C38" s="34"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="19"/>
       <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="11"/>
       <c r="C39" s="33" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E39" s="3"/>
-      <c r="F39" s="17"/>
-      <c r="G39" s="46">
-        <f>IF(SUM(Fixed_costs)&lt;&gt;0,SUM(Fixed_costs),0)</f>
-        <v>144900</v>
+      <c r="G39" s="47">
+        <f>IF(OR(Gross_margin&lt;&gt;0,Total_fixed&lt;&gt;0),Gross_margin-Total_fixed,0)</f>
+        <v>3600</v>
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
-      <c r="F40" s="17"/>
       <c r="G40" s="19"/>
-      <c r="H40" s="1"/>
-    </row>
-    <row r="41" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="3"/>
-      <c r="G41" s="47">
-        <f>IF(OR(Gross_margin&lt;&gt;0,Total_fixed&lt;&gt;0),Gross_margin-Total_fixed,0)</f>
-        <v>4950</v>
-      </c>
-      <c r="H41" s="1"/>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B42" s="34"/>
-      <c r="C42" s="34"/>
-      <c r="G42" s="19"/>
-    </row>
-    <row r="43" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
-      <c r="B43" s="34"/>
-      <c r="C43" s="34"/>
-      <c r="F43" s="23"/>
-    </row>
-    <row r="44" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
-      <c r="B44" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C44" s="23"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="1"/>
-    </row>
-    <row r="45" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B45" s="39" t="s">
+    </row>
+    <row r="41" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
+      <c r="B41" s="34"/>
+      <c r="C41" s="34"/>
+      <c r="F41" s="23"/>
+    </row>
+    <row r="42" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
+      <c r="B42" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C45" s="39"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="38">
+      <c r="C42" s="23"/>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+    </row>
+    <row r="43" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B43" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C43" s="39"/>
+      <c r="D43" s="25"/>
+      <c r="E43" s="25"/>
+      <c r="F43" s="38">
         <f>IF(AND(Unit_contrib_margin&gt;0,Total_fixed&gt;0),Total_fixed/Unit_contrib_margin,"")</f>
-        <v>61.659574468085104</v>
-      </c>
-      <c r="G45" s="24"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="26"/>
-    </row>
-    <row r="46" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B46" s="39" t="s">
+        <v>89.214285714285708</v>
+      </c>
+      <c r="G43" s="24"/>
+      <c r="H43" s="25"/>
+      <c r="I43" s="25"/>
+      <c r="J43" s="26"/>
+    </row>
+    <row r="44" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B44" s="39" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="39"/>
+      <c r="D44" s="25"/>
+      <c r="E44" s="25"/>
+      <c r="F44" s="26"/>
+      <c r="G44" s="24"/>
+      <c r="H44" s="25"/>
+      <c r="I44" s="25"/>
+      <c r="J44" s="26"/>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B45" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="34"/>
+      <c r="D45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0,0)</f>
+        <v>0</v>
+      </c>
+      <c r="E45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.1,0)</f>
+        <v>2.5</v>
+      </c>
+      <c r="F45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.2,0)</f>
+        <v>5</v>
+      </c>
+      <c r="G45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.3,0)</f>
+        <v>7.5</v>
+      </c>
+      <c r="H45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.4,0)</f>
+        <v>10</v>
+      </c>
+      <c r="I45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.5,0)</f>
+        <v>12.5</v>
+      </c>
+      <c r="J45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.6,0)</f>
+        <v>15</v>
+      </c>
+      <c r="K45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.7,0)</f>
+        <v>17.5</v>
+      </c>
+      <c r="L45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.8,0)</f>
         <v>20</v>
       </c>
-      <c r="C46" s="39"/>
-      <c r="D46" s="25"/>
-      <c r="E46" s="25"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="25"/>
-      <c r="J46" s="26"/>
+      <c r="M45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.9,0)</f>
+        <v>22.5</v>
+      </c>
+      <c r="N45" s="35">
+        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA),0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="B46" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C46" s="34"/>
+      <c r="D46" s="36">
+        <f t="shared" ref="D46:N46" si="0">(Sales_price_unitA)</f>
+        <v>3100</v>
+      </c>
+      <c r="E46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="F46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="G46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="H46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="I46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="J46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="K46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="L46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="M46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
+      <c r="N46" s="36">
+        <f t="shared" si="0"/>
+        <v>3100</v>
+      </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B47" s="34" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="C47" s="34"/>
       <c r="D47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0,0)</f>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0,0)</f>
         <v>0</v>
       </c>
       <c r="E47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.0833,0)</f>
-        <v>2.2490999999999999</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.1,0)</f>
+        <v>0.5</v>
       </c>
       <c r="F47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.2,0)</f>
-        <v>5.4</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.2,0)</f>
+        <v>1</v>
       </c>
       <c r="G47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.3,0)</f>
-        <v>8.1</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.3,0)</f>
+        <v>1.5</v>
       </c>
       <c r="H47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.4,0)</f>
-        <v>10.8</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.4,0)</f>
+        <v>2</v>
       </c>
       <c r="I47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.5,0)</f>
-        <v>13.5</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.5,0)</f>
+        <v>2.5</v>
       </c>
       <c r="J47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.6,0)</f>
-        <v>16.2</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.6,0)</f>
+        <v>3</v>
       </c>
       <c r="K47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.7,0)</f>
-        <v>18.899999999999999</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.7,0)</f>
+        <v>3.5</v>
       </c>
       <c r="L47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.8,0)</f>
-        <v>21.6</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.8,0)</f>
+        <v>4</v>
       </c>
       <c r="M47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*0.9,0)</f>
-        <v>24.3</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.9,0)</f>
+        <v>4.5</v>
       </c>
       <c r="N47" s="35">
-        <f>IF(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC,(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC)*1,0)</f>
-        <v>27</v>
+        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB),0)</f>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B48" s="34" t="s">
-        <v>8</v>
+        <v>51</v>
       </c>
       <c r="C48" s="34"/>
       <c r="D48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="E48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="F48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="G48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="H48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="I48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="J48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="K48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="L48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="M48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
       <c r="N48" s="36">
-        <f>(Sales_price_unitA)</f>
-        <v>3200</v>
+        <f>Sales_price_unitB</f>
+        <v>11160</v>
       </c>
     </row>
     <row r="49" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B49" s="34" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C49" s="34"/>
-      <c r="D49" s="36">
-        <f>Total_Subscription*D47</f>
+      <c r="D49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0,0)</f>
         <v>0</v>
       </c>
-      <c r="E49" s="36">
-        <f>Total_Subscription*E47</f>
-        <v>0</v>
-      </c>
-      <c r="F49" s="36">
-        <f>Total_Subscription*F47</f>
-        <v>0</v>
-      </c>
-      <c r="G49" s="36">
-        <f>Total_Subscription*G47</f>
-        <v>0</v>
-      </c>
-      <c r="H49" s="36">
-        <f>Total_Subscription*H47</f>
-        <v>0</v>
-      </c>
-      <c r="I49" s="36">
-        <f>Total_Subscription*I47</f>
-        <v>0</v>
-      </c>
-      <c r="J49" s="36">
-        <f>Total_Subscription*J47</f>
-        <v>0</v>
-      </c>
-      <c r="K49" s="36">
-        <f>Total_Subscription*K47</f>
-        <v>0</v>
-      </c>
-      <c r="L49" s="36">
-        <f>Total_Subscription*L47</f>
-        <v>0</v>
-      </c>
-      <c r="M49" s="36">
-        <f>Total_Subscription*M47</f>
-        <v>0</v>
-      </c>
-      <c r="N49" s="36">
-        <f>Total_Subscription*N47</f>
-        <v>0</v>
+      <c r="E49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.1,0)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.2,0)</f>
+        <v>0.4</v>
+      </c>
+      <c r="G49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.3,0)</f>
+        <v>0.6</v>
+      </c>
+      <c r="H49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.4,0)</f>
+        <v>0.8</v>
+      </c>
+      <c r="I49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.5,0)</f>
+        <v>1</v>
+      </c>
+      <c r="J49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.6,0)</f>
+        <v>1.2</v>
+      </c>
+      <c r="K49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.7,0)</f>
+        <v>1.4</v>
+      </c>
+      <c r="L49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.8,0)</f>
+        <v>1.6</v>
+      </c>
+      <c r="M49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.9,0)</f>
+        <v>1.8</v>
+      </c>
+      <c r="N49" s="35">
+        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC),0)</f>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B50" s="34" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="C50" s="34"/>
-      <c r="D50" s="36">
-        <f t="shared" ref="D50:N50" si="0">Total_fixed</f>
-        <v>144900</v>
-      </c>
-      <c r="E50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="F50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="G50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="H50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="I50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="J50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="K50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="L50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="M50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
-      </c>
-      <c r="N50" s="36">
-        <f t="shared" si="0"/>
-        <v>144900</v>
+      <c r="D50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="E50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="F50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="G50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="H50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="I50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="J50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="K50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="L50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="M50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
+      </c>
+      <c r="N50" s="66">
+        <f>Sales_price_unitC</f>
+        <v>24800</v>
       </c>
     </row>
     <row r="51" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B51" s="37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C51" s="37"/>
+      <c r="B51" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="C51" s="34"/>
       <c r="D51" s="36">
-        <f>Variable_Unit_Cost*D47</f>
-        <v>0</v>
+        <f t="shared" ref="D51:N51" si="1">Total_fixed</f>
+        <v>124900</v>
       </c>
       <c r="E51" s="36">
-        <f>Variable_Unit_Cost*E47</f>
-        <v>1911.7349999999999</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="F51" s="36">
-        <f>Variable_Unit_Cost*F47</f>
-        <v>4590</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="G51" s="36">
-        <f>Variable_Unit_Cost*G47</f>
-        <v>6885</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="H51" s="36">
-        <f>Variable_Unit_Cost*H47</f>
-        <v>9180</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="I51" s="36">
-        <f>Variable_Unit_Cost*I47</f>
-        <v>11475</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="J51" s="36">
-        <f>Variable_Unit_Cost*J47</f>
-        <v>13770</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="K51" s="36">
-        <f>Variable_Unit_Cost*K47</f>
-        <v>16064.999999999998</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="L51" s="36">
-        <f>Variable_Unit_Cost*L47</f>
-        <v>18360</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="M51" s="36">
-        <f>Variable_Unit_Cost*M47</f>
-        <v>20655</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
       <c r="N51" s="36">
-        <f>Variable_Unit_Cost*N47</f>
-        <v>22950</v>
+        <f t="shared" si="1"/>
+        <v>124900</v>
       </c>
     </row>
     <row r="52" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B52" s="37" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="36">
-        <f t="shared" ref="D52:N52" si="1">SUM(D50:D51)</f>
-        <v>144900</v>
+        <f>Variable_Unit_Cost*D45</f>
+        <v>0</v>
       </c>
       <c r="E52" s="36">
-        <f t="shared" si="1"/>
-        <v>146811.73499999999</v>
+        <f>Variable_Unit_Cost*E45</f>
+        <v>4250</v>
       </c>
       <c r="F52" s="36">
-        <f t="shared" si="1"/>
-        <v>149490</v>
+        <f>Variable_Unit_Cost*F45</f>
+        <v>8500</v>
       </c>
       <c r="G52" s="36">
-        <f t="shared" si="1"/>
-        <v>151785</v>
+        <f>Variable_Unit_Cost*G45</f>
+        <v>12750</v>
       </c>
       <c r="H52" s="36">
-        <f t="shared" si="1"/>
-        <v>154080</v>
+        <f>Variable_Unit_Cost*H45</f>
+        <v>17000</v>
       </c>
       <c r="I52" s="36">
-        <f t="shared" si="1"/>
-        <v>156375</v>
+        <f>Variable_Unit_Cost*I45</f>
+        <v>21250</v>
       </c>
       <c r="J52" s="36">
-        <f t="shared" si="1"/>
-        <v>158670</v>
+        <f>Variable_Unit_Cost*J45</f>
+        <v>25500</v>
       </c>
       <c r="K52" s="36">
-        <f t="shared" si="1"/>
-        <v>160965</v>
+        <f>Variable_Unit_Cost*K45</f>
+        <v>29750</v>
       </c>
       <c r="L52" s="36">
-        <f t="shared" si="1"/>
-        <v>163260</v>
+        <f>Variable_Unit_Cost*L45</f>
+        <v>34000</v>
       </c>
       <c r="M52" s="36">
-        <f t="shared" si="1"/>
-        <v>165555</v>
+        <f>Variable_Unit_Cost*M45</f>
+        <v>38250</v>
       </c>
       <c r="N52" s="36">
-        <f t="shared" si="1"/>
-        <v>167850</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B53" s="34" t="s">
+        <f>Variable_Unit_Cost*N45</f>
+        <v>42500</v>
+      </c>
+    </row>
+    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B53" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="C53" s="34"/>
-      <c r="D53" s="50">
-        <f>(D48*D47)+D49</f>
+      <c r="C53" s="37"/>
+      <c r="D53" s="36">
+        <f>SUM(D51:D52)</f>
+        <v>124900</v>
+      </c>
+      <c r="E53" s="36">
+        <f t="shared" ref="E53:N53" si="2">SUM(E51:E52)</f>
+        <v>129150</v>
+      </c>
+      <c r="F53" s="36">
+        <f t="shared" si="2"/>
+        <v>133400</v>
+      </c>
+      <c r="G53" s="36">
+        <f t="shared" si="2"/>
+        <v>137650</v>
+      </c>
+      <c r="H53" s="36">
+        <f t="shared" si="2"/>
+        <v>141900</v>
+      </c>
+      <c r="I53" s="36">
+        <f t="shared" si="2"/>
+        <v>146150</v>
+      </c>
+      <c r="J53" s="36">
+        <f t="shared" si="2"/>
+        <v>150400</v>
+      </c>
+      <c r="K53" s="36">
+        <f t="shared" si="2"/>
+        <v>154650</v>
+      </c>
+      <c r="L53" s="36">
+        <f t="shared" si="2"/>
+        <v>158900</v>
+      </c>
+      <c r="M53" s="36">
+        <f t="shared" si="2"/>
+        <v>163150</v>
+      </c>
+      <c r="N53" s="36">
+        <f t="shared" si="2"/>
+        <v>167400</v>
+      </c>
+    </row>
+    <row r="54" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C54" s="34"/>
+      <c r="D54" s="50">
+        <f>((D46*D45)+(D47*D48)+(D49*D50))</f>
         <v>0</v>
       </c>
-      <c r="E53" s="50">
-        <f>(E48*E47)+E49</f>
-        <v>7197.12</v>
-      </c>
-      <c r="F53" s="50">
-        <f>(F48*F47)+F49</f>
-        <v>17280</v>
-      </c>
-      <c r="G53" s="50">
-        <f>(G48*G47)+G49</f>
-        <v>25920</v>
-      </c>
-      <c r="H53" s="50">
-        <f>(H48*H47)+H49</f>
-        <v>34560</v>
-      </c>
-      <c r="I53" s="50">
-        <f>(I48*I47)+I49</f>
-        <v>43200</v>
-      </c>
-      <c r="J53" s="50">
-        <f>(J48*J47)+J49</f>
-        <v>51840</v>
-      </c>
-      <c r="K53" s="50">
-        <f>(K48*K47)+K49</f>
-        <v>60479.999999999993</v>
-      </c>
-      <c r="L53" s="50">
-        <f>(L48*L47)+L49</f>
-        <v>69120</v>
-      </c>
-      <c r="M53" s="50">
-        <f>(M48*M47)+M49</f>
-        <v>77760</v>
-      </c>
-      <c r="N53" s="50">
-        <f>(N48*N47)+N49</f>
-        <v>86400</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B54" s="37" t="s">
-        <v>19</v>
-      </c>
-      <c r="C54" s="37"/>
-      <c r="D54" s="51">
-        <f>D53-D52</f>
-        <v>-144900</v>
-      </c>
-      <c r="E54" s="51">
-        <f t="shared" ref="E54:N54" si="2">E53-E52</f>
-        <v>-139614.61499999999</v>
-      </c>
-      <c r="F54" s="51">
-        <f t="shared" si="2"/>
-        <v>-132210</v>
-      </c>
-      <c r="G54" s="51">
-        <f t="shared" si="2"/>
-        <v>-125865</v>
-      </c>
-      <c r="H54" s="51">
-        <f t="shared" si="2"/>
-        <v>-119520</v>
-      </c>
-      <c r="I54" s="51">
-        <f t="shared" si="2"/>
-        <v>-113175</v>
-      </c>
-      <c r="J54" s="51">
-        <f t="shared" si="2"/>
-        <v>-106830</v>
-      </c>
-      <c r="K54" s="51">
-        <f t="shared" si="2"/>
-        <v>-100485</v>
-      </c>
-      <c r="L54" s="51">
-        <f t="shared" si="2"/>
-        <v>-94140</v>
-      </c>
-      <c r="M54" s="51">
-        <f t="shared" si="2"/>
-        <v>-87795</v>
-      </c>
-      <c r="N54" s="51">
-        <f t="shared" si="2"/>
-        <v>-81450</v>
+      <c r="E54" s="50">
+        <f t="shared" ref="E54:N54" si="3">((E46*E45)+(E47*E48)+(E49*E50))</f>
+        <v>18290</v>
+      </c>
+      <c r="F54" s="50">
+        <f t="shared" si="3"/>
+        <v>36580</v>
+      </c>
+      <c r="G54" s="50">
+        <f t="shared" si="3"/>
+        <v>54870</v>
+      </c>
+      <c r="H54" s="50">
+        <f t="shared" si="3"/>
+        <v>73160</v>
+      </c>
+      <c r="I54" s="50">
+        <f t="shared" si="3"/>
+        <v>91450</v>
+      </c>
+      <c r="J54" s="50">
+        <f t="shared" si="3"/>
+        <v>109740</v>
+      </c>
+      <c r="K54" s="50">
+        <f t="shared" si="3"/>
+        <v>128030</v>
+      </c>
+      <c r="L54" s="50">
+        <f t="shared" si="3"/>
+        <v>146320</v>
+      </c>
+      <c r="M54" s="50">
+        <f t="shared" si="3"/>
+        <v>164610</v>
+      </c>
+      <c r="N54" s="50">
+        <f t="shared" si="3"/>
+        <v>182900</v>
+      </c>
+    </row>
+    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B55" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C55" s="37"/>
+      <c r="D55" s="51">
+        <f>D54-D53</f>
+        <v>-124900</v>
+      </c>
+      <c r="E55" s="51">
+        <f t="shared" ref="E55:N55" si="4">E54-E53</f>
+        <v>-110860</v>
+      </c>
+      <c r="F55" s="51">
+        <f t="shared" si="4"/>
+        <v>-96820</v>
+      </c>
+      <c r="G55" s="51">
+        <f t="shared" si="4"/>
+        <v>-82780</v>
+      </c>
+      <c r="H55" s="51">
+        <f t="shared" si="4"/>
+        <v>-68740</v>
+      </c>
+      <c r="I55" s="51">
+        <f t="shared" si="4"/>
+        <v>-54700</v>
+      </c>
+      <c r="J55" s="51">
+        <f t="shared" si="4"/>
+        <v>-40660</v>
+      </c>
+      <c r="K55" s="51">
+        <f t="shared" si="4"/>
+        <v>-26620</v>
+      </c>
+      <c r="L55" s="51">
+        <f t="shared" si="4"/>
+        <v>-12580</v>
+      </c>
+      <c r="M55" s="51">
+        <f t="shared" si="4"/>
+        <v>1460</v>
+      </c>
+      <c r="N55" s="51">
+        <f t="shared" si="4"/>
+        <v>15500</v>
       </c>
     </row>
   </sheetData>
@@ -4508,12 +4605,12 @@
   </scenarios>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F46 F27:F28 F57:F65549 G2 G40 F39 G42 F41 D51:N51 H58:H65549 J45:J46 G28 F11:F13 G11:G21" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F44 F25:F26 F58:F65550 G2 G38 F37 G40 F39 D52:N52 H59:H65550 J43:J44 G26 F11 G11:G19" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>-10000000</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F45 G23:G27 G9 H2 F22:F26 G58:G65549 G39 F40 G41" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between (10,000,000) and 10,000,000." sqref="F14:F21 F29:F38 F11:F12" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F43 G21:G25 G9 H2 F20:F24 G59:G65550 G37 F38 G39" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between (10,000,000) and 10,000,000." sqref="F12:F19 F27:F36" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>-10000000</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
@@ -4578,13 +4675,13 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>19</xdr:row>
+                    <xdr:row>17</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>20</xdr:row>
+                    <xdr:row>18</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4600,13 +4697,13 @@
                   <from>
                     <xdr:col>6</xdr:col>
                     <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>17</xdr:row>
+                    <xdr:row>15</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </from>
                   <to>
                     <xdr:col>7</xdr:col>
                     <xdr:colOff>9525</xdr:colOff>
-                    <xdr:row>18</xdr:row>
+                    <xdr:row>16</xdr:row>
                     <xdr:rowOff>9525</xdr:rowOff>
                   </to>
                 </anchor>
@@ -4616,29 +4713,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1046" r:id="rId8" name="Scroll Bar 22">
-              <controlPr defaultSize="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>19050</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>790575</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1048" r:id="rId9" name="Scroll Bar 24">
+            <control shapeId="1048" r:id="rId8" name="Scroll Bar 24">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4660,7 +4735,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1050" r:id="rId10" name="Scroll Bar 26">
+            <control shapeId="1050" r:id="rId9" name="Scroll Bar 26">
               <controlPr defaultSize="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -4687,6 +4762,693 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00898D41-8ABF-4196-BA02-3A6610D1872A}">
+  <dimension ref="A1:Q33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G17" sqref="G17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="67" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="67"/>
+      <c r="D1" s="67"/>
+      <c r="E1" s="67"/>
+      <c r="F1" s="67"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" s="68" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="68" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+      <c r="P2" s="69"/>
+      <c r="Q2" s="69"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="69">
+        <v>1.34E-2</v>
+      </c>
+      <c r="C3" s="69">
+        <v>2.6800000000000001E-2</v>
+      </c>
+      <c r="D3" s="69"/>
+      <c r="E3" s="69"/>
+      <c r="F3" s="69"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="69"/>
+      <c r="J3" s="69"/>
+      <c r="K3" s="69"/>
+      <c r="L3" s="69"/>
+      <c r="M3" s="69"/>
+      <c r="N3" s="69"/>
+      <c r="O3" s="69"/>
+      <c r="P3" s="69"/>
+      <c r="Q3" s="69"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="68" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="70">
+        <v>18</v>
+      </c>
+      <c r="C4" s="70"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
+      <c r="H4" s="69"/>
+      <c r="I4" s="69"/>
+      <c r="J4" s="69"/>
+      <c r="K4" s="69"/>
+      <c r="L4" s="69"/>
+      <c r="M4" s="69"/>
+      <c r="N4" s="69"/>
+      <c r="O4" s="69"/>
+      <c r="P4" s="69"/>
+      <c r="Q4" s="69"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="68" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="70">
+        <v>6</v>
+      </c>
+      <c r="C5" s="70"/>
+      <c r="D5" s="69"/>
+      <c r="E5" s="69"/>
+      <c r="F5" s="69"/>
+      <c r="G5" s="69"/>
+      <c r="H5" s="69"/>
+      <c r="I5" s="69"/>
+      <c r="J5" s="69"/>
+      <c r="K5" s="69"/>
+      <c r="L5" s="69"/>
+      <c r="M5" s="69"/>
+      <c r="N5" s="69"/>
+      <c r="O5" s="69"/>
+      <c r="P5" s="69"/>
+      <c r="Q5" s="69"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="70">
+        <v>52</v>
+      </c>
+      <c r="C6" s="70"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
+      <c r="G6" s="69"/>
+      <c r="H6" s="69"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="69"/>
+      <c r="K6" s="69"/>
+      <c r="L6" s="69"/>
+      <c r="M6" s="69"/>
+      <c r="N6" s="69"/>
+      <c r="O6" s="69"/>
+      <c r="P6" s="69"/>
+      <c r="Q6" s="69"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="69"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="69"/>
+      <c r="D7" s="69"/>
+      <c r="E7" s="69"/>
+      <c r="F7" s="69"/>
+      <c r="G7" s="69"/>
+      <c r="H7" s="69"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="69"/>
+      <c r="K7" s="69"/>
+      <c r="L7" s="69"/>
+      <c r="M7" s="69"/>
+      <c r="N7" s="69"/>
+      <c r="O7" s="69"/>
+      <c r="P7" s="69"/>
+      <c r="Q7" s="69"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="69">
+        <f>B3*B4*B5*B6</f>
+        <v>75.254400000000004</v>
+      </c>
+      <c r="C8" s="69">
+        <f>C3*B4*B5*B6</f>
+        <v>150.50880000000001</v>
+      </c>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="G8" s="69"/>
+      <c r="H8" s="69"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="69"/>
+      <c r="K8" s="69"/>
+      <c r="L8" s="69"/>
+      <c r="M8" s="69"/>
+      <c r="N8" s="69"/>
+      <c r="O8" s="69"/>
+      <c r="P8" s="69"/>
+      <c r="Q8" s="69"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="71"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="69"/>
+      <c r="D9" s="69"/>
+      <c r="E9" s="69"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="69"/>
+      <c r="H9" s="69"/>
+      <c r="I9" s="69"/>
+      <c r="J9" s="69"/>
+      <c r="K9" s="69"/>
+      <c r="L9" s="69"/>
+      <c r="M9" s="69"/>
+      <c r="N9" s="69"/>
+      <c r="O9" s="69"/>
+      <c r="P9" s="69"/>
+      <c r="Q9" s="69"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="B10" s="70">
+        <v>1.2</v>
+      </c>
+      <c r="C10" s="70"/>
+      <c r="D10" s="69"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="69"/>
+      <c r="G10" s="69"/>
+      <c r="H10" s="69"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="69"/>
+      <c r="K10" s="69"/>
+      <c r="L10" s="69"/>
+      <c r="M10" s="69"/>
+      <c r="N10" s="69"/>
+      <c r="O10" s="69"/>
+      <c r="P10" s="69"/>
+      <c r="Q10" s="69"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="71" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="69">
+        <f>B8*B10</f>
+        <v>90.305279999999996</v>
+      </c>
+      <c r="C11" s="69">
+        <f>C8*B10</f>
+        <v>180.61055999999999</v>
+      </c>
+      <c r="D11" s="69"/>
+      <c r="E11" s="69"/>
+      <c r="F11" s="69"/>
+      <c r="G11" s="69"/>
+      <c r="H11" s="69"/>
+      <c r="I11" s="69"/>
+      <c r="J11" s="69"/>
+      <c r="K11" s="69"/>
+      <c r="L11" s="69"/>
+      <c r="M11" s="69"/>
+      <c r="N11" s="69"/>
+      <c r="O11" s="69"/>
+      <c r="P11" s="69"/>
+      <c r="Q11" s="69"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="69"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="69"/>
+      <c r="L12" s="69"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="69"/>
+      <c r="O12" s="69"/>
+      <c r="P12" s="69"/>
+      <c r="Q12" s="69"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="69"/>
+      <c r="B13" s="69"/>
+      <c r="C13" s="69"/>
+      <c r="D13" s="69"/>
+      <c r="E13" s="69"/>
+      <c r="F13" s="69"/>
+      <c r="G13" s="69"/>
+      <c r="H13" s="69"/>
+      <c r="I13" s="69"/>
+      <c r="J13" s="69"/>
+      <c r="K13" s="69"/>
+      <c r="L13" s="69"/>
+      <c r="M13" s="69"/>
+      <c r="N13" s="69"/>
+      <c r="O13" s="69"/>
+      <c r="P13" s="69"/>
+      <c r="Q13" s="69"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="69"/>
+      <c r="B14" s="69"/>
+      <c r="C14" s="69"/>
+      <c r="D14" s="69"/>
+      <c r="E14" s="69"/>
+      <c r="F14" s="69"/>
+      <c r="G14" s="69"/>
+      <c r="H14" s="69"/>
+      <c r="I14" s="69"/>
+      <c r="J14" s="69"/>
+      <c r="K14" s="69"/>
+      <c r="L14" s="69"/>
+      <c r="M14" s="69"/>
+      <c r="N14" s="69"/>
+      <c r="O14" s="69"/>
+      <c r="P14" s="69"/>
+      <c r="Q14" s="69"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="69"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="69"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
+      <c r="K15" s="69"/>
+      <c r="L15" s="69"/>
+      <c r="M15" s="69"/>
+      <c r="N15" s="69"/>
+      <c r="O15" s="69"/>
+      <c r="P15" s="69"/>
+      <c r="Q15" s="69"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="69"/>
+      <c r="B16" s="69"/>
+      <c r="C16" s="69"/>
+      <c r="D16" s="69"/>
+      <c r="E16" s="69"/>
+      <c r="F16" s="69"/>
+      <c r="G16" s="69"/>
+      <c r="H16" s="69"/>
+      <c r="I16" s="69"/>
+      <c r="J16" s="69"/>
+      <c r="K16" s="69"/>
+      <c r="L16" s="69"/>
+      <c r="M16" s="69"/>
+      <c r="N16" s="69"/>
+      <c r="O16" s="69"/>
+      <c r="P16" s="69"/>
+      <c r="Q16" s="69"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="69"/>
+      <c r="B17" s="69"/>
+      <c r="C17" s="69"/>
+      <c r="D17" s="69"/>
+      <c r="E17" s="69"/>
+      <c r="F17" s="69"/>
+      <c r="G17" s="69"/>
+      <c r="H17" s="69"/>
+      <c r="I17" s="69"/>
+      <c r="J17" s="69"/>
+      <c r="K17" s="69"/>
+      <c r="L17" s="69"/>
+      <c r="M17" s="69"/>
+      <c r="N17" s="69"/>
+      <c r="O17" s="69"/>
+      <c r="P17" s="69"/>
+      <c r="Q17" s="69"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A18" s="69"/>
+      <c r="B18" s="69"/>
+      <c r="C18" s="69"/>
+      <c r="D18" s="69"/>
+      <c r="E18" s="69"/>
+      <c r="F18" s="69"/>
+      <c r="G18" s="69"/>
+      <c r="H18" s="69"/>
+      <c r="I18" s="69"/>
+      <c r="J18" s="69"/>
+      <c r="K18" s="69"/>
+      <c r="L18" s="69"/>
+      <c r="M18" s="69"/>
+      <c r="N18" s="69"/>
+      <c r="O18" s="69"/>
+      <c r="P18" s="69"/>
+      <c r="Q18" s="69"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A19" s="69"/>
+      <c r="B19" s="69"/>
+      <c r="C19" s="69"/>
+      <c r="D19" s="69"/>
+      <c r="E19" s="69"/>
+      <c r="F19" s="69"/>
+      <c r="G19" s="69"/>
+      <c r="H19" s="69"/>
+      <c r="I19" s="69"/>
+      <c r="J19" s="69"/>
+      <c r="K19" s="69"/>
+      <c r="L19" s="69"/>
+      <c r="M19" s="69"/>
+      <c r="N19" s="69"/>
+      <c r="O19" s="69"/>
+      <c r="P19" s="69"/>
+      <c r="Q19" s="69"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A20" s="69"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="69"/>
+      <c r="D20" s="69"/>
+      <c r="E20" s="69"/>
+      <c r="F20" s="69"/>
+      <c r="G20" s="69"/>
+      <c r="H20" s="69"/>
+      <c r="I20" s="69"/>
+      <c r="J20" s="69"/>
+      <c r="K20" s="69"/>
+      <c r="L20" s="69"/>
+      <c r="M20" s="69"/>
+      <c r="N20" s="69"/>
+      <c r="O20" s="69"/>
+      <c r="P20" s="69"/>
+      <c r="Q20" s="69"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A21" s="69"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="69"/>
+      <c r="D21" s="69"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="69"/>
+      <c r="G21" s="69"/>
+      <c r="H21" s="69"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="69"/>
+      <c r="K21" s="69"/>
+      <c r="L21" s="69"/>
+      <c r="M21" s="69"/>
+      <c r="N21" s="69"/>
+      <c r="O21" s="69"/>
+      <c r="P21" s="69"/>
+      <c r="Q21" s="69"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A22" s="69"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="69"/>
+      <c r="D22" s="69"/>
+      <c r="E22" s="69"/>
+      <c r="F22" s="69"/>
+      <c r="G22" s="69"/>
+      <c r="H22" s="69"/>
+      <c r="I22" s="69"/>
+      <c r="J22" s="69"/>
+      <c r="K22" s="69"/>
+      <c r="L22" s="69"/>
+      <c r="M22" s="69"/>
+      <c r="N22" s="69"/>
+      <c r="O22" s="69"/>
+      <c r="P22" s="69"/>
+      <c r="Q22" s="69"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A23" s="69"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="69"/>
+      <c r="D23" s="69"/>
+      <c r="E23" s="69"/>
+      <c r="F23" s="69"/>
+      <c r="G23" s="69"/>
+      <c r="H23" s="69"/>
+      <c r="I23" s="69"/>
+      <c r="J23" s="69"/>
+      <c r="K23" s="69"/>
+      <c r="L23" s="69"/>
+      <c r="M23" s="69"/>
+      <c r="N23" s="69"/>
+      <c r="O23" s="69"/>
+      <c r="P23" s="69"/>
+      <c r="Q23" s="69"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A24" s="69"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="69"/>
+      <c r="J24" s="69"/>
+      <c r="K24" s="69"/>
+      <c r="L24" s="69"/>
+      <c r="M24" s="69"/>
+      <c r="N24" s="69"/>
+      <c r="O24" s="69"/>
+      <c r="P24" s="69"/>
+      <c r="Q24" s="69"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A25" s="69"/>
+      <c r="B25" s="69"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="69"/>
+      <c r="E25" s="69"/>
+      <c r="F25" s="69"/>
+      <c r="G25" s="69"/>
+      <c r="H25" s="69"/>
+      <c r="I25" s="69"/>
+      <c r="J25" s="69"/>
+      <c r="K25" s="69"/>
+      <c r="L25" s="69"/>
+      <c r="M25" s="69"/>
+      <c r="N25" s="69"/>
+      <c r="O25" s="69"/>
+      <c r="P25" s="69"/>
+      <c r="Q25" s="69"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A26" s="69"/>
+      <c r="B26" s="69"/>
+      <c r="C26" s="69"/>
+      <c r="D26" s="69"/>
+      <c r="E26" s="69"/>
+      <c r="F26" s="69"/>
+      <c r="G26" s="69"/>
+      <c r="H26" s="69"/>
+      <c r="I26" s="69"/>
+      <c r="J26" s="69"/>
+      <c r="K26" s="69"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="69"/>
+      <c r="N26" s="69"/>
+      <c r="O26" s="69"/>
+      <c r="P26" s="69"/>
+      <c r="Q26" s="69"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A27" s="69"/>
+      <c r="B27" s="69"/>
+      <c r="C27" s="69"/>
+      <c r="D27" s="69"/>
+      <c r="E27" s="69"/>
+      <c r="F27" s="69"/>
+      <c r="G27" s="69"/>
+      <c r="H27" s="69"/>
+      <c r="I27" s="69"/>
+      <c r="J27" s="69"/>
+      <c r="K27" s="69"/>
+      <c r="L27" s="69"/>
+      <c r="M27" s="69"/>
+      <c r="N27" s="69"/>
+      <c r="O27" s="69"/>
+      <c r="P27" s="69"/>
+      <c r="Q27" s="69"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A28" s="69"/>
+      <c r="B28" s="69"/>
+      <c r="C28" s="69"/>
+      <c r="D28" s="69"/>
+      <c r="E28" s="69"/>
+      <c r="F28" s="69"/>
+      <c r="G28" s="69"/>
+      <c r="H28" s="69"/>
+      <c r="I28" s="69"/>
+      <c r="J28" s="69"/>
+      <c r="K28" s="69"/>
+      <c r="L28" s="69"/>
+      <c r="M28" s="69"/>
+      <c r="N28" s="69"/>
+      <c r="O28" s="69"/>
+      <c r="P28" s="69"/>
+      <c r="Q28" s="69"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A29" s="69"/>
+      <c r="B29" s="69"/>
+      <c r="C29" s="69"/>
+      <c r="D29" s="69"/>
+      <c r="E29" s="69"/>
+      <c r="F29" s="69"/>
+      <c r="G29" s="69"/>
+      <c r="H29" s="69"/>
+      <c r="I29" s="69"/>
+      <c r="J29" s="69"/>
+      <c r="K29" s="69"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="69"/>
+      <c r="N29" s="69"/>
+      <c r="O29" s="69"/>
+      <c r="P29" s="69"/>
+      <c r="Q29" s="69"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A30" s="69"/>
+      <c r="B30" s="69"/>
+      <c r="C30" s="69"/>
+      <c r="D30" s="69"/>
+      <c r="E30" s="69"/>
+      <c r="F30" s="69"/>
+      <c r="G30" s="69"/>
+      <c r="H30" s="69"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="69"/>
+      <c r="M30" s="69"/>
+      <c r="N30" s="69"/>
+      <c r="O30" s="69"/>
+      <c r="P30" s="69"/>
+      <c r="Q30" s="69"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="69"/>
+      <c r="B31" s="69"/>
+      <c r="C31" s="69"/>
+      <c r="D31" s="69"/>
+      <c r="E31" s="69"/>
+      <c r="F31" s="69"/>
+      <c r="G31" s="69"/>
+      <c r="H31" s="69"/>
+      <c r="I31" s="69"/>
+      <c r="J31" s="69"/>
+      <c r="K31" s="69"/>
+      <c r="L31" s="69"/>
+      <c r="M31" s="69"/>
+      <c r="N31" s="69"/>
+      <c r="O31" s="69"/>
+      <c r="P31" s="69"/>
+      <c r="Q31" s="69"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32" s="69"/>
+      <c r="B32" s="69"/>
+      <c r="C32" s="69"/>
+      <c r="D32" s="69"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="69"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="69"/>
+      <c r="O32" s="69"/>
+      <c r="P32" s="69"/>
+      <c r="Q32" s="69"/>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A33" s="69"/>
+      <c r="B33" s="69"/>
+      <c r="C33" s="69"/>
+      <c r="D33" s="69"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="69"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="69"/>
+      <c r="O33" s="69"/>
+      <c r="P33" s="69"/>
+      <c r="Q33" s="69"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="B10:C10"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:B4"/>

</xml_diff>

<commit_message>
added SaaS hosting calculation. removed column below
</commit_message>
<xml_diff>
--- a/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
+++ b/Ontime/Administratie/Financiele analyse/breakeven-analysis OnTime.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" tabRatio="646" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" tabRatio="646" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Breakeven Analysis Data" sheetId="2" r:id="rId1"/>
@@ -169,7 +169,9 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Kost van 1 jaar servers te draaien</t>
+          <t>Kost van 1 jaar servers te draaien
+Zie sheet "Hosting cost"
+Lichte overschatting.</t>
         </r>
       </text>
     </comment>
@@ -210,17 +212,8 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Tuur:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
+          <t>Kosten van helpdesk.
+NIET aangerekend aan de klant</t>
         </r>
       </text>
     </comment>
@@ -260,9 +253,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Deze kost stijgt of daalt naar het aantal actieve klanten. Ruwe berekening (gebruikte hardware: Amazon EC2 t2.micro instance)
-Per active klant: 50 euro per periode
-Ook infrastructuur inbegrepen (computers werknemers, ISP, ...)</t>
+          <t>infrastructuur, (computers werknemers, ISP, ...)</t>
         </r>
       </text>
     </comment>
@@ -348,7 +339,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>_Example</t>
   </si>
@@ -512,9 +503,6 @@
     <t>Sales price per unit 500</t>
   </si>
   <si>
-    <t>Zie sheet "Hosting cost"</t>
-  </si>
-  <si>
     <t>Hosting Cost</t>
   </si>
   <si>
@@ -546,6 +534,12 @@
   </si>
   <si>
     <t>Dollar to Euro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved instance pricing, </t>
+  </si>
+  <si>
+    <t>Geen represantatief getal</t>
   </si>
 </sst>
 </file>
@@ -850,7 +844,7 @@
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="38" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="38" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -994,15 +988,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="40" fontId="0" fillId="3" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="38" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="38" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Date" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -1261,10 +1259,10 @@
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1700</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1400</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1563,7 +1561,10 @@
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>500</c:v>
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>100</c:v>
@@ -1572,7 +1573,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>500</c:v>
+                  <c:v>700</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -1856,10 +1857,10 @@
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1700</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1400</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2072,42 +2073,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$51:$N$51</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$51:$M$51</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>124900</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2158,42 +2156,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$53:$N$53</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$53:$M$53</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>124900</c:v>
+                  <c:v>116900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>129150</c:v>
+                  <c:v>119900</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>133400</c:v>
+                  <c:v>122900</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>137650</c:v>
+                  <c:v>125900</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>141900</c:v>
+                  <c:v>128900</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>146150</c:v>
+                  <c:v>131900</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>150400</c:v>
+                  <c:v>134900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>154650</c:v>
+                  <c:v>137900</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>158900</c:v>
+                  <c:v>140900</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>163150</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>167400</c:v>
+                  <c:v>143900</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2244,42 +2239,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$54:$N$54</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$54:$M$54</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>18290</c:v>
+                  <c:v>18150</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36580</c:v>
+                  <c:v>36300</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>54870</c:v>
+                  <c:v>54450</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>73160</c:v>
+                  <c:v>72600</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>91450</c:v>
+                  <c:v>90750</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>109740</c:v>
+                  <c:v>108900</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>128030</c:v>
+                  <c:v>127050</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>146320</c:v>
+                  <c:v>145200</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>164610</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>182900</c:v>
+                  <c:v>163350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2328,42 +2320,39 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>'Breakeven Analysis Data'!$D$55:$N$55</c:f>
+              <c:f>'Breakeven Analysis Data'!$D$55:$M$55</c:f>
               <c:numCache>
                 <c:formatCode>#,##0.00_);[Red]\(#,##0.00\)</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>-124900</c:v>
+                  <c:v>-116900</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-110860</c:v>
+                  <c:v>-101750</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-96820</c:v>
+                  <c:v>-86600</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-82780</c:v>
+                  <c:v>-71450</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-68740</c:v>
+                  <c:v>-56300</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-54700</c:v>
+                  <c:v>-41150</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-40660</c:v>
+                  <c:v>-26000</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-26620</c:v>
+                  <c:v>-10850</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-12580</c:v>
+                  <c:v>4300</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1460</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>15500</c:v>
+                  <c:v>19450</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2665,11 +2654,11 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" inc="100" max="10000" min="500" page="10" val="3100"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" inc="100" max="10000" min="500" page="10" val="3000"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$7" horiz="1" max="50" min="1" page="10" val="25"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$7" horiz="1" max="50" min="1" page="10" val="20"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2677,7 +2666,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$16" horiz="1" inc="50" max="1000" page="10" val="500"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$16" horiz="1" inc="50" max="1000" page="10" val="700"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2685,7 +2674,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp6.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$J$7" horiz="1" max="50" min="1" page="10" val="2"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$J$7" horiz="1" max="50" min="1" page="10" val="3"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2738,8 +2727,8 @@
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>318376</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>241300</xdr:rowOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>257175</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3466,10 +3455,10 @@
     <tabColor indexed="26"/>
     <pageSetUpPr autoPageBreaks="0" fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:M55"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" zoomScalePageLayoutView="145" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3542,7 +3531,7 @@
       </c>
       <c r="I4" s="14"/>
       <c r="J4" s="63">
-        <v>0.2</v>
+        <v>0.25</v>
       </c>
       <c r="K4" s="14"/>
     </row>
@@ -3573,16 +3562,16 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="58">
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="G6" s="7"/>
       <c r="H6" s="58">
         <f>Sales_price_unitA*(H5/F5)*(1-H4)</f>
-        <v>11160</v>
+        <v>10800</v>
       </c>
       <c r="J6" s="58">
         <f>Sales_price_unitA*(J5/F5)*(1-J4)</f>
-        <v>24800</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -3593,14 +3582,14 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="43">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="43">
         <v>5</v>
       </c>
       <c r="J7" s="43">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
@@ -3608,16 +3597,16 @@
       <c r="C8" s="12"/>
       <c r="F8" s="61">
         <f>IF(OR(Sales_price_unitA&lt;&gt;0,Sales_volume_unitsA&lt;&gt;0),Sales_price_unitA*Sales_volume_unitsA,0)</f>
-        <v>77500</v>
+        <v>60000</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="61">
         <f>IF(OR(Sales_price_unitB&lt;&gt;0,Sales_volume_unitsB&lt;&gt;0),Sales_price_unitB*Sales_volume_unitsB,0)</f>
-        <v>55800</v>
+        <v>54000</v>
       </c>
       <c r="J8" s="61">
         <f>IF(OR(Sales_price_unitC&lt;&gt;0,Sales_volume_unitsC&lt;&gt;0),Sales_price_unitC*Sales_volume_unitsC,0)</f>
-        <v>49600</v>
+        <v>67500</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -3627,7 +3616,7 @@
       </c>
       <c r="G9" s="59">
         <f>F8+H8+J8</f>
-        <v>182900</v>
+        <v>181500</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -3657,11 +3646,9 @@
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="30">
-        <v>500</v>
-      </c>
-      <c r="G12" s="55" t="s">
-        <v>54</v>
-      </c>
+        <v>100</v>
+      </c>
+      <c r="G12" s="55"/>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
@@ -3670,7 +3657,9 @@
         <v>29</v>
       </c>
       <c r="E13" s="3"/>
-      <c r="F13" s="30"/>
+      <c r="F13" s="30">
+        <v>0</v>
+      </c>
       <c r="G13" s="53"/>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -3705,7 +3694,7 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="30">
-        <v>500</v>
+        <v>700</v>
       </c>
       <c r="G16" s="53"/>
     </row>
@@ -3754,7 +3743,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="32">
         <f>IF(SUM(Variable_costs_unit),SUM(Variable_costs_unit),0)</f>
-        <v>1700</v>
+        <v>1500</v>
       </c>
       <c r="G20" s="54"/>
     </row>
@@ -3768,7 +3757,7 @@
       <c r="F21" s="18"/>
       <c r="G21" s="44">
         <f>IF(Variable_Unit_Cost,Variable_Unit_Cost*(Sales_volume_unitsA+Sales_volume_unitsB+Sales_volume_unitsC),0)</f>
-        <v>54400</v>
+        <v>42000</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -3789,7 +3778,7 @@
       <c r="E23" s="3"/>
       <c r="F23" s="31">
         <f>IF(Sales_price_unitA&gt;0,MAX(0,Sales_price_unitA-Variable_Unit_Cost),0)</f>
-        <v>1400</v>
+        <v>1500</v>
       </c>
       <c r="G23" s="18"/>
       <c r="H23" s="1"/>
@@ -3804,7 +3793,7 @@
       <c r="F24" s="18"/>
       <c r="G24" s="31">
         <f>IF(OR(Total_Sales&lt;&gt;0,Total_variable&lt;&gt;0),Total_Sales-Total_variable,0)</f>
-        <v>128500</v>
+        <v>139500</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -3864,7 +3853,7 @@
       </c>
       <c r="E29" s="3"/>
       <c r="F29" s="30">
-        <v>20000</v>
+        <v>15000</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
@@ -3908,7 +3897,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="11"/>
       <c r="C33" s="11" t="s">
@@ -3919,7 +3908,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" s="4"/>
       <c r="B34" s="11"/>
       <c r="C34" s="52" t="s">
@@ -3932,7 +3921,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="4"/>
       <c r="B35" s="11"/>
       <c r="C35" s="52" t="s">
@@ -3940,12 +3929,12 @@
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="48">
-        <v>15000</v>
+        <v>12000</v>
       </c>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="4"/>
       <c r="B36" s="11"/>
       <c r="C36" s="11" t="s">
@@ -3958,7 +3947,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="11"/>
       <c r="C37" s="33" t="s">
@@ -3968,18 +3957,18 @@
       <c r="F37" s="17"/>
       <c r="G37" s="46">
         <f>IF(SUM(Fixed_costs)&lt;&gt;0,SUM(Fixed_costs),0)</f>
-        <v>124900</v>
+        <v>116900</v>
       </c>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B38" s="34"/>
       <c r="C38" s="34"/>
       <c r="F38" s="17"/>
       <c r="G38" s="19"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="11"/>
       <c r="C39" s="33" t="s">
@@ -3988,21 +3977,21 @@
       <c r="E39" s="3"/>
       <c r="G39" s="47">
         <f>IF(OR(Gross_margin&lt;&gt;0,Total_fixed&lt;&gt;0),Gross_margin-Total_fixed,0)</f>
-        <v>3600</v>
+        <v>22600</v>
       </c>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B40" s="34"/>
       <c r="C40" s="34"/>
       <c r="G40" s="19"/>
     </row>
-    <row r="41" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
+    <row r="41" spans="1:13" ht="33.75" x14ac:dyDescent="0.65">
       <c r="B41" s="34"/>
       <c r="C41" s="34"/>
       <c r="F41" s="23"/>
     </row>
-    <row r="42" spans="1:14" ht="33.75" x14ac:dyDescent="0.65">
+    <row r="42" spans="1:13" ht="33.75" x14ac:dyDescent="0.65">
       <c r="B42" s="23" t="s">
         <v>13</v>
       </c>
@@ -4012,7 +4001,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B43" s="39" t="s">
         <v>12</v>
       </c>
@@ -4021,14 +4010,16 @@
       <c r="E43" s="25"/>
       <c r="F43" s="38">
         <f>IF(AND(Unit_contrib_margin&gt;0,Total_fixed&gt;0),Total_fixed/Unit_contrib_margin,"")</f>
-        <v>89.214285714285708</v>
-      </c>
-      <c r="G43" s="24"/>
+        <v>77.933333333333337</v>
+      </c>
+      <c r="G43" s="73" t="s">
+        <v>66</v>
+      </c>
       <c r="H43" s="25"/>
       <c r="I43" s="25"/>
       <c r="J43" s="26"/>
     </row>
-    <row r="44" spans="1:14" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B44" s="39" t="s">
         <v>19</v>
       </c>
@@ -4041,7 +4032,7 @@
       <c r="I44" s="25"/>
       <c r="J44" s="26"/>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B45" s="34" t="s">
         <v>48</v>
       </c>
@@ -4052,96 +4043,88 @@
       </c>
       <c r="E45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.1,0)</f>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="F45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.2,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.3,0)</f>
-        <v>7.5</v>
+        <v>6</v>
       </c>
       <c r="H45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.4,0)</f>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="I45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.5,0)</f>
-        <v>12.5</v>
+        <v>10</v>
       </c>
       <c r="J45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.6,0)</f>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="K45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.7,0)</f>
-        <v>17.5</v>
+        <v>14</v>
       </c>
       <c r="L45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.8,0)</f>
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="M45" s="35">
         <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA)*0.9,0)</f>
-        <v>22.5</v>
-      </c>
-      <c r="N45" s="35">
-        <f>IF(Sales_volume_unitsA,(Sales_volume_unitsA),0)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B46" s="34" t="s">
         <v>49</v>
       </c>
       <c r="C46" s="34"/>
       <c r="D46" s="36">
-        <f t="shared" ref="D46:N46" si="0">(Sales_price_unitA)</f>
-        <v>3100</v>
+        <f t="shared" ref="D46:M46" si="0">(Sales_price_unitA)</f>
+        <v>3000</v>
       </c>
       <c r="E46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="F46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="G46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="H46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="I46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="J46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="K46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="L46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>3000</v>
       </c>
       <c r="M46" s="36">
         <f t="shared" si="0"/>
-        <v>3100</v>
-      </c>
-      <c r="N46" s="36">
-        <f t="shared" si="0"/>
-        <v>3100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B47" s="34" t="s">
         <v>50</v>
       </c>
@@ -4186,62 +4169,54 @@
         <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB)*0.9,0)</f>
         <v>4.5</v>
       </c>
-      <c r="N47" s="35">
-        <f>IF(Sales_volume_unitsB,(Sales_volume_unitsB),0)</f>
-        <v>5</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B48" s="34" t="s">
         <v>51</v>
       </c>
       <c r="C48" s="34"/>
       <c r="D48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" ref="D48:M48" si="1">Sales_price_unitB</f>
+        <v>10800</v>
       </c>
       <c r="E48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" si="1"/>
+        <v>10800</v>
       </c>
       <c r="F48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" si="1"/>
+        <v>10800</v>
       </c>
       <c r="G48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" si="1"/>
+        <v>10800</v>
       </c>
       <c r="H48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" si="1"/>
+        <v>10800</v>
       </c>
       <c r="I48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" si="1"/>
+        <v>10800</v>
       </c>
       <c r="J48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" si="1"/>
+        <v>10800</v>
       </c>
       <c r="K48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" si="1"/>
+        <v>10800</v>
       </c>
       <c r="L48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
+        <f t="shared" si="1"/>
+        <v>10800</v>
       </c>
       <c r="M48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
-      </c>
-      <c r="N48" s="36">
-        <f>Sales_price_unitB</f>
-        <v>11160</v>
-      </c>
-    </row>
-    <row r="49" spans="2:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="1"/>
+        <v>10800</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B49" s="34" t="s">
         <v>52</v>
       </c>
@@ -4252,246 +4227,226 @@
       </c>
       <c r="E49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.1,0)</f>
-        <v>0.2</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="F49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.2,0)</f>
-        <v>0.4</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="G49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.3,0)</f>
-        <v>0.6</v>
+        <v>0.89999999999999991</v>
       </c>
       <c r="H49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.4,0)</f>
-        <v>0.8</v>
+        <v>1.2000000000000002</v>
       </c>
       <c r="I49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.5,0)</f>
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="J49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.6,0)</f>
-        <v>1.2</v>
+        <v>1.7999999999999998</v>
       </c>
       <c r="K49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.7,0)</f>
-        <v>1.4</v>
+        <v>2.0999999999999996</v>
       </c>
       <c r="L49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.8,0)</f>
-        <v>1.6</v>
+        <v>2.4000000000000004</v>
       </c>
       <c r="M49" s="35">
         <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC)*0.9,0)</f>
-        <v>1.8</v>
-      </c>
-      <c r="N49" s="35">
-        <f>IF(Sales_volume_unitsC,(Sales_volume_unitsC),0)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.2">
+        <v>2.7</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B50" s="34" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="34"/>
       <c r="D50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" ref="D50:M50" si="2">Sales_price_unitC</f>
+        <v>22500</v>
       </c>
       <c r="E50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" si="2"/>
+        <v>22500</v>
       </c>
       <c r="F50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" si="2"/>
+        <v>22500</v>
       </c>
       <c r="G50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" si="2"/>
+        <v>22500</v>
       </c>
       <c r="H50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" si="2"/>
+        <v>22500</v>
       </c>
       <c r="I50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" si="2"/>
+        <v>22500</v>
       </c>
       <c r="J50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" si="2"/>
+        <v>22500</v>
       </c>
       <c r="K50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" si="2"/>
+        <v>22500</v>
       </c>
       <c r="L50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
+        <f t="shared" si="2"/>
+        <v>22500</v>
       </c>
       <c r="M50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
-      </c>
-      <c r="N50" s="66">
-        <f>Sales_price_unitC</f>
-        <v>24800</v>
-      </c>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="2"/>
+        <v>22500</v>
+      </c>
+    </row>
+    <row r="51" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B51" s="34" t="s">
         <v>25</v>
       </c>
       <c r="C51" s="34"/>
       <c r="D51" s="36">
-        <f t="shared" ref="D51:N51" si="1">Total_fixed</f>
-        <v>124900</v>
+        <f t="shared" ref="D51:M51" si="3">Total_fixed</f>
+        <v>116900</v>
       </c>
       <c r="E51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
+        <f t="shared" si="3"/>
+        <v>116900</v>
       </c>
       <c r="F51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
+        <f t="shared" si="3"/>
+        <v>116900</v>
       </c>
       <c r="G51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
+        <f t="shared" si="3"/>
+        <v>116900</v>
       </c>
       <c r="H51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
+        <f t="shared" si="3"/>
+        <v>116900</v>
       </c>
       <c r="I51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
+        <f t="shared" si="3"/>
+        <v>116900</v>
       </c>
       <c r="J51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
+        <f t="shared" si="3"/>
+        <v>116900</v>
       </c>
       <c r="K51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
+        <f t="shared" si="3"/>
+        <v>116900</v>
       </c>
       <c r="L51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
+        <f t="shared" si="3"/>
+        <v>116900</v>
       </c>
       <c r="M51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
-      </c>
-      <c r="N51" s="36">
-        <f t="shared" si="1"/>
-        <v>124900</v>
-      </c>
-    </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="3"/>
+        <v>116900</v>
+      </c>
+    </row>
+    <row r="52" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B52" s="37" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="37"/>
       <c r="D52" s="36">
-        <f>Variable_Unit_Cost*D45</f>
+        <f t="shared" ref="D52:M52" si="4">Variable_Unit_Cost*D45</f>
         <v>0</v>
       </c>
       <c r="E52" s="36">
-        <f>Variable_Unit_Cost*E45</f>
-        <v>4250</v>
+        <f t="shared" si="4"/>
+        <v>3000</v>
       </c>
       <c r="F52" s="36">
-        <f>Variable_Unit_Cost*F45</f>
-        <v>8500</v>
+        <f t="shared" si="4"/>
+        <v>6000</v>
       </c>
       <c r="G52" s="36">
-        <f>Variable_Unit_Cost*G45</f>
-        <v>12750</v>
+        <f t="shared" si="4"/>
+        <v>9000</v>
       </c>
       <c r="H52" s="36">
-        <f>Variable_Unit_Cost*H45</f>
-        <v>17000</v>
+        <f t="shared" si="4"/>
+        <v>12000</v>
       </c>
       <c r="I52" s="36">
-        <f>Variable_Unit_Cost*I45</f>
-        <v>21250</v>
+        <f t="shared" si="4"/>
+        <v>15000</v>
       </c>
       <c r="J52" s="36">
-        <f>Variable_Unit_Cost*J45</f>
-        <v>25500</v>
+        <f t="shared" si="4"/>
+        <v>18000</v>
       </c>
       <c r="K52" s="36">
-        <f>Variable_Unit_Cost*K45</f>
-        <v>29750</v>
+        <f t="shared" si="4"/>
+        <v>21000</v>
       </c>
       <c r="L52" s="36">
-        <f>Variable_Unit_Cost*L45</f>
-        <v>34000</v>
+        <f t="shared" si="4"/>
+        <v>24000</v>
       </c>
       <c r="M52" s="36">
-        <f>Variable_Unit_Cost*M45</f>
-        <v>38250</v>
-      </c>
-      <c r="N52" s="36">
-        <f>Variable_Unit_Cost*N45</f>
-        <v>42500</v>
-      </c>
-    </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="4"/>
+        <v>27000</v>
+      </c>
+    </row>
+    <row r="53" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B53" s="37" t="s">
         <v>17</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="36">
         <f>SUM(D51:D52)</f>
-        <v>124900</v>
+        <v>116900</v>
       </c>
       <c r="E53" s="36">
-        <f t="shared" ref="E53:N53" si="2">SUM(E51:E52)</f>
-        <v>129150</v>
+        <f t="shared" ref="E53:M53" si="5">SUM(E51:E52)</f>
+        <v>119900</v>
       </c>
       <c r="F53" s="36">
-        <f t="shared" si="2"/>
-        <v>133400</v>
+        <f t="shared" si="5"/>
+        <v>122900</v>
       </c>
       <c r="G53" s="36">
-        <f t="shared" si="2"/>
-        <v>137650</v>
+        <f t="shared" si="5"/>
+        <v>125900</v>
       </c>
       <c r="H53" s="36">
-        <f t="shared" si="2"/>
-        <v>141900</v>
+        <f t="shared" si="5"/>
+        <v>128900</v>
       </c>
       <c r="I53" s="36">
-        <f t="shared" si="2"/>
-        <v>146150</v>
+        <f t="shared" si="5"/>
+        <v>131900</v>
       </c>
       <c r="J53" s="36">
-        <f t="shared" si="2"/>
-        <v>150400</v>
+        <f t="shared" si="5"/>
+        <v>134900</v>
       </c>
       <c r="K53" s="36">
-        <f t="shared" si="2"/>
-        <v>154650</v>
+        <f t="shared" si="5"/>
+        <v>137900</v>
       </c>
       <c r="L53" s="36">
-        <f t="shared" si="2"/>
-        <v>158900</v>
+        <f t="shared" si="5"/>
+        <v>140900</v>
       </c>
       <c r="M53" s="36">
-        <f t="shared" si="2"/>
-        <v>163150</v>
-      </c>
-      <c r="N53" s="36">
-        <f t="shared" si="2"/>
-        <v>167400</v>
-      </c>
-    </row>
-    <row r="54" spans="2:14" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>143900</v>
+      </c>
+    </row>
+    <row r="54" spans="2:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B54" s="34" t="s">
         <v>16</v>
       </c>
@@ -4501,94 +4456,86 @@
         <v>0</v>
       </c>
       <c r="E54" s="50">
-        <f t="shared" ref="E54:N54" si="3">((E46*E45)+(E47*E48)+(E49*E50))</f>
-        <v>18290</v>
+        <f t="shared" ref="E54:M54" si="6">((E46*E45)+(E47*E48)+(E49*E50))</f>
+        <v>18150</v>
       </c>
       <c r="F54" s="50">
-        <f t="shared" si="3"/>
-        <v>36580</v>
+        <f t="shared" si="6"/>
+        <v>36300</v>
       </c>
       <c r="G54" s="50">
-        <f t="shared" si="3"/>
-        <v>54870</v>
+        <f t="shared" si="6"/>
+        <v>54450</v>
       </c>
       <c r="H54" s="50">
-        <f t="shared" si="3"/>
-        <v>73160</v>
+        <f t="shared" si="6"/>
+        <v>72600</v>
       </c>
       <c r="I54" s="50">
-        <f t="shared" si="3"/>
-        <v>91450</v>
+        <f t="shared" si="6"/>
+        <v>90750</v>
       </c>
       <c r="J54" s="50">
-        <f t="shared" si="3"/>
-        <v>109740</v>
+        <f t="shared" si="6"/>
+        <v>108900</v>
       </c>
       <c r="K54" s="50">
-        <f t="shared" si="3"/>
-        <v>128030</v>
+        <f t="shared" si="6"/>
+        <v>127050</v>
       </c>
       <c r="L54" s="50">
-        <f t="shared" si="3"/>
-        <v>146320</v>
+        <f t="shared" si="6"/>
+        <v>145200</v>
       </c>
       <c r="M54" s="50">
-        <f t="shared" si="3"/>
-        <v>164610</v>
-      </c>
-      <c r="N54" s="50">
-        <f t="shared" si="3"/>
-        <v>182900</v>
-      </c>
-    </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.2">
+        <f t="shared" si="6"/>
+        <v>163350</v>
+      </c>
+    </row>
+    <row r="55" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B55" s="37" t="s">
         <v>18</v>
       </c>
       <c r="C55" s="37"/>
       <c r="D55" s="51">
         <f>D54-D53</f>
-        <v>-124900</v>
+        <v>-116900</v>
       </c>
       <c r="E55" s="51">
-        <f t="shared" ref="E55:N55" si="4">E54-E53</f>
-        <v>-110860</v>
+        <f t="shared" ref="E55:M55" si="7">E54-E53</f>
+        <v>-101750</v>
       </c>
       <c r="F55" s="51">
-        <f t="shared" si="4"/>
-        <v>-96820</v>
+        <f t="shared" si="7"/>
+        <v>-86600</v>
       </c>
       <c r="G55" s="51">
-        <f t="shared" si="4"/>
-        <v>-82780</v>
+        <f t="shared" si="7"/>
+        <v>-71450</v>
       </c>
       <c r="H55" s="51">
-        <f t="shared" si="4"/>
-        <v>-68740</v>
+        <f t="shared" si="7"/>
+        <v>-56300</v>
       </c>
       <c r="I55" s="51">
-        <f t="shared" si="4"/>
-        <v>-54700</v>
+        <f t="shared" si="7"/>
+        <v>-41150</v>
       </c>
       <c r="J55" s="51">
-        <f t="shared" si="4"/>
-        <v>-40660</v>
+        <f t="shared" si="7"/>
+        <v>-26000</v>
       </c>
       <c r="K55" s="51">
-        <f t="shared" si="4"/>
-        <v>-26620</v>
+        <f t="shared" si="7"/>
+        <v>-10850</v>
       </c>
       <c r="L55" s="51">
-        <f t="shared" si="4"/>
-        <v>-12580</v>
+        <f t="shared" si="7"/>
+        <v>4300</v>
       </c>
       <c r="M55" s="51">
-        <f t="shared" si="4"/>
-        <v>1460</v>
-      </c>
-      <c r="N55" s="51">
-        <f t="shared" si="4"/>
-        <v>15500</v>
+        <f t="shared" si="7"/>
+        <v>19450</v>
       </c>
     </row>
   </sheetData>
@@ -4605,7 +4552,7 @@
   </scenarios>
   <phoneticPr fontId="0" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F44 F25:F26 F58:F65550 G2 G38 F37 G40 F39 D52:N52 H59:H65550 J43:J44 G26 F11 G11:G19" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Please enter an amount between -10,000,000 and 10,000,000." sqref="F44 F25:F26 F58:F65550 G2 G38 F37 G40 F39 D52:M52 H59:H65550 J43:J44 G26 F11 G11:G19" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>-10000000</formula1>
       <formula2>10000000</formula2>
     </dataValidation>
@@ -4763,10 +4710,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00898D41-8ABF-4196-BA02-3A6610D1872A}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4775,674 +4722,696 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="67" t="s">
+      <c r="A1" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="D1" s="67"/>
-      <c r="E1" s="67"/>
-      <c r="F1" s="67"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="68" t="s">
+      <c r="B2" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+      <c r="H2" s="68"/>
+      <c r="I2" s="68"/>
+      <c r="J2" s="68"/>
+      <c r="K2" s="68"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="72"/>
+      <c r="C3" s="72"/>
+      <c r="D3" s="72"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="68"/>
+      <c r="H3" s="68"/>
+      <c r="I3" s="68"/>
+      <c r="J3" s="68"/>
+      <c r="K3" s="68"/>
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="67" t="s">
         <v>58</v>
       </c>
-      <c r="C2" s="68" t="s">
-        <v>57</v>
-      </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="68" t="s">
+      <c r="B4" s="68">
+        <v>1.4E-2</v>
+      </c>
+      <c r="C4" s="68">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D4" s="68"/>
+      <c r="E4" s="68"/>
+      <c r="F4" s="68"/>
+      <c r="G4" s="68"/>
+      <c r="H4" s="68"/>
+      <c r="I4" s="68"/>
+      <c r="J4" s="68"/>
+      <c r="K4" s="68"/>
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="69">
-        <v>1.34E-2</v>
-      </c>
-      <c r="C3" s="69">
-        <v>2.6800000000000001E-2</v>
-      </c>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="69"/>
-      <c r="H3" s="69"/>
-      <c r="I3" s="69"/>
-      <c r="J3" s="69"/>
-      <c r="K3" s="69"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="68" t="s">
+      <c r="B5" s="71">
+        <v>12</v>
+      </c>
+      <c r="C5" s="71"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
+      <c r="L5" s="68"/>
+      <c r="M5" s="68"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="68"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="67" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="70">
-        <v>18</v>
-      </c>
-      <c r="C4" s="70"/>
-      <c r="D4" s="69"/>
-      <c r="E4" s="69"/>
-      <c r="F4" s="69"/>
-      <c r="G4" s="69"/>
-      <c r="H4" s="69"/>
-      <c r="I4" s="69"/>
-      <c r="J4" s="69"/>
-      <c r="K4" s="69"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="68" t="s">
+      <c r="B6" s="71">
+        <v>6</v>
+      </c>
+      <c r="C6" s="71"/>
+      <c r="D6" s="68"/>
+      <c r="E6" s="68"/>
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="68"/>
+      <c r="J6" s="68"/>
+      <c r="K6" s="68"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="68"/>
+      <c r="O6" s="68"/>
+      <c r="P6" s="68"/>
+      <c r="Q6" s="68"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="71">
+        <v>52</v>
+      </c>
+      <c r="C7" s="71"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="68"/>
+      <c r="F7" s="68"/>
+      <c r="G7" s="68"/>
+      <c r="H7" s="68"/>
+      <c r="I7" s="68"/>
+      <c r="J7" s="68"/>
+      <c r="K7" s="68"/>
+      <c r="L7" s="68"/>
+      <c r="M7" s="68"/>
+      <c r="N7" s="68"/>
+      <c r="O7" s="68"/>
+      <c r="P7" s="68"/>
+      <c r="Q7" s="68"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="68"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="68"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="68"/>
+      <c r="J8" s="68"/>
+      <c r="K8" s="68"/>
+      <c r="L8" s="68"/>
+      <c r="M8" s="68"/>
+      <c r="N8" s="68"/>
+      <c r="O8" s="68"/>
+      <c r="P8" s="68"/>
+      <c r="Q8" s="68"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="B5" s="70">
-        <v>6</v>
-      </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="69"/>
-      <c r="E5" s="69"/>
-      <c r="F5" s="69"/>
-      <c r="G5" s="69"/>
-      <c r="H5" s="69"/>
-      <c r="I5" s="69"/>
-      <c r="J5" s="69"/>
-      <c r="K5" s="69"/>
-      <c r="L5" s="69"/>
-      <c r="M5" s="69"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="68" t="s">
+      <c r="B9" s="68">
+        <f>B4*B5*B6*B7</f>
+        <v>52.415999999999997</v>
+      </c>
+      <c r="C9" s="68">
+        <f>C4*B5*B6*B7</f>
+        <v>104.83199999999999</v>
+      </c>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="68"/>
+      <c r="K9" s="68"/>
+      <c r="L9" s="68"/>
+      <c r="M9" s="68"/>
+      <c r="N9" s="68"/>
+      <c r="O9" s="68"/>
+      <c r="P9" s="68"/>
+      <c r="Q9" s="68"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="69"/>
+      <c r="B10" s="68"/>
+      <c r="C10" s="68"/>
+      <c r="D10" s="68"/>
+      <c r="E10" s="68"/>
+      <c r="F10" s="68"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="68"/>
+      <c r="J10" s="68"/>
+      <c r="K10" s="68"/>
+      <c r="L10" s="68"/>
+      <c r="M10" s="68"/>
+      <c r="N10" s="68"/>
+      <c r="O10" s="68"/>
+      <c r="P10" s="68"/>
+      <c r="Q10" s="68"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="69" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="71">
+        <v>1.2</v>
+      </c>
+      <c r="C11" s="71"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="68"/>
+      <c r="F11" s="68"/>
+      <c r="G11" s="68"/>
+      <c r="H11" s="68"/>
+      <c r="I11" s="68"/>
+      <c r="J11" s="68"/>
+      <c r="K11" s="68"/>
+      <c r="L11" s="68"/>
+      <c r="M11" s="68"/>
+      <c r="N11" s="68"/>
+      <c r="O11" s="68"/>
+      <c r="P11" s="68"/>
+      <c r="Q11" s="68"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="69" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="70">
-        <v>52</v>
-      </c>
-      <c r="C6" s="70"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="69"/>
-      <c r="H6" s="69"/>
-      <c r="I6" s="69"/>
-      <c r="J6" s="69"/>
-      <c r="K6" s="69"/>
-      <c r="L6" s="69"/>
-      <c r="M6" s="69"/>
-      <c r="N6" s="69"/>
-      <c r="O6" s="69"/>
-      <c r="P6" s="69"/>
-      <c r="Q6" s="69"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="69"/>
-      <c r="B7" s="69"/>
-      <c r="C7" s="69"/>
-      <c r="D7" s="69"/>
-      <c r="E7" s="69"/>
-      <c r="F7" s="69"/>
-      <c r="G7" s="69"/>
-      <c r="H7" s="69"/>
-      <c r="I7" s="69"/>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-      <c r="L7" s="69"/>
-      <c r="M7" s="69"/>
-      <c r="N7" s="69"/>
-      <c r="O7" s="69"/>
-      <c r="P7" s="69"/>
-      <c r="Q7" s="69"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="71" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8" s="69">
-        <f>B3*B4*B5*B6</f>
-        <v>75.254400000000004</v>
-      </c>
-      <c r="C8" s="69">
-        <f>C3*B4*B5*B6</f>
-        <v>150.50880000000001</v>
-      </c>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="69"/>
-      <c r="H8" s="69"/>
-      <c r="I8" s="69"/>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
-      <c r="L8" s="69"/>
-      <c r="M8" s="69"/>
-      <c r="N8" s="69"/>
-      <c r="O8" s="69"/>
-      <c r="P8" s="69"/>
-      <c r="Q8" s="69"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="71"/>
-      <c r="B9" s="69"/>
-      <c r="C9" s="69"/>
-      <c r="D9" s="69"/>
-      <c r="E9" s="69"/>
-      <c r="F9" s="69"/>
-      <c r="G9" s="69"/>
-      <c r="H9" s="69"/>
-      <c r="I9" s="69"/>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
-      <c r="L9" s="69"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="69"/>
-      <c r="O9" s="69"/>
-      <c r="P9" s="69"/>
-      <c r="Q9" s="69"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="71" t="s">
-        <v>65</v>
-      </c>
-      <c r="B10" s="70">
-        <v>1.2</v>
-      </c>
-      <c r="C10" s="70"/>
-      <c r="D10" s="69"/>
-      <c r="E10" s="69"/>
-      <c r="F10" s="69"/>
-      <c r="G10" s="69"/>
-      <c r="H10" s="69"/>
-      <c r="I10" s="69"/>
-      <c r="J10" s="69"/>
-      <c r="K10" s="69"/>
-      <c r="L10" s="69"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="69"/>
-      <c r="O10" s="69"/>
-      <c r="P10" s="69"/>
-      <c r="Q10" s="69"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="71" t="s">
-        <v>64</v>
-      </c>
-      <c r="B11" s="69">
-        <f>B8*B10</f>
-        <v>90.305279999999996</v>
-      </c>
-      <c r="C11" s="69">
-        <f>C8*B10</f>
-        <v>180.61055999999999</v>
-      </c>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="69"/>
-      <c r="K11" s="69"/>
-      <c r="L11" s="69"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="69"/>
-      <c r="O11" s="69"/>
-      <c r="P11" s="69"/>
-      <c r="Q11" s="69"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="69"/>
-      <c r="B12" s="69"/>
-      <c r="C12" s="69"/>
-      <c r="D12" s="69"/>
-      <c r="E12" s="69"/>
-      <c r="F12" s="69"/>
-      <c r="G12" s="69"/>
-      <c r="H12" s="69"/>
-      <c r="I12" s="69"/>
-      <c r="J12" s="69"/>
-      <c r="K12" s="69"/>
-      <c r="L12" s="69"/>
-      <c r="M12" s="69"/>
-      <c r="N12" s="69"/>
-      <c r="O12" s="69"/>
-      <c r="P12" s="69"/>
-      <c r="Q12" s="69"/>
+      <c r="B12" s="68">
+        <f>B9*B11</f>
+        <v>62.899199999999993</v>
+      </c>
+      <c r="C12" s="68">
+        <f>C9*B11</f>
+        <v>125.79839999999999</v>
+      </c>
+      <c r="D12" s="68"/>
+      <c r="E12" s="68"/>
+      <c r="F12" s="68"/>
+      <c r="G12" s="68"/>
+      <c r="H12" s="68"/>
+      <c r="I12" s="68"/>
+      <c r="J12" s="68"/>
+      <c r="K12" s="68"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="68"/>
+      <c r="N12" s="68"/>
+      <c r="O12" s="68"/>
+      <c r="P12" s="68"/>
+      <c r="Q12" s="68"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A13" s="69"/>
-      <c r="B13" s="69"/>
-      <c r="C13" s="69"/>
-      <c r="D13" s="69"/>
-      <c r="E13" s="69"/>
-      <c r="F13" s="69"/>
-      <c r="G13" s="69"/>
-      <c r="H13" s="69"/>
-      <c r="I13" s="69"/>
-      <c r="J13" s="69"/>
-      <c r="K13" s="69"/>
-      <c r="L13" s="69"/>
-      <c r="M13" s="69"/>
-      <c r="N13" s="69"/>
-      <c r="O13" s="69"/>
-      <c r="P13" s="69"/>
-      <c r="Q13" s="69"/>
+      <c r="A13" s="68"/>
+      <c r="B13" s="68"/>
+      <c r="C13" s="68"/>
+      <c r="D13" s="68"/>
+      <c r="E13" s="68"/>
+      <c r="F13" s="68"/>
+      <c r="G13" s="68"/>
+      <c r="H13" s="68"/>
+      <c r="I13" s="68"/>
+      <c r="J13" s="68"/>
+      <c r="K13" s="68"/>
+      <c r="L13" s="68"/>
+      <c r="M13" s="68"/>
+      <c r="N13" s="68"/>
+      <c r="O13" s="68"/>
+      <c r="P13" s="68"/>
+      <c r="Q13" s="68"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A14" s="69"/>
-      <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="69"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
-      <c r="K14" s="69"/>
-      <c r="L14" s="69"/>
-      <c r="M14" s="69"/>
-      <c r="N14" s="69"/>
-      <c r="O14" s="69"/>
-      <c r="P14" s="69"/>
-      <c r="Q14" s="69"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
+      <c r="H14" s="68"/>
+      <c r="I14" s="68"/>
+      <c r="J14" s="68"/>
+      <c r="K14" s="68"/>
+      <c r="L14" s="68"/>
+      <c r="M14" s="68"/>
+      <c r="N14" s="68"/>
+      <c r="O14" s="68"/>
+      <c r="P14" s="68"/>
+      <c r="Q14" s="68"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="69"/>
-      <c r="B15" s="69"/>
-      <c r="C15" s="69"/>
-      <c r="D15" s="69"/>
-      <c r="E15" s="69"/>
-      <c r="F15" s="69"/>
-      <c r="G15" s="69"/>
-      <c r="H15" s="69"/>
-      <c r="I15" s="69"/>
-      <c r="J15" s="69"/>
-      <c r="K15" s="69"/>
-      <c r="L15" s="69"/>
-      <c r="M15" s="69"/>
-      <c r="N15" s="69"/>
-      <c r="O15" s="69"/>
-      <c r="P15" s="69"/>
-      <c r="Q15" s="69"/>
+      <c r="A15" s="68"/>
+      <c r="B15" s="68"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="68"/>
+      <c r="O15" s="68"/>
+      <c r="P15" s="68"/>
+      <c r="Q15" s="68"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A16" s="69"/>
-      <c r="B16" s="69"/>
-      <c r="C16" s="69"/>
-      <c r="D16" s="69"/>
-      <c r="E16" s="69"/>
-      <c r="F16" s="69"/>
-      <c r="G16" s="69"/>
-      <c r="H16" s="69"/>
-      <c r="I16" s="69"/>
-      <c r="J16" s="69"/>
-      <c r="K16" s="69"/>
-      <c r="L16" s="69"/>
-      <c r="M16" s="69"/>
-      <c r="N16" s="69"/>
-      <c r="O16" s="69"/>
-      <c r="P16" s="69"/>
-      <c r="Q16" s="69"/>
+      <c r="A16" s="68"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="68"/>
+      <c r="D16" s="68"/>
+      <c r="E16" s="68"/>
+      <c r="F16" s="68"/>
+      <c r="G16" s="68"/>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="68"/>
+      <c r="P16" s="68"/>
+      <c r="Q16" s="68"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A17" s="69"/>
-      <c r="B17" s="69"/>
-      <c r="C17" s="69"/>
-      <c r="D17" s="69"/>
-      <c r="E17" s="69"/>
-      <c r="F17" s="69"/>
-      <c r="G17" s="69"/>
-      <c r="H17" s="69"/>
-      <c r="I17" s="69"/>
-      <c r="J17" s="69"/>
-      <c r="K17" s="69"/>
-      <c r="L17" s="69"/>
-      <c r="M17" s="69"/>
-      <c r="N17" s="69"/>
-      <c r="O17" s="69"/>
-      <c r="P17" s="69"/>
-      <c r="Q17" s="69"/>
+      <c r="A17" s="68"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="68"/>
+      <c r="D17" s="68"/>
+      <c r="E17" s="68"/>
+      <c r="F17" s="68"/>
+      <c r="G17" s="68"/>
+      <c r="H17" s="68"/>
+      <c r="I17" s="68"/>
+      <c r="J17" s="68"/>
+      <c r="K17" s="68"/>
+      <c r="L17" s="68"/>
+      <c r="M17" s="68"/>
+      <c r="N17" s="68"/>
+      <c r="O17" s="68"/>
+      <c r="P17" s="68"/>
+      <c r="Q17" s="68"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A18" s="69"/>
-      <c r="B18" s="69"/>
-      <c r="C18" s="69"/>
-      <c r="D18" s="69"/>
-      <c r="E18" s="69"/>
-      <c r="F18" s="69"/>
-      <c r="G18" s="69"/>
-      <c r="H18" s="69"/>
-      <c r="I18" s="69"/>
-      <c r="J18" s="69"/>
-      <c r="K18" s="69"/>
-      <c r="L18" s="69"/>
-      <c r="M18" s="69"/>
-      <c r="N18" s="69"/>
-      <c r="O18" s="69"/>
-      <c r="P18" s="69"/>
-      <c r="Q18" s="69"/>
+      <c r="A18" s="68"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="68"/>
+      <c r="E18" s="68"/>
+      <c r="F18" s="68"/>
+      <c r="G18" s="68"/>
+      <c r="H18" s="68"/>
+      <c r="I18" s="68"/>
+      <c r="J18" s="68"/>
+      <c r="K18" s="68"/>
+      <c r="L18" s="68"/>
+      <c r="M18" s="68"/>
+      <c r="N18" s="68"/>
+      <c r="O18" s="68"/>
+      <c r="P18" s="68"/>
+      <c r="Q18" s="68"/>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A19" s="69"/>
-      <c r="B19" s="69"/>
-      <c r="C19" s="69"/>
-      <c r="D19" s="69"/>
-      <c r="E19" s="69"/>
-      <c r="F19" s="69"/>
-      <c r="G19" s="69"/>
-      <c r="H19" s="69"/>
-      <c r="I19" s="69"/>
-      <c r="J19" s="69"/>
-      <c r="K19" s="69"/>
-      <c r="L19" s="69"/>
-      <c r="M19" s="69"/>
-      <c r="N19" s="69"/>
-      <c r="O19" s="69"/>
-      <c r="P19" s="69"/>
-      <c r="Q19" s="69"/>
+      <c r="A19" s="68"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="68"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="68"/>
+      <c r="H19" s="68"/>
+      <c r="I19" s="68"/>
+      <c r="J19" s="68"/>
+      <c r="K19" s="68"/>
+      <c r="L19" s="68"/>
+      <c r="M19" s="68"/>
+      <c r="N19" s="68"/>
+      <c r="O19" s="68"/>
+      <c r="P19" s="68"/>
+      <c r="Q19" s="68"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A20" s="69"/>
-      <c r="B20" s="69"/>
-      <c r="C20" s="69"/>
-      <c r="D20" s="69"/>
-      <c r="E20" s="69"/>
-      <c r="F20" s="69"/>
-      <c r="G20" s="69"/>
-      <c r="H20" s="69"/>
-      <c r="I20" s="69"/>
-      <c r="J20" s="69"/>
-      <c r="K20" s="69"/>
-      <c r="L20" s="69"/>
-      <c r="M20" s="69"/>
-      <c r="N20" s="69"/>
-      <c r="O20" s="69"/>
-      <c r="P20" s="69"/>
-      <c r="Q20" s="69"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="68"/>
+      <c r="H20" s="68"/>
+      <c r="I20" s="68"/>
+      <c r="J20" s="68"/>
+      <c r="K20" s="68"/>
+      <c r="L20" s="68"/>
+      <c r="M20" s="68"/>
+      <c r="N20" s="68"/>
+      <c r="O20" s="68"/>
+      <c r="P20" s="68"/>
+      <c r="Q20" s="68"/>
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A21" s="69"/>
-      <c r="B21" s="69"/>
-      <c r="C21" s="69"/>
-      <c r="D21" s="69"/>
-      <c r="E21" s="69"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="69"/>
-      <c r="H21" s="69"/>
-      <c r="I21" s="69"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="69"/>
-      <c r="L21" s="69"/>
-      <c r="M21" s="69"/>
-      <c r="N21" s="69"/>
-      <c r="O21" s="69"/>
-      <c r="P21" s="69"/>
-      <c r="Q21" s="69"/>
+      <c r="A21" s="68"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="68"/>
+      <c r="J21" s="68"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="68"/>
+      <c r="N21" s="68"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="68"/>
+      <c r="Q21" s="68"/>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A22" s="69"/>
-      <c r="B22" s="69"/>
-      <c r="C22" s="69"/>
-      <c r="D22" s="69"/>
-      <c r="E22" s="69"/>
-      <c r="F22" s="69"/>
-      <c r="G22" s="69"/>
-      <c r="H22" s="69"/>
-      <c r="I22" s="69"/>
-      <c r="J22" s="69"/>
-      <c r="K22" s="69"/>
-      <c r="L22" s="69"/>
-      <c r="M22" s="69"/>
-      <c r="N22" s="69"/>
-      <c r="O22" s="69"/>
-      <c r="P22" s="69"/>
-      <c r="Q22" s="69"/>
+      <c r="A22" s="68"/>
+      <c r="B22" s="68"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="68"/>
+      <c r="F22" s="68"/>
+      <c r="G22" s="68"/>
+      <c r="H22" s="68"/>
+      <c r="I22" s="68"/>
+      <c r="J22" s="68"/>
+      <c r="K22" s="68"/>
+      <c r="L22" s="68"/>
+      <c r="M22" s="68"/>
+      <c r="N22" s="68"/>
+      <c r="O22" s="68"/>
+      <c r="P22" s="68"/>
+      <c r="Q22" s="68"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A23" s="69"/>
-      <c r="B23" s="69"/>
-      <c r="C23" s="69"/>
-      <c r="D23" s="69"/>
-      <c r="E23" s="69"/>
-      <c r="F23" s="69"/>
-      <c r="G23" s="69"/>
-      <c r="H23" s="69"/>
-      <c r="I23" s="69"/>
-      <c r="J23" s="69"/>
-      <c r="K23" s="69"/>
-      <c r="L23" s="69"/>
-      <c r="M23" s="69"/>
-      <c r="N23" s="69"/>
-      <c r="O23" s="69"/>
-      <c r="P23" s="69"/>
-      <c r="Q23" s="69"/>
+      <c r="A23" s="68"/>
+      <c r="B23" s="68"/>
+      <c r="C23" s="68"/>
+      <c r="D23" s="68"/>
+      <c r="E23" s="68"/>
+      <c r="F23" s="68"/>
+      <c r="G23" s="68"/>
+      <c r="H23" s="68"/>
+      <c r="I23" s="68"/>
+      <c r="J23" s="68"/>
+      <c r="K23" s="68"/>
+      <c r="L23" s="68"/>
+      <c r="M23" s="68"/>
+      <c r="N23" s="68"/>
+      <c r="O23" s="68"/>
+      <c r="P23" s="68"/>
+      <c r="Q23" s="68"/>
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A24" s="69"/>
-      <c r="B24" s="69"/>
-      <c r="C24" s="69"/>
-      <c r="D24" s="69"/>
-      <c r="E24" s="69"/>
-      <c r="F24" s="69"/>
-      <c r="G24" s="69"/>
-      <c r="H24" s="69"/>
-      <c r="I24" s="69"/>
-      <c r="J24" s="69"/>
-      <c r="K24" s="69"/>
-      <c r="L24" s="69"/>
-      <c r="M24" s="69"/>
-      <c r="N24" s="69"/>
-      <c r="O24" s="69"/>
-      <c r="P24" s="69"/>
-      <c r="Q24" s="69"/>
+      <c r="A24" s="68"/>
+      <c r="B24" s="68"/>
+      <c r="C24" s="68"/>
+      <c r="D24" s="68"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="68"/>
+      <c r="G24" s="68"/>
+      <c r="H24" s="68"/>
+      <c r="I24" s="68"/>
+      <c r="J24" s="68"/>
+      <c r="K24" s="68"/>
+      <c r="L24" s="68"/>
+      <c r="M24" s="68"/>
+      <c r="N24" s="68"/>
+      <c r="O24" s="68"/>
+      <c r="P24" s="68"/>
+      <c r="Q24" s="68"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A25" s="69"/>
-      <c r="B25" s="69"/>
-      <c r="C25" s="69"/>
-      <c r="D25" s="69"/>
-      <c r="E25" s="69"/>
-      <c r="F25" s="69"/>
-      <c r="G25" s="69"/>
-      <c r="H25" s="69"/>
-      <c r="I25" s="69"/>
-      <c r="J25" s="69"/>
-      <c r="K25" s="69"/>
-      <c r="L25" s="69"/>
-      <c r="M25" s="69"/>
-      <c r="N25" s="69"/>
-      <c r="O25" s="69"/>
-      <c r="P25" s="69"/>
-      <c r="Q25" s="69"/>
+      <c r="A25" s="68"/>
+      <c r="B25" s="68"/>
+      <c r="C25" s="68"/>
+      <c r="D25" s="68"/>
+      <c r="E25" s="68"/>
+      <c r="F25" s="68"/>
+      <c r="G25" s="68"/>
+      <c r="H25" s="68"/>
+      <c r="I25" s="68"/>
+      <c r="J25" s="68"/>
+      <c r="K25" s="68"/>
+      <c r="L25" s="68"/>
+      <c r="M25" s="68"/>
+      <c r="N25" s="68"/>
+      <c r="O25" s="68"/>
+      <c r="P25" s="68"/>
+      <c r="Q25" s="68"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A26" s="69"/>
-      <c r="B26" s="69"/>
-      <c r="C26" s="69"/>
-      <c r="D26" s="69"/>
-      <c r="E26" s="69"/>
-      <c r="F26" s="69"/>
-      <c r="G26" s="69"/>
-      <c r="H26" s="69"/>
-      <c r="I26" s="69"/>
-      <c r="J26" s="69"/>
-      <c r="K26" s="69"/>
-      <c r="L26" s="69"/>
-      <c r="M26" s="69"/>
-      <c r="N26" s="69"/>
-      <c r="O26" s="69"/>
-      <c r="P26" s="69"/>
-      <c r="Q26" s="69"/>
+      <c r="A26" s="68"/>
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="68"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="68"/>
+      <c r="M26" s="68"/>
+      <c r="N26" s="68"/>
+      <c r="O26" s="68"/>
+      <c r="P26" s="68"/>
+      <c r="Q26" s="68"/>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A27" s="69"/>
-      <c r="B27" s="69"/>
-      <c r="C27" s="69"/>
-      <c r="D27" s="69"/>
-      <c r="E27" s="69"/>
-      <c r="F27" s="69"/>
-      <c r="G27" s="69"/>
-      <c r="H27" s="69"/>
-      <c r="I27" s="69"/>
-      <c r="J27" s="69"/>
-      <c r="K27" s="69"/>
-      <c r="L27" s="69"/>
-      <c r="M27" s="69"/>
-      <c r="N27" s="69"/>
-      <c r="O27" s="69"/>
-      <c r="P27" s="69"/>
-      <c r="Q27" s="69"/>
+      <c r="A27" s="68"/>
+      <c r="B27" s="68"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="68"/>
+      <c r="I27" s="68"/>
+      <c r="J27" s="68"/>
+      <c r="K27" s="68"/>
+      <c r="L27" s="68"/>
+      <c r="M27" s="68"/>
+      <c r="N27" s="68"/>
+      <c r="O27" s="68"/>
+      <c r="P27" s="68"/>
+      <c r="Q27" s="68"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A28" s="69"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="69"/>
-      <c r="D28" s="69"/>
-      <c r="E28" s="69"/>
-      <c r="F28" s="69"/>
-      <c r="G28" s="69"/>
-      <c r="H28" s="69"/>
-      <c r="I28" s="69"/>
-      <c r="J28" s="69"/>
-      <c r="K28" s="69"/>
-      <c r="L28" s="69"/>
-      <c r="M28" s="69"/>
-      <c r="N28" s="69"/>
-      <c r="O28" s="69"/>
-      <c r="P28" s="69"/>
-      <c r="Q28" s="69"/>
+      <c r="A28" s="68"/>
+      <c r="B28" s="68"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="68"/>
+      <c r="G28" s="68"/>
+      <c r="H28" s="68"/>
+      <c r="I28" s="68"/>
+      <c r="J28" s="68"/>
+      <c r="K28" s="68"/>
+      <c r="L28" s="68"/>
+      <c r="M28" s="68"/>
+      <c r="N28" s="68"/>
+      <c r="O28" s="68"/>
+      <c r="P28" s="68"/>
+      <c r="Q28" s="68"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A29" s="69"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="69"/>
-      <c r="D29" s="69"/>
-      <c r="E29" s="69"/>
-      <c r="F29" s="69"/>
-      <c r="G29" s="69"/>
-      <c r="H29" s="69"/>
-      <c r="I29" s="69"/>
-      <c r="J29" s="69"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
-      <c r="N29" s="69"/>
-      <c r="O29" s="69"/>
-      <c r="P29" s="69"/>
-      <c r="Q29" s="69"/>
+      <c r="A29" s="68"/>
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="68"/>
+      <c r="F29" s="68"/>
+      <c r="G29" s="68"/>
+      <c r="H29" s="68"/>
+      <c r="I29" s="68"/>
+      <c r="J29" s="68"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="68"/>
+      <c r="M29" s="68"/>
+      <c r="N29" s="68"/>
+      <c r="O29" s="68"/>
+      <c r="P29" s="68"/>
+      <c r="Q29" s="68"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A30" s="69"/>
-      <c r="B30" s="69"/>
-      <c r="C30" s="69"/>
-      <c r="D30" s="69"/>
-      <c r="E30" s="69"/>
-      <c r="F30" s="69"/>
-      <c r="G30" s="69"/>
-      <c r="H30" s="69"/>
-      <c r="I30" s="69"/>
-      <c r="J30" s="69"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
-      <c r="N30" s="69"/>
-      <c r="O30" s="69"/>
-      <c r="P30" s="69"/>
-      <c r="Q30" s="69"/>
+      <c r="A30" s="68"/>
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="68"/>
+      <c r="E30" s="68"/>
+      <c r="F30" s="68"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="68"/>
+      <c r="J30" s="68"/>
+      <c r="K30" s="68"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="68"/>
+      <c r="O30" s="68"/>
+      <c r="P30" s="68"/>
+      <c r="Q30" s="68"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A31" s="69"/>
-      <c r="B31" s="69"/>
-      <c r="C31" s="69"/>
-      <c r="D31" s="69"/>
-      <c r="E31" s="69"/>
-      <c r="F31" s="69"/>
-      <c r="G31" s="69"/>
-      <c r="H31" s="69"/>
-      <c r="I31" s="69"/>
-      <c r="J31" s="69"/>
-      <c r="K31" s="69"/>
-      <c r="L31" s="69"/>
-      <c r="M31" s="69"/>
-      <c r="N31" s="69"/>
-      <c r="O31" s="69"/>
-      <c r="P31" s="69"/>
-      <c r="Q31" s="69"/>
+      <c r="A31" s="68"/>
+      <c r="B31" s="68"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="68"/>
+      <c r="E31" s="68"/>
+      <c r="F31" s="68"/>
+      <c r="G31" s="68"/>
+      <c r="H31" s="68"/>
+      <c r="I31" s="68"/>
+      <c r="J31" s="68"/>
+      <c r="K31" s="68"/>
+      <c r="L31" s="68"/>
+      <c r="M31" s="68"/>
+      <c r="N31" s="68"/>
+      <c r="O31" s="68"/>
+      <c r="P31" s="68"/>
+      <c r="Q31" s="68"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A32" s="69"/>
-      <c r="B32" s="69"/>
-      <c r="C32" s="69"/>
-      <c r="D32" s="69"/>
-      <c r="E32" s="69"/>
-      <c r="F32" s="69"/>
-      <c r="G32" s="69"/>
-      <c r="H32" s="69"/>
-      <c r="I32" s="69"/>
-      <c r="J32" s="69"/>
-      <c r="K32" s="69"/>
-      <c r="L32" s="69"/>
-      <c r="M32" s="69"/>
-      <c r="N32" s="69"/>
-      <c r="O32" s="69"/>
-      <c r="P32" s="69"/>
-      <c r="Q32" s="69"/>
+      <c r="A32" s="68"/>
+      <c r="B32" s="68"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="68"/>
+      <c r="O32" s="68"/>
+      <c r="P32" s="68"/>
+      <c r="Q32" s="68"/>
     </row>
     <row r="33" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A33" s="69"/>
-      <c r="B33" s="69"/>
-      <c r="C33" s="69"/>
-      <c r="D33" s="69"/>
-      <c r="E33" s="69"/>
-      <c r="F33" s="69"/>
-      <c r="G33" s="69"/>
-      <c r="H33" s="69"/>
-      <c r="I33" s="69"/>
-      <c r="J33" s="69"/>
-      <c r="K33" s="69"/>
-      <c r="L33" s="69"/>
-      <c r="M33" s="69"/>
-      <c r="N33" s="69"/>
-      <c r="O33" s="69"/>
-      <c r="P33" s="69"/>
-      <c r="Q33" s="69"/>
+      <c r="A33" s="68"/>
+      <c r="B33" s="68"/>
+      <c r="C33" s="68"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="68"/>
+      <c r="F33" s="68"/>
+      <c r="G33" s="68"/>
+      <c r="H33" s="68"/>
+      <c r="I33" s="68"/>
+      <c r="J33" s="68"/>
+      <c r="K33" s="68"/>
+      <c r="L33" s="68"/>
+      <c r="M33" s="68"/>
+      <c r="N33" s="68"/>
+      <c r="O33" s="68"/>
+      <c r="P33" s="68"/>
+      <c r="Q33" s="68"/>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A34" s="68"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="68"/>
+      <c r="N34" s="68"/>
+      <c r="O34" s="68"/>
+      <c r="P34" s="68"/>
+      <c r="Q34" s="68"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="A3:F3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>